<commit_message>
Todas las lookup tables y coeficientes aerodinamicos sacados. Quedan lso coeficientes de amrotiguaciin que son teoricos
</commit_message>
<xml_diff>
--- a/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
+++ b/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
@@ -4715,7 +4715,7 @@
         <v>2.7856670546677567</v>
       </c>
       <c r="M7">
-        <v>0.60422455801932451</v>
+        <v>0.59905399448358443</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -4756,7 +4756,7 @@
         <v>2.3582835261975021</v>
       </c>
       <c r="M8">
-        <v>0.59457233560527789</v>
+        <v>0.54796083267641138</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -4797,7 +4797,7 @@
         <v>1.2908468906059773</v>
       </c>
       <c r="M9">
-        <v>0.5714944072333854</v>
+        <v>0.34928342370854448</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -4838,7 +4838,7 @@
         <v>2.8556608596391975</v>
       </c>
       <c r="M10">
-        <v>0.58603026498810507</v>
+        <v>0.58513802914613056</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -4920,7 +4920,7 @@
         <v>1.4552774960110393</v>
       </c>
       <c r="M12">
-        <v>1.0204630191563318</v>
+        <v>1.0136972085446088</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -4961,7 +4961,7 @@
         <v>1.4773585450330173</v>
       </c>
       <c r="M13">
-        <v>0.96976636741979672</v>
+        <v>0.94397012748038178</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -5002,7 +5002,7 @@
         <v>1.2816085670899657</v>
       </c>
       <c r="M14">
-        <v>0.76113146441353707</v>
+        <v>0.60569334853151069</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -5043,7 +5043,7 @@
         <v>1.4681689489973853</v>
       </c>
       <c r="M15">
-        <v>1.0307253672546959</v>
+        <v>1.0307654858374153</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -7380,7 +7380,7 @@
         <v>0.3972073187545293</v>
       </c>
       <c r="M72">
-        <v>6.2747112142194694E-2</v>
+        <v>4.7505716244460337E-2</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
@@ -7421,7 +7421,7 @@
         <v>1.8127020062726227</v>
       </c>
       <c r="M73">
-        <v>0.1777627280397478</v>
+        <v>0.16122163330318987</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
@@ -7462,7 +7462,7 @@
         <v>2.1955092292140619</v>
       </c>
       <c r="M74">
-        <v>0.2271614362967018</v>
+        <v>0.22073396456343947</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
@@ -7503,7 +7503,7 @@
         <v>2.6417255731941154</v>
       </c>
       <c r="M75">
-        <v>0.28399292878689086</v>
+        <v>0.27833019303960183</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
@@ -7544,7 +7544,7 @@
         <v>0.72020938901401477</v>
       </c>
       <c r="M76">
-        <v>5.6903913815647508E-2</v>
+        <v>4.1089234461886816E-2</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
@@ -7585,7 +7585,7 @@
         <v>1.0692906279386272</v>
       </c>
       <c r="M77">
-        <v>8.7429243252462749E-2</v>
+        <v>7.0912458614977983E-2</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -7626,7 +7626,7 @@
         <v>-0.38413124152576072</v>
       </c>
       <c r="M78">
-        <v>0.12623649519322286</v>
+        <v>0.11445860068689892</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
@@ -7667,7 +7667,7 @@
         <v>6.71442265757278E-2</v>
       </c>
       <c r="M79">
-        <v>6.7279658631792763E-2</v>
+        <v>5.3362290172122205E-2</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
@@ -7708,7 +7708,7 @@
         <v>0.30084637733205799</v>
       </c>
       <c r="M80">
-        <v>8.9134878903643494E-2</v>
+        <v>2.3364533049572544E-2</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
@@ -7749,7 +7749,7 @@
         <v>1.6047705833257557</v>
       </c>
       <c r="M81">
-        <v>0.20035054592369858</v>
+        <v>0.13528791080449187</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
@@ -7790,7 +7790,7 @@
         <v>1.9542278015189098</v>
       </c>
       <c r="M82">
-        <v>0.24559129505320115</v>
+        <v>0.18412749088146577</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
@@ -7831,7 +7831,7 @@
         <v>1.946391405701315</v>
       </c>
       <c r="M83">
-        <v>0.39194458632299817</v>
+        <v>0.33200168932777918</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
@@ -7872,7 +7872,7 @@
         <v>0.59279329040318485</v>
       </c>
       <c r="M84">
-        <v>8.560652592627864E-2</v>
+        <v>1.9125258887405225E-2</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -7913,7 +7913,7 @@
         <v>0.90884784585525014</v>
       </c>
       <c r="M85">
-        <v>0.1118406496414306</v>
+        <v>4.4171698979813906E-2</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
@@ -7954,7 +7954,7 @@
         <v>-0.37100018499813575</v>
       </c>
       <c r="M86">
-        <v>0.1666251990856247</v>
+        <v>0.1162170426322178</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -7995,7 +7995,7 @@
         <v>6.7826852862145043E-2</v>
       </c>
       <c r="M87">
-        <v>9.61493609518555E-2</v>
+        <v>3.8949194167201794E-2</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -8036,7 +8036,7 @@
         <v>0.26292881549732261</v>
       </c>
       <c r="M88">
-        <v>0.23094840006628753</v>
+        <v>-1.4562382430074136E-2</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -8077,7 +8077,7 @@
         <v>0.8765004087746503</v>
       </c>
       <c r="M89">
-        <v>0.33702404704451111</v>
+        <v>0.11806986317915942</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
@@ -8118,7 +8118,7 @@
         <v>0.88699824281153261</v>
       </c>
       <c r="M90">
-        <v>0.41386390896759262</v>
+        <v>0.16035439882918592</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -8159,7 +8159,7 @@
         <v>1.1319028726797504</v>
       </c>
       <c r="M91">
-        <v>0.45551102033549801</v>
+        <v>0.23279046238150966</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -8200,7 +8200,7 @@
         <v>0.42272606539050189</v>
       </c>
       <c r="M92">
-        <v>0.23413418562903801</v>
+        <v>-1.7951605742576524E-2</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -8241,7 +8241,7 @@
         <v>0.58364671397835965</v>
       </c>
       <c r="M93">
-        <v>0.25614354658640848</v>
+        <v>2.5095911377773148E-2</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -8282,7 +8282,7 @@
         <v>-0.15121451905138086</v>
       </c>
       <c r="M94">
-        <v>0.3161120665413949</v>
+        <v>8.0071160866515792E-2</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -8323,7 +8323,7 @@
         <v>0.1297887965843986</v>
       </c>
       <c r="M95">
-        <v>0.24362020655854169</v>
+        <v>4.681144616371917E-3</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -8364,7 +8364,7 @@
         <v>0.45321817305868006</v>
       </c>
       <c r="M96">
-        <v>6.3043022110943578E-2</v>
+        <v>5.9277281356348716E-2</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
@@ -8405,7 +8405,7 @@
         <v>1.8604870559400697</v>
       </c>
       <c r="M97">
-        <v>0.18121187790161089</v>
+        <v>0.17700513443223193</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -8446,7 +8446,7 @@
         <v>2.2475648258271175</v>
       </c>
       <c r="M98">
-        <v>0.22997736307633398</v>
+        <v>0.22587140466270847</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
@@ -8487,7 +8487,7 @@
         <v>2.6417255731941163</v>
       </c>
       <c r="M99">
-        <v>0.28223555239936887</v>
+        <v>0.27833019303960171</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -8528,7 +8528,7 @@
         <v>0.77115217116192813</v>
       </c>
       <c r="M100">
-        <v>5.6781453340377042E-2</v>
+        <v>5.2873288477746201E-2</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -8569,7 +8569,7 @@
         <v>1.1261908593889041</v>
       </c>
       <c r="M101">
-        <v>9.1215745471783752E-2</v>
+        <v>8.7098728692080046E-2</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -8610,7 +8610,7 @@
         <v>-0.35313650151309578</v>
       </c>
       <c r="M102">
-        <v>0.11698201558860154</v>
+        <v>0.11298610409047583</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -8651,7 +8651,7 @@
         <v>0.12197104710511522</v>
       </c>
       <c r="M103">
-        <v>6.3759664211753816E-2</v>
+        <v>6.0141495773510356E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -8692,7 +8692,7 @@
         <v>3.6261797567294335E-2</v>
       </c>
       <c r="M104">
-        <v>0.36392368744617631</v>
+        <v>-1.7041213729324382E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mas datos del CFD del DBX 1. Hay controles elevator hasta 25 deg AoA
</commit_message>
<xml_diff>
--- a/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
+++ b/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
@@ -4423,10 +4423,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M111"/>
+  <dimension ref="A1:M123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M111"/>
+      <selection activeCell="K1" sqref="K1:M123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5827,7 +5827,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5842,33 +5842,33 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>-2.3304508550854926E-2</v>
+        <v>0.72257858245084117</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>-0.97656185923510674</v>
+        <v>-2.9578097861150385</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>-0.24467922970624151</v>
+        <v>0.12330119266677141</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
-        <v>0.97400385140723522</v>
+        <v>3.0131161798127146</v>
       </c>
       <c r="M35">
-        <v>7.4381869265280662E-2</v>
+        <v>0.43805185264462587</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5883,33 +5883,33 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>2.6952950831595199E-2</v>
+        <v>0.58565621338973528</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>-1.3307533742524675</v>
+        <v>-2.7818879292521048</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>-0.21095811311478116</v>
+        <v>4.7748252489993689E-2</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>1.3262807185602445</v>
+        <v>2.768755703824854</v>
       </c>
       <c r="M36">
-        <v>0.11229630545204901</v>
+        <v>0.64489185429644336</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>-10</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5924,33 +5924,33 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>-7.718607828718764E-2</v>
+        <v>-2.3304508550854926E-2</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0.18832547032290964</v>
+        <v>-0.97656185923510674</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37">
-        <v>-0.14746361651005876</v>
+        <v>-0.24467922970624151</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>-0.17206116142784475</v>
+        <v>0.97400385140723522</v>
       </c>
       <c r="M37">
-        <v>0.10871582305167048</v>
+        <v>7.4381869265280662E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -5965,33 +5965,33 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>-8.7916609710199989E-2</v>
+        <v>2.6952950831595199E-2</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>-0.32266759723232541</v>
+        <v>-1.3307533742524675</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
       <c r="J38">
-        <v>-0.30691885907496097</v>
+        <v>-0.21095811311478116</v>
       </c>
       <c r="K38">
         <v>0</v>
       </c>
       <c r="L38">
-        <v>0.32682659234331435</v>
+        <v>1.3262807185602445</v>
       </c>
       <c r="M38">
-        <v>7.0909005802329672E-2</v>
+        <v>0.11229630545204901</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -6000,39 +6000,39 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
-        <v>-8.5429671993744891E-2</v>
+        <v>-7.718607828718764E-2</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>-0.72370940298428799</v>
+        <v>0.18832547032290964</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39">
-        <v>-0.54379963954552524</v>
+        <v>-0.14746361651005876</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>0.72370940298428799</v>
+        <v>-0.17206116142784475</v>
       </c>
       <c r="M39">
-        <v>8.5429671993744891E-2</v>
+        <v>0.10871582305167048</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>12</v>
+        <v>-3</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -6041,39 +6041,39 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.21332993320000762</v>
+        <v>-8.7916609710199989E-2</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>-2.0993820970085664</v>
+        <v>-0.32266759723232541</v>
       </c>
       <c r="I40">
         <v>0</v>
       </c>
       <c r="J40">
-        <v>-0.25829277660138666</v>
+        <v>-0.30691885907496097</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>2.0978593483260881</v>
+        <v>0.32682659234331435</v>
       </c>
       <c r="M40">
-        <v>0.22781791913729374</v>
+        <v>7.0909005802329672E-2</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -6088,33 +6088,33 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.36775805680102264</v>
+        <v>-8.5429671993744891E-2</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>-2.455894824377868</v>
+        <v>-0.72370940298428799</v>
       </c>
       <c r="I41">
         <v>0</v>
       </c>
       <c r="J41">
-        <v>-0.14263048587484461</v>
+        <v>-0.54379963954552524</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>2.4673950266062379</v>
+        <v>0.72370940298428799</v>
       </c>
       <c r="M41">
-        <v>0.28040534842771281</v>
+        <v>8.5429671993744891E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6129,33 +6129,33 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0.55303757989544111</v>
+        <v>0.21332993320000762</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>-2.787104511410142</v>
+        <v>-2.0993820970085664</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>5.6639586294437348E-2</v>
+        <v>-0.25829277660138666</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>2.8215919178879201</v>
+        <v>2.0978593483260881</v>
       </c>
       <c r="M42">
-        <v>0.3352926650091575</v>
+        <v>0.22781791913729374</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6170,33 +6170,33 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>-3.3598927806487079E-2</v>
+        <v>0.36775805680102264</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>-1.0353841375278308</v>
+        <v>-2.455894824377868</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
       <c r="J43">
-        <v>-0.49392877418713621</v>
+        <v>-0.14263048587484461</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>1.0322067475361931</v>
+        <v>2.4673950266062379</v>
       </c>
       <c r="M43">
-        <v>8.7740700559939391E-2</v>
+        <v>0.28040534842771281</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6211,33 +6211,33 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>1.6491058929627832E-2</v>
+        <v>0.55303757989544111</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>-1.3852009656776634</v>
+        <v>-2.787104511410142</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>-0.41934117520233494</v>
+        <v>5.6639586294437348E-2</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
-        <v>1.3793364748992825</v>
+        <v>2.8215919178879201</v>
       </c>
       <c r="M44">
-        <v>0.12839220907583238</v>
+        <v>0.3352926650091575</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>-10</v>
+        <v>22</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6252,33 +6252,33 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>-9.8626430925695188E-2</v>
+        <v>0.68116461703126108</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>9.0518855786986888E-2</v>
+        <v>-2.8980406823460374</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>-0.55841392539558155</v>
+        <v>0.31872311046694207</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>-7.2017370972778313E-2</v>
+        <v>2.9421852872904966</v>
       </c>
       <c r="M45">
-        <v>0.11284650817945356</v>
+        <v>0.45406031238082001</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>-3</v>
+        <v>25</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -6293,33 +6293,33 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>-0.10181096777716636</v>
+        <v>0.52641255960326594</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>-0.40003493281219354</v>
+        <v>-2.670212924281651</v>
       </c>
       <c r="I46">
         <v>0</v>
       </c>
       <c r="J46">
-        <v>-0.62825495094738204</v>
+        <v>5.9318386681059529E-2</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>0.40481507319445559</v>
+        <v>2.6425063272203695</v>
       </c>
       <c r="M46">
-        <v>8.0735228644916612E-2</v>
+        <v>0.65138894257512669</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6328,39 +6328,39 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>-6.8496245088475988E-2</v>
+        <v>-3.3598927806487079E-2</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>-0.56496728530850515</v>
+        <v>-1.0353841375278308</v>
       </c>
       <c r="I47">
         <v>0</v>
       </c>
       <c r="J47">
-        <v>0.121901923520936</v>
+        <v>-0.49392877418713621</v>
       </c>
       <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
-        <v>0.56496728530850515</v>
+        <v>1.0322067475361931</v>
       </c>
       <c r="M47">
-        <v>6.8496245088475988E-2</v>
+        <v>8.7740700559939391E-2</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -6369,80 +6369,80 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0.22271152705902242</v>
+        <v>1.6491058929627832E-2</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>-1.9788706129954865</v>
+        <v>-1.3852009656776634</v>
       </c>
       <c r="I48">
         <v>0</v>
       </c>
       <c r="J48">
-        <v>0.24523509821471629</v>
+        <v>-0.41934117520233494</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
       <c r="L48">
-        <v>1.9819318724196169</v>
+        <v>1.3793364748992825</v>
       </c>
       <c r="M48">
-        <v>0.19358558920892258</v>
+        <v>0.12839220907583238</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
+        <v>-10</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
         <v>15</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>5</v>
-      </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0.37856085750210883</v>
+        <v>-9.8626430925695188E-2</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>-2.3520082753719005</v>
+        <v>9.0518855786986888E-2</v>
       </c>
       <c r="I49">
         <v>0</v>
       </c>
       <c r="J49">
-        <v>0.28937363651564396</v>
+        <v>-0.55841392539558155</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>2.3698442964792168</v>
+        <v>-7.2017370972778313E-2</v>
       </c>
       <c r="M49">
-        <v>0.24308282682155927</v>
+        <v>0.11284650817945356</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -6451,39 +6451,39 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>0.57310594071170506</v>
+        <v>-0.10181096777716636</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>-2.7216349311976553</v>
+        <v>-0.40003493281219354</v>
       </c>
       <c r="I50">
         <v>0</v>
       </c>
       <c r="J50">
-        <v>0.32755054698950536</v>
+        <v>-0.62825495094738204</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
-        <v>2.7655281115491999</v>
+        <v>0.40481507319445559</v>
       </c>
       <c r="M50">
-        <v>0.29597530678323508</v>
+        <v>8.0735228644916612E-2</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -6498,33 +6498,33 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>-1.844713876167519E-2</v>
+        <v>-6.8496245088475988E-2</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>-0.88384405730146687</v>
+        <v>-0.56496728530850515</v>
       </c>
       <c r="I51">
         <v>0</v>
       </c>
       <c r="J51">
-        <v>0.14107790350215352</v>
+        <v>0.121901923520936</v>
       </c>
       <c r="K51">
         <v>0</v>
       </c>
       <c r="L51">
-        <v>0.88166733109152029</v>
+        <v>0.56496728530850515</v>
       </c>
       <c r="M51">
-        <v>6.4678681507640265E-2</v>
+        <v>6.8496245088475988E-2</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -6539,33 +6539,33 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <v>2.8352590222335456E-2</v>
+        <v>0.22271152705902242</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>-1.2563519895601134</v>
+        <v>-1.9788706129954865</v>
       </c>
       <c r="I52">
         <v>0</v>
       </c>
       <c r="J52">
-        <v>0.18562367421745316</v>
+        <v>0.24523509821471629</v>
       </c>
       <c r="K52">
         <v>0</v>
       </c>
       <c r="L52">
-        <v>1.2524332145926234</v>
+        <v>1.9819318724196169</v>
       </c>
       <c r="M52">
-        <v>0.10312727102546061</v>
+        <v>0.19358558920892258</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>-10</v>
+        <v>15</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -6580,33 +6580,33 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>-6.0064392872935371E-2</v>
+        <v>0.37856085750210883</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>0.28251967244743303</v>
+        <v>-2.3520082753719005</v>
       </c>
       <c r="I53">
         <v>0</v>
       </c>
       <c r="J53">
-        <v>0.25045575785478952</v>
+        <v>0.28937363651564396</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
-        <v>-0.26779749143964576</v>
+        <v>2.3698442964792168</v>
       </c>
       <c r="M53">
-        <v>0.10821090605679277</v>
+        <v>0.24308282682155927</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>-3</v>
+        <v>18</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6621,33 +6621,33 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>-7.7799878933980257E-2</v>
+        <v>0.57310594071170506</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>-0.22835660951135309</v>
+        <v>-2.7216349311976553</v>
       </c>
       <c r="I54">
         <v>0</v>
       </c>
       <c r="J54">
-        <v>8.3652201891138964E-2</v>
+        <v>0.32755054698950536</v>
       </c>
       <c r="K54">
         <v>0</v>
       </c>
       <c r="L54">
-        <v>0.23211538577404953</v>
+        <v>2.7655281115491999</v>
       </c>
       <c r="M54">
-        <v>6.5741995380629692E-2</v>
+        <v>0.29597530678323508</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -6656,39 +6656,39 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>-7.7195931073887322E-2</v>
+        <v>0.70886868953398696</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>-0.30548908261149982</v>
+        <v>-2.8763578652502293</v>
       </c>
       <c r="I55">
         <v>0</v>
       </c>
       <c r="J55">
-        <v>1.2170847420967017</v>
+        <v>0.33843077078853501</v>
       </c>
       <c r="K55">
         <v>0</v>
       </c>
       <c r="L55">
-        <v>0.30548908261149982</v>
+        <v>2.9324594575817322</v>
       </c>
       <c r="M55">
-        <v>7.7195931073887322E-2</v>
+        <v>0.42025101740262394</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -6697,39 +6697,39 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0.18073217616807821</v>
+        <v>0.56918423918376349</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>-1.7188149530669425</v>
+        <v>-2.6987792799381118</v>
       </c>
       <c r="I56">
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1.3494623786828075</v>
+        <v>0.22392012366737543</v>
       </c>
       <c r="K56">
         <v>0</v>
       </c>
       <c r="L56">
-        <v>1.7188310547800971</v>
+        <v>2.6864723306751181</v>
       </c>
       <c r="M56">
-        <v>0.18057897860079045</v>
+        <v>0.62469729987848532</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -6738,39 +6738,39 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0.3296738451692775</v>
+        <v>-1.844713876167519E-2</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>-2.0922229843557751</v>
+        <v>-0.88384405730146687</v>
       </c>
       <c r="I57">
         <v>0</v>
       </c>
       <c r="J57">
-        <v>1.3871647891826986</v>
+        <v>0.14107790350215352</v>
       </c>
       <c r="K57">
         <v>0</v>
       </c>
       <c r="L57">
-        <v>2.1062580847468211</v>
+        <v>0.88166733109152029</v>
       </c>
       <c r="M57">
-        <v>0.22306667365147909</v>
+        <v>6.4678681507640265E-2</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -6779,39 +6779,39 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>0.51972032803105017</v>
+        <v>2.8352590222335456E-2</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>-2.4682677185949227</v>
+        <v>-1.2563519895601134</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
       <c r="J58">
-        <v>1.4034418238536202</v>
+        <v>0.18562367421745316</v>
       </c>
       <c r="K58">
         <v>0</v>
       </c>
       <c r="L58">
-        <v>2.5080645114143905</v>
+        <v>1.2524332145926234</v>
       </c>
       <c r="M58">
-        <v>0.26845326708792649</v>
+        <v>0.10312727102546061</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>3</v>
+        <v>-10</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -6820,39 +6820,39 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>-3.5178793356106131E-2</v>
+        <v>-6.0064392872935371E-2</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>-0.62958462063937748</v>
+        <v>0.28251967244743303</v>
       </c>
       <c r="I59">
         <v>0</v>
       </c>
       <c r="J59">
-        <v>1.2167173554646495</v>
+        <v>0.25045575785478952</v>
       </c>
       <c r="K59">
         <v>0</v>
       </c>
       <c r="L59">
-        <v>0.62688068100797167</v>
+        <v>-0.26779749143964576</v>
       </c>
       <c r="M59">
-        <v>6.8080495199448407E-2</v>
+        <v>0.10821090605679277</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -6861,39 +6861,39 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>4.3461943916355593E-3</v>
+        <v>-7.7799878933980257E-2</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>-0.98649921800662743</v>
+        <v>-0.22835660951135309</v>
       </c>
       <c r="I60">
         <v>0</v>
       </c>
       <c r="J60">
-        <v>1.2779142661211149</v>
+        <v>8.3652201891138964E-2</v>
       </c>
       <c r="K60">
         <v>0</v>
       </c>
       <c r="L60">
-        <v>0.98154937309209067</v>
+        <v>0.23211538577404953</v>
       </c>
       <c r="M60">
-        <v>9.8794861788966265E-2</v>
+        <v>6.5741995380629692E-2</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -6908,33 +6908,33 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>-4.7459353129715436E-2</v>
+        <v>-7.7195931073887322E-2</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>0.53483256261998691</v>
+        <v>-0.30548908261149982</v>
       </c>
       <c r="I61">
         <v>0</v>
       </c>
       <c r="J61">
-        <v>1.3350547545921554</v>
+        <v>1.2170847420967017</v>
       </c>
       <c r="K61">
         <v>0</v>
       </c>
       <c r="L61">
-        <v>-0.518466024047324</v>
+        <v>0.30548908261149982</v>
       </c>
       <c r="M61">
-        <v>0.1396110387709831</v>
+        <v>7.7195931073887322E-2</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>-3</v>
+        <v>12</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -6949,33 +6949,33 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>-7.9837764981612436E-2</v>
+        <v>0.18073217616807821</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>3.3530079840469615E-2</v>
+        <v>-1.7188149530669425</v>
       </c>
       <c r="I62">
         <v>0</v>
       </c>
       <c r="J62">
-        <v>1.1838308031410509</v>
+        <v>1.3494623786828075</v>
       </c>
       <c r="K62">
         <v>0</v>
       </c>
       <c r="L62">
-        <v>-2.9305742256759783E-2</v>
+        <v>1.7188310547800971</v>
       </c>
       <c r="M62">
-        <v>8.1483178890785865E-2</v>
+        <v>0.18057897860079045</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -6984,39 +6984,39 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>-9.4084386734767128E-2</v>
+        <v>0.3296738451692775</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>-0.29196217368460958</v>
+        <v>-2.0922229843557751</v>
       </c>
       <c r="I63">
         <v>0</v>
       </c>
       <c r="J63">
-        <v>1.2767926677740682</v>
+        <v>1.3871647891826986</v>
       </c>
       <c r="K63">
         <v>0</v>
       </c>
       <c r="L63">
-        <v>0.29196217368460958</v>
+        <v>2.1062580847468211</v>
       </c>
       <c r="M63">
-        <v>9.4084386734767128E-2</v>
+        <v>0.22306667365147909</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -7025,39 +7025,39 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0.16224482491377495</v>
+        <v>0.51972032803105017</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>-1.6758814822736328</v>
+        <v>-2.4682677185949227</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64">
-        <v>1.52793577983716</v>
+        <v>1.4034418238536202</v>
       </c>
       <c r="K64">
         <v>0</v>
       </c>
       <c r="L64">
-        <v>1.6729920468744219</v>
+        <v>2.5080645114143905</v>
       </c>
       <c r="M64">
-        <v>0.18973596636879836</v>
+        <v>0.26845326708792649</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -7066,39 +7066,39 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0.30967124915718819</v>
+        <v>0.68599736513590925</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>-2.0444556517804156</v>
+        <v>-2.7239339886543155</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65">
-        <v>1.5881823258710199</v>
+        <v>1.1538807318073121</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
-        <v>2.0549413317599217</v>
+        <v>2.7825667512318466</v>
       </c>
       <c r="M65">
-        <v>0.23002460232813388</v>
+        <v>0.38435795095023834</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -7107,34 +7107,34 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.49826906045543068</v>
+        <v>0.54597524770037775</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>-2.4167766263258925</v>
+        <v>-2.5273816121985733</v>
       </c>
       <c r="I66">
         <v>0</v>
       </c>
       <c r="J66">
-        <v>1.6217210464330269</v>
+        <v>0.7076472884268511</v>
       </c>
       <c r="K66">
         <v>0</v>
       </c>
       <c r="L66">
-        <v>2.4524647663490233</v>
+        <v>2.5213247460853911</v>
       </c>
       <c r="M66">
-        <v>0.27294301232845158</v>
+        <v>0.57329600518265156</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -7148,34 +7148,34 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>-5.128071050976004E-2</v>
+        <v>-3.5178793356106131E-2</v>
       </c>
       <c r="G67">
         <v>0</v>
       </c>
       <c r="H67">
-        <v>-0.60674342555727956</v>
+        <v>-0.62958462063937748</v>
       </c>
       <c r="I67">
         <v>0</v>
       </c>
       <c r="J67">
-        <v>1.3126931746017902</v>
+        <v>1.2167173554646495</v>
       </c>
       <c r="K67">
         <v>0</v>
       </c>
       <c r="L67">
-        <v>0.6032280797583166</v>
+        <v>0.62688068100797167</v>
       </c>
       <c r="M67">
-        <v>8.2964929448905295E-2</v>
+        <v>6.8080495199448407E-2</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -7189,34 +7189,34 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68">
-        <v>-1.1924779959131403E-2</v>
+        <v>4.3461943916355593E-3</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>-0.95197972830722333</v>
+        <v>-0.98649921800662743</v>
       </c>
       <c r="I68">
         <v>0</v>
       </c>
       <c r="J68">
-        <v>1.3932105676535247</v>
+        <v>1.2779142661211149</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>0.9455182048243409</v>
+        <v>0.98154937309209067</v>
       </c>
       <c r="M68">
-        <v>0.11136843282871728</v>
+        <v>9.8794861788966265E-2</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -7230,34 +7230,34 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>-7.273515734660975E-2</v>
+        <v>-4.7459353129715436E-2</v>
       </c>
       <c r="G69">
         <v>0</v>
       </c>
       <c r="H69">
-        <v>0.50501444943067242</v>
+        <v>0.53483256261998691</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69">
-        <v>1.2261210668769142</v>
+        <v>1.3350547545921554</v>
       </c>
       <c r="K69">
         <v>0</v>
       </c>
       <c r="L69">
-        <v>-0.48471181765696153</v>
+        <v>-0.518466024047324</v>
       </c>
       <c r="M69">
-        <v>0.15932498571060855</v>
+        <v>0.1396110387709831</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
@@ -7271,34 +7271,34 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>-9.8108715481738343E-2</v>
+        <v>-7.9837764981612436E-2</v>
       </c>
       <c r="G70">
         <v>0</v>
       </c>
       <c r="H70">
-        <v>3.6631169446297338E-2</v>
+        <v>3.3530079840469615E-2</v>
       </c>
       <c r="I70">
         <v>0</v>
       </c>
       <c r="J70">
-        <v>1.2019920439586451</v>
+        <v>1.1838308031410509</v>
       </c>
       <c r="K70">
         <v>0</v>
       </c>
       <c r="L70">
-        <v>-3.1446354261168187E-2</v>
+        <v>-2.9305742256759783E-2</v>
       </c>
       <c r="M70">
-        <v>9.9891388178166493E-2</v>
+        <v>8.1483178890785865E-2</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -7312,34 +7312,34 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71">
-        <v>-6.9506435658708704E-2</v>
+        <v>-9.4084386734767128E-2</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>-0.38543276188102249</v>
+        <v>-0.29196217368460958</v>
       </c>
       <c r="I71">
         <v>0</v>
       </c>
       <c r="J71">
-        <v>0.8757747552691485</v>
+        <v>1.2767926677740682</v>
       </c>
       <c r="K71">
         <v>0</v>
       </c>
       <c r="L71">
-        <v>0.38543276188102249</v>
+        <v>0.29196217368460958</v>
       </c>
       <c r="M71">
-        <v>6.9506435658708704E-2</v>
+        <v>9.4084386734767128E-2</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
@@ -7353,34 +7353,34 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0.19825346612774047</v>
+        <v>0.16224482491377495</v>
       </c>
       <c r="G72">
         <v>0</v>
       </c>
       <c r="H72">
-        <v>-1.8003892255870124</v>
+        <v>-1.6758814822736328</v>
       </c>
       <c r="I72">
         <v>0</v>
       </c>
       <c r="J72">
-        <v>1.0042032638441956</v>
+        <v>1.52793577983716</v>
       </c>
       <c r="K72">
         <v>0</v>
       </c>
       <c r="L72">
-        <v>1.8022656147480305</v>
+        <v>1.6729920468744219</v>
       </c>
       <c r="M72">
-        <v>0.18040081579186187</v>
+        <v>0.18973596636879836</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
@@ -7394,34 +7394,34 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0.35013168866706651</v>
+        <v>0.30967124915718819</v>
       </c>
       <c r="G73">
         <v>0</v>
       </c>
       <c r="H73">
-        <v>-2.1757430242328892</v>
+        <v>-2.0444556517804156</v>
       </c>
       <c r="I73">
         <v>0</v>
       </c>
       <c r="J73">
-        <v>1.0383394874624312</v>
+        <v>1.5881823258710199</v>
       </c>
       <c r="K73">
         <v>0</v>
       </c>
       <c r="L73">
-        <v>2.1922271277957734</v>
+        <v>2.0549413317599217</v>
       </c>
       <c r="M73">
-        <v>0.22492249123470398</v>
+        <v>0.23002460232813388</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
@@ -7435,39 +7435,39 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74">
-        <v>0.54186440388334123</v>
+        <v>0.49826906045543068</v>
       </c>
       <c r="G74">
         <v>0</v>
       </c>
       <c r="H74">
-        <v>-2.550474490105854</v>
+        <v>-2.4167766263258925</v>
       </c>
       <c r="I74">
         <v>0</v>
       </c>
       <c r="J74">
-        <v>1.0574676302980566</v>
+        <v>1.6217210464330269</v>
       </c>
       <c r="K74">
         <v>0</v>
       </c>
       <c r="L74">
-        <v>2.5930906929065345</v>
+        <v>2.4524647663490233</v>
       </c>
       <c r="M74">
-        <v>0.27279628890084689</v>
+        <v>0.27294301232845158</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -7476,39 +7476,39 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75">
-        <v>-2.5652572187046505E-2</v>
+        <v>0.66792475237610327</v>
       </c>
       <c r="G75">
         <v>0</v>
       </c>
       <c r="H75">
-        <v>-0.70789263545777181</v>
+        <v>-2.6750815273685014</v>
       </c>
       <c r="I75">
         <v>0</v>
       </c>
       <c r="J75">
-        <v>0.88175100866170597</v>
+        <v>1.3783582285479135</v>
       </c>
       <c r="K75">
         <v>0</v>
       </c>
       <c r="L75">
-        <v>0.7055799413078836</v>
+        <v>2.7305014179717149</v>
       </c>
       <c r="M75">
-        <v>6.2665654222428507E-2</v>
+        <v>0.38281413160870664</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -7517,39 +7517,39 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76">
-        <v>1.6022318341714921E-2</v>
+        <v>0.54569339438146058</v>
       </c>
       <c r="G76">
         <v>0</v>
       </c>
       <c r="H76">
-        <v>-1.0616865599799663</v>
+        <v>-2.523399903135628</v>
       </c>
       <c r="I76">
         <v>0</v>
       </c>
       <c r="J76">
-        <v>0.93396082483092047</v>
+        <v>0.89559177374302767</v>
       </c>
       <c r="K76">
         <v>0</v>
       </c>
       <c r="L76">
-        <v>1.0575453182325425</v>
+        <v>2.5175969757962227</v>
       </c>
       <c r="M76">
-        <v>9.5041918181231075E-2</v>
+        <v>0.57186870807744916</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>-10</v>
+        <v>3</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -7558,39 +7558,39 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>-4.6563791707584221E-2</v>
+        <v>-5.128071050976004E-2</v>
       </c>
       <c r="G77">
         <v>0</v>
       </c>
       <c r="H77">
-        <v>0.46332119055672866</v>
+        <v>-0.60674342555727956</v>
       </c>
       <c r="I77">
         <v>0</v>
       </c>
       <c r="J77">
-        <v>1.0152388816190119</v>
+        <v>1.3126931746017902</v>
       </c>
       <c r="K77">
         <v>0</v>
       </c>
       <c r="L77">
-        <v>-0.44819658301982845</v>
+        <v>0.6032280797583166</v>
       </c>
       <c r="M77">
-        <v>0.12631126349792302</v>
+        <v>8.2964929448905295E-2</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -7599,534 +7599,534 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78">
-        <v>-7.4515806858318878E-2</v>
+        <v>-1.1924779959131403E-2</v>
       </c>
       <c r="G78">
         <v>0</v>
       </c>
       <c r="H78">
-        <v>-4.5358521817180072E-2</v>
+        <v>-0.95197972830722333</v>
       </c>
       <c r="I78">
         <v>0</v>
       </c>
       <c r="J78">
-        <v>0.84653828497766881</v>
+        <v>1.3932105676535247</v>
       </c>
       <c r="K78">
         <v>0</v>
       </c>
       <c r="L78">
-        <v>4.9196215546590351E-2</v>
+        <v>0.9455182048243409</v>
       </c>
       <c r="M78">
-        <v>7.203980392171612E-2</v>
+        <v>0.11136843282871728</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="B79">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79">
-        <v>-4.7505716244460337E-2</v>
+        <v>-7.273515734660975E-2</v>
       </c>
       <c r="G79">
-        <v>-9.1927912441848697E-2</v>
+        <v>0</v>
       </c>
       <c r="H79">
-        <v>-0.3972073187545293</v>
+        <v>0.50501444943067242</v>
       </c>
       <c r="I79">
-        <v>-2.7772150835726466E-3</v>
+        <v>0</v>
       </c>
       <c r="J79">
-        <v>0.60339027191894345</v>
+        <v>1.2261210668769142</v>
       </c>
       <c r="K79">
-        <v>8.3511717676247581E-3</v>
+        <v>0</v>
       </c>
       <c r="L79">
-        <v>0.3972073187545293</v>
+        <v>-0.48471181765696153</v>
       </c>
       <c r="M79">
-        <v>4.7505716244460337E-2</v>
+        <v>0.15932498571060855</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>12</v>
+        <v>-3</v>
       </c>
       <c r="B80">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="F80">
-        <v>0.21918338527098491</v>
+        <v>-9.8108715481738343E-2</v>
       </c>
       <c r="G80">
-        <v>-0.10936143335693478</v>
+        <v>0</v>
       </c>
       <c r="H80">
-        <v>-1.8066099806573888</v>
+        <v>3.6631169446297338E-2</v>
       </c>
       <c r="I80">
-        <v>3.4781461798756652E-3</v>
+        <v>0</v>
       </c>
       <c r="J80">
-        <v>0.65452518973355323</v>
+        <v>1.2019920439586451</v>
       </c>
       <c r="K80">
-        <v>1.4571289994414448E-2</v>
+        <v>0</v>
       </c>
       <c r="L80">
-        <v>1.8127020062726227</v>
+        <v>-3.1446354261168187E-2</v>
       </c>
       <c r="M80">
-        <v>0.16122163330318987</v>
+        <v>9.9891388178166493E-2</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B81">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0.35502696510795262</v>
+        <v>-6.9506435658708704E-2</v>
       </c>
       <c r="G81">
-        <v>-5.632605405318529E-2</v>
+        <v>0</v>
       </c>
       <c r="H81">
-        <v>-2.1778292202838712</v>
+        <v>-0.38543276188102249</v>
       </c>
       <c r="I81">
-        <v>2.3263079710197521E-3</v>
+        <v>0</v>
       </c>
       <c r="J81">
-        <v>0.66060889480146268</v>
+        <v>0.8757747552691485</v>
       </c>
       <c r="K81">
-        <v>7.8148588022492471E-3</v>
+        <v>0</v>
       </c>
       <c r="L81">
-        <v>2.1955092292140619</v>
+        <v>0.38543276188102249</v>
       </c>
       <c r="M81">
-        <v>0.22073396456343947</v>
+        <v>6.9506435658708704E-2</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B82">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82">
-        <v>0.55163035281987938</v>
+        <v>0.19825346612774047</v>
       </c>
       <c r="G82">
-        <v>-5.696113208327748E-2</v>
+        <v>0</v>
       </c>
       <c r="H82">
-        <v>-2.5984390803467101</v>
+        <v>-1.8003892255870124</v>
       </c>
       <c r="I82">
-        <v>4.3182000198387091E-3</v>
+        <v>0</v>
       </c>
       <c r="J82">
-        <v>0.71727025064819516</v>
+        <v>1.0042032638441956</v>
       </c>
       <c r="K82">
-        <v>9.0375173385818137E-3</v>
+        <v>0</v>
       </c>
       <c r="L82">
-        <v>2.6417255731941154</v>
+        <v>1.8022656147480305</v>
       </c>
       <c r="M82">
-        <v>0.27833019303960183</v>
+        <v>0.18040081579186187</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B83">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83">
-        <v>-3.3400760249008552E-3</v>
+        <v>0.35013168866706651</v>
       </c>
       <c r="G83">
-        <v>-9.4667950871191994E-2</v>
+        <v>0</v>
       </c>
       <c r="H83">
-        <v>-0.72137281145379484</v>
+        <v>-2.1757430242328892</v>
       </c>
       <c r="I83">
-        <v>-2.7330319478969314E-3</v>
+        <v>0</v>
       </c>
       <c r="J83">
-        <v>0.58733921900315789</v>
+        <v>1.0383394874624312</v>
       </c>
       <c r="K83">
-        <v>1.1036506388339591E-2</v>
+        <v>0</v>
       </c>
       <c r="L83">
-        <v>0.72020938901401477</v>
+        <v>2.1922271277957734</v>
       </c>
       <c r="M83">
-        <v>4.1089234461886816E-2</v>
+        <v>0.22492249123470398</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B84">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
-        <v>4.1247313377936731E-2</v>
+        <v>0.54186440388334123</v>
       </c>
       <c r="G84">
-        <v>-0.1013204080783493</v>
+        <v>0</v>
       </c>
       <c r="H84">
-        <v>-1.0708453123226094</v>
+        <v>-2.550474490105854</v>
       </c>
       <c r="I84">
-        <v>-1.9956999129138462E-3</v>
+        <v>0</v>
       </c>
       <c r="J84">
-        <v>0.60730047628207351</v>
+        <v>1.0574676302980566</v>
       </c>
       <c r="K84">
-        <v>1.2228822106443904E-2</v>
+        <v>0</v>
       </c>
       <c r="L84">
-        <v>1.0692906279386272</v>
+        <v>2.5930906929065345</v>
       </c>
       <c r="M84">
-        <v>7.0912458614977983E-2</v>
+        <v>0.27279628890084689</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>-10</v>
+        <v>22</v>
       </c>
       <c r="B85">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>-4.6016027279502686E-2</v>
+        <v>0.69502513502635788</v>
       </c>
       <c r="G85">
-        <v>-7.784002123974218E-2</v>
+        <v>0</v>
       </c>
       <c r="H85">
-        <v>0.39817095225636107</v>
+        <v>-2.7704264894431851</v>
       </c>
       <c r="I85">
-        <v>1.6575631411882306E-2</v>
+        <v>0</v>
       </c>
       <c r="J85">
-        <v>0.7114984781554804</v>
+        <v>0.87795100675087234</v>
       </c>
       <c r="K85">
-        <v>6.0144605612426332E-3</v>
+        <v>0</v>
       </c>
       <c r="L85">
-        <v>-0.38413124152576072</v>
+        <v>2.8290557094465236</v>
       </c>
       <c r="M85">
-        <v>0.11445860068689892</v>
+        <v>0.39340394580497529</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>-3</v>
+        <v>25</v>
       </c>
       <c r="B86">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C86">
         <v>0</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86">
-        <v>-5.680321631205857E-2</v>
+        <v>0.54353953160692858</v>
       </c>
       <c r="G86">
-        <v>-8.481552613842655E-2</v>
+        <v>0</v>
       </c>
       <c r="H86">
-        <v>-6.4259441263303296E-2</v>
+        <v>-2.5745798477787449</v>
       </c>
       <c r="I86">
-        <v>-3.0187146553080106E-3</v>
+        <v>0</v>
       </c>
       <c r="J86">
-        <v>0.60023980708646352</v>
+        <v>0.54974438996758113</v>
       </c>
       <c r="K86">
-        <v>6.5520842415802702E-3</v>
+        <v>0</v>
       </c>
       <c r="L86">
-        <v>6.71442265757278E-2</v>
+        <v>2.5630714964245831</v>
       </c>
       <c r="M86">
-        <v>5.3362290172122205E-2</v>
+        <v>0.59545034992327506</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B87">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87">
-        <v>-2.3364533049572544E-2</v>
+        <v>-2.5652572187046505E-2</v>
       </c>
       <c r="G87">
-        <v>-0.19641942417667502</v>
+        <v>0</v>
       </c>
       <c r="H87">
-        <v>-0.30084637733205799</v>
+        <v>-0.70789263545777181</v>
       </c>
       <c r="I87">
-        <v>-2.4212806579202743E-3</v>
+        <v>0</v>
       </c>
       <c r="J87">
-        <v>0.60271620419005245</v>
+        <v>0.88175100866170597</v>
       </c>
       <c r="K87">
-        <v>1.5651856650643513E-2</v>
+        <v>0</v>
       </c>
       <c r="L87">
-        <v>0.30084637733205799</v>
+        <v>0.7055799413078836</v>
       </c>
       <c r="M87">
-        <v>2.3364533049572544E-2</v>
+        <v>6.2665654222428507E-2</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88">
-        <v>0.20131901999215693</v>
+        <v>1.6022318341714921E-2</v>
       </c>
       <c r="G88">
-        <v>-0.2140853276862541</v>
+        <v>0</v>
       </c>
       <c r="H88">
-        <v>-1.5978304340908418</v>
+        <v>-1.0616865599799663</v>
       </c>
       <c r="I88">
-        <v>2.5996595099345016E-3</v>
+        <v>0</v>
       </c>
       <c r="J88">
-        <v>0.73759258791242588</v>
+        <v>0.93396082483092047</v>
       </c>
       <c r="K88">
-        <v>1.8409391591195663E-2</v>
+        <v>0</v>
       </c>
       <c r="L88">
-        <v>1.6047705833257557</v>
+        <v>1.0575453182325425</v>
       </c>
       <c r="M88">
-        <v>0.13528791080449187</v>
+        <v>9.5041918181231075E-2</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>15</v>
+        <v>-10</v>
       </c>
       <c r="B89">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89">
-        <v>0.32793787472970998</v>
+        <v>-4.6563791707584221E-2</v>
       </c>
       <c r="G89">
-        <v>-0.21217478562063638</v>
+        <v>0</v>
       </c>
       <c r="H89">
-        <v>-1.9352948053062868</v>
+        <v>0.46332119055672866</v>
       </c>
       <c r="I89">
-        <v>5.3145576626830839E-3</v>
+        <v>0</v>
       </c>
       <c r="J89">
-        <v>0.77104684638811694</v>
+        <v>1.0152388816190119</v>
       </c>
       <c r="K89">
-        <v>1.8521905389749266E-2</v>
+        <v>0</v>
       </c>
       <c r="L89">
-        <v>1.9542278015189098</v>
+        <v>-0.44819658301982845</v>
       </c>
       <c r="M89">
-        <v>0.18412749088146577</v>
+        <v>0.12631126349792302</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B90">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0.28571565201086574</v>
+        <v>-7.4515806858318878E-2</v>
       </c>
       <c r="G90">
-        <v>-0.23380216146242108</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>-1.9537223938165951</v>
+        <v>-4.5358521817180072E-2</v>
       </c>
       <c r="I90">
-        <v>2.1534872412220261E-2</v>
+        <v>0</v>
       </c>
       <c r="J90">
-        <v>0.52412751484017817</v>
+        <v>0.84653828497766881</v>
       </c>
       <c r="K90">
-        <v>1.7067399436774752E-2</v>
+        <v>0</v>
       </c>
       <c r="L90">
-        <v>1.946391405701315</v>
+        <v>4.9196215546590351E-2</v>
       </c>
       <c r="M90">
-        <v>0.33200168932777918</v>
+        <v>7.203980392171612E-2</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B91">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -8138,36 +8138,36 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <v>1.192535532286151E-2</v>
+        <v>-4.7505716244460337E-2</v>
       </c>
       <c r="G91">
-        <v>-0.1977505202515592</v>
+        <v>-9.1927912441848697E-2</v>
       </c>
       <c r="H91">
-        <v>-0.59298182651323161</v>
+        <v>-0.3972073187545293</v>
       </c>
       <c r="I91">
-        <v>-3.9364841775132121E-3</v>
+        <v>-2.7772150835726466E-3</v>
       </c>
       <c r="J91">
-        <v>0.6254041524460493</v>
+        <v>0.60339027191894345</v>
       </c>
       <c r="K91">
-        <v>1.7362751369570727E-2</v>
+        <v>8.3511717676247581E-3</v>
       </c>
       <c r="L91">
-        <v>0.59279329040318485</v>
+        <v>0.3972073187545293</v>
       </c>
       <c r="M91">
-        <v>1.9125258887405225E-2</v>
+        <v>4.7505716244460337E-2</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B92">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -8179,36 +8179,36 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <v>5.1070746880325146E-2</v>
+        <v>0.21918338527098491</v>
       </c>
       <c r="G92">
-        <v>-0.20563943801272749</v>
+        <v>-0.10936143335693478</v>
       </c>
       <c r="H92">
-        <v>-0.9084862820756171</v>
+        <v>-1.8066099806573888</v>
       </c>
       <c r="I92">
-        <v>-4.4806121859410578E-3</v>
+        <v>3.4781461798756652E-3</v>
       </c>
       <c r="J92">
-        <v>0.67356942233129458</v>
+        <v>0.65452518973355323</v>
       </c>
       <c r="K92">
-        <v>1.8293177597732562E-2</v>
+        <v>1.4571289994414448E-2</v>
       </c>
       <c r="L92">
-        <v>0.90884784585525014</v>
+        <v>1.8127020062726227</v>
       </c>
       <c r="M92">
-        <v>4.4171698979813906E-2</v>
+        <v>0.16122163330318987</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>-10</v>
+        <v>15</v>
       </c>
       <c r="B93">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -8220,36 +8220,36 @@
         <v>0</v>
       </c>
       <c r="F93">
-        <v>-5.0027938577338123E-2</v>
+        <v>0.35502696510795262</v>
       </c>
       <c r="G93">
-        <v>-0.16787578987678636</v>
+        <v>-5.632605405318529E-2</v>
       </c>
       <c r="H93">
-        <v>0.38554473622205221</v>
+        <v>-2.1778292202838712</v>
       </c>
       <c r="I93">
-        <v>2.575041145684303E-2</v>
+        <v>2.3263079710197521E-3</v>
       </c>
       <c r="J93">
-        <v>0.58381833783153814</v>
+        <v>0.66060889480146268</v>
       </c>
       <c r="K93">
-        <v>1.3972419247413822E-2</v>
+        <v>7.8148588022492471E-3</v>
       </c>
       <c r="L93">
-        <v>-0.37100018499813575</v>
+        <v>2.1955092292140619</v>
       </c>
       <c r="M93">
-        <v>0.1162170426322178</v>
+        <v>0.22073396456343947</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>-3</v>
+        <v>18</v>
       </c>
       <c r="B94">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -8261,36 +8261,36 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <v>-4.2445598853748108E-2</v>
+        <v>0.55163035281987938</v>
       </c>
       <c r="G94">
-        <v>-0.17410989314356345</v>
+        <v>-5.696113208327748E-2</v>
       </c>
       <c r="H94">
-        <v>-6.5695455195958236E-2</v>
+        <v>-2.5984390803467101</v>
       </c>
       <c r="I94">
-        <v>4.3400079189802607E-3</v>
+        <v>4.3182000198387091E-3</v>
       </c>
       <c r="J94">
-        <v>0.60973770489389667</v>
+        <v>0.71727025064819516</v>
       </c>
       <c r="K94">
-        <v>1.5545018857230822E-2</v>
+        <v>9.0375173385818137E-3</v>
       </c>
       <c r="L94">
-        <v>6.7826852862145043E-2</v>
+        <v>2.6417255731941154</v>
       </c>
       <c r="M94">
-        <v>3.8949194167201794E-2</v>
+        <v>0.27833019303960183</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B95">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -8302,36 +8302,36 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <v>1.4562382430074136E-2</v>
+        <v>-3.3400760249008552E-3</v>
       </c>
       <c r="G95">
-        <v>-0.34117274201218539</v>
+        <v>-9.4667950871191994E-2</v>
       </c>
       <c r="H95">
-        <v>-0.26292881549732261</v>
+        <v>-0.72137281145379484</v>
       </c>
       <c r="I95">
-        <v>1.2974792629972969E-2</v>
+        <v>-2.7330319478969314E-3</v>
       </c>
       <c r="J95">
-        <v>0.13071235106523052</v>
+        <v>0.58733921900315789</v>
       </c>
       <c r="K95">
-        <v>3.6569708865806155E-2</v>
+        <v>1.1036506388339591E-2</v>
       </c>
       <c r="L95">
-        <v>0.26292881549732261</v>
+        <v>0.72020938901401477</v>
       </c>
       <c r="M95">
-        <v>-1.4562382430074136E-2</v>
+        <v>4.1089234461886816E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B96">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -8343,36 +8343,36 @@
         <v>0</v>
       </c>
       <c r="F96">
-        <v>6.6744928603131207E-2</v>
+        <v>4.1247313377936731E-2</v>
       </c>
       <c r="G96">
-        <v>-0.35855411499705614</v>
+        <v>-0.1013204080783493</v>
       </c>
       <c r="H96">
-        <v>-0.88189487677332457</v>
+        <v>-1.0708453123226094</v>
       </c>
       <c r="I96">
-        <v>1.1494985182503414E-3</v>
+        <v>-1.9956999129138462E-3</v>
       </c>
       <c r="J96">
-        <v>0.50424292019560746</v>
+        <v>0.60730047628207351</v>
       </c>
       <c r="K96">
-        <v>1.5293832187298809E-2</v>
+        <v>1.2228822106443904E-2</v>
       </c>
       <c r="L96">
-        <v>0.8765004087746503</v>
+        <v>1.0692906279386272</v>
       </c>
       <c r="M96">
-        <v>0.11806986317915942</v>
+        <v>7.0912458614977983E-2</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>15</v>
+        <v>-10</v>
       </c>
       <c r="B97">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -8384,36 +8384,36 @@
         <v>0</v>
       </c>
       <c r="F97">
-        <v>7.4681583023926496E-2</v>
+        <v>-4.6016027279502686E-2</v>
       </c>
       <c r="G97">
-        <v>-0.42493755420952761</v>
+        <v>-7.784002123974218E-2</v>
       </c>
       <c r="H97">
-        <v>-0.89827728298763987</v>
+        <v>0.39817095225636107</v>
       </c>
       <c r="I97">
-        <v>6.6431830838151089E-3</v>
+        <v>1.6575631411882306E-2</v>
       </c>
       <c r="J97">
-        <v>0.35353635633790342</v>
+        <v>0.7114984781554804</v>
       </c>
       <c r="K97">
-        <v>1.2082185600684459E-2</v>
+        <v>6.0144605612426332E-3</v>
       </c>
       <c r="L97">
-        <v>0.88699824281153261</v>
+        <v>-0.38413124152576072</v>
       </c>
       <c r="M97">
-        <v>0.16035439882918592</v>
+        <v>0.11445860068689892</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B98">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -8425,36 +8425,36 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <v>0.12838033746056865</v>
+        <v>-5.680321631205857E-2</v>
       </c>
       <c r="G98">
-        <v>-0.41139940038735839</v>
+        <v>-8.481552613842655E-2</v>
       </c>
       <c r="H98">
-        <v>-1.1484398118795685</v>
+        <v>-6.4259441263303296E-2</v>
       </c>
       <c r="I98">
-        <v>1.1027315119311985E-2</v>
+        <v>-3.0187146553080106E-3</v>
       </c>
       <c r="J98">
-        <v>0.36333856542398846</v>
+        <v>0.60023980708646352</v>
       </c>
       <c r="K98">
-        <v>1.1973187671428076E-2</v>
+        <v>6.5520842415802702E-3</v>
       </c>
       <c r="L98">
-        <v>1.1319028726797504</v>
+        <v>6.71442265757278E-2</v>
       </c>
       <c r="M98">
-        <v>0.23279046238150966</v>
+        <v>5.3362290172122205E-2</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B99">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -8466,36 +8466,36 @@
         <v>0</v>
       </c>
       <c r="F99">
-        <v>4.0050776551835844E-2</v>
+        <v>-2.3364533049572544E-2</v>
       </c>
       <c r="G99">
-        <v>-0.34906734647434196</v>
+        <v>-0.19641942417667502</v>
       </c>
       <c r="H99">
-        <v>-0.42120721955691437</v>
+        <v>-0.30084637733205799</v>
       </c>
       <c r="I99">
-        <v>9.6645159441334314E-3</v>
+        <v>-2.4212806579202743E-3</v>
       </c>
       <c r="J99">
-        <v>0.21134821837795698</v>
+        <v>0.60271620419005245</v>
       </c>
       <c r="K99">
-        <v>3.5861930521240704E-2</v>
+        <v>1.5651856650643513E-2</v>
       </c>
       <c r="L99">
-        <v>0.42272606539050189</v>
+        <v>0.30084637733205799</v>
       </c>
       <c r="M99">
-        <v>-1.7951605742576524E-2</v>
+        <v>2.3364533049572544E-2</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B100">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -8507,36 +8507,36 @@
         <v>0</v>
       </c>
       <c r="F100">
-        <v>3.6049260753956452E-2</v>
+        <v>0.20131901999215693</v>
       </c>
       <c r="G100">
-        <v>-0.33714576611907043</v>
+        <v>-0.2140853276862541</v>
       </c>
       <c r="H100">
-        <v>-0.58307267326184264</v>
+        <v>-1.5978304340908418</v>
       </c>
       <c r="I100">
-        <v>5.1722990716013108E-3</v>
+        <v>2.5996595099345016E-3</v>
       </c>
       <c r="J100">
-        <v>0.37265308151036075</v>
+        <v>0.73759258791242588</v>
       </c>
       <c r="K100">
-        <v>2.5274150641253865E-2</v>
+        <v>1.8409391591195663E-2</v>
       </c>
       <c r="L100">
-        <v>0.58364671397835965</v>
+        <v>1.6047705833257557</v>
       </c>
       <c r="M100">
-        <v>2.5095911377773148E-2</v>
+        <v>0.13528791080449187</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>-10</v>
+        <v>15</v>
       </c>
       <c r="B101">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -8548,36 +8548,36 @@
         <v>0</v>
       </c>
       <c r="F101">
-        <v>-5.2596574343978866E-2</v>
+        <v>0.32793787472970998</v>
       </c>
       <c r="G101">
-        <v>-0.36697881086611123</v>
+        <v>-0.21217478562063638</v>
       </c>
       <c r="H101">
-        <v>0.16282144189795822</v>
+        <v>-1.9352948053062868</v>
       </c>
       <c r="I101">
-        <v>2.054244668063852E-2</v>
+        <v>5.3145576626830839E-3</v>
       </c>
       <c r="J101">
-        <v>1.8191006122906254E-2</v>
+        <v>0.77104684638811694</v>
       </c>
       <c r="K101">
-        <v>3.2009131654802486E-2</v>
+        <v>1.8521905389749266E-2</v>
       </c>
       <c r="L101">
-        <v>-0.15121451905138086</v>
+        <v>1.9542278015189098</v>
       </c>
       <c r="M101">
-        <v>8.0071160866515792E-2</v>
+        <v>0.18412749088146577</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>-3</v>
+        <v>18</v>
       </c>
       <c r="B102">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -8589,36 +8589,36 @@
         <v>0</v>
       </c>
       <c r="F102">
-        <v>-1.1467350049231788E-2</v>
+        <v>0.28571565201086574</v>
       </c>
       <c r="G102">
-        <v>-0.33984985556685265</v>
+        <v>-0.23380216146242108</v>
       </c>
       <c r="H102">
-        <v>-0.12936593336962468</v>
+        <v>-1.9537223938165951</v>
       </c>
       <c r="I102">
-        <v>1.6670300320380294E-2</v>
+        <v>2.1534872412220261E-2</v>
       </c>
       <c r="J102">
-        <v>3.0627950040284596E-2</v>
+        <v>0.52412751484017817</v>
       </c>
       <c r="K102">
-        <v>3.5839742035837806E-2</v>
+        <v>1.7067399436774752E-2</v>
       </c>
       <c r="L102">
-        <v>0.1297887965843986</v>
+        <v>1.946391405701315</v>
       </c>
       <c r="M102">
-        <v>4.681144616371917E-3</v>
+        <v>0.33200168932777918</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B103">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -8630,36 +8630,36 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <v>-5.9277281356348716E-2</v>
+        <v>1.192535532286151E-2</v>
       </c>
       <c r="G103">
-        <v>-4.5795131572825248E-2</v>
+        <v>-0.1977505202515592</v>
       </c>
       <c r="H103">
-        <v>-0.45321817305868006</v>
+        <v>-0.59298182651323161</v>
       </c>
       <c r="I103">
-        <v>4.790722037972777E-4</v>
+        <v>-3.9364841775132121E-3</v>
       </c>
       <c r="J103">
-        <v>0.53588946501178747</v>
+        <v>0.6254041524460493</v>
       </c>
       <c r="K103">
-        <v>4.556494574114188E-3</v>
+        <v>1.7362751369570727E-2</v>
       </c>
       <c r="L103">
-        <v>0.45321817305868006</v>
+        <v>0.59279329040318485</v>
       </c>
       <c r="M103">
-        <v>5.9277281356348716E-2</v>
+        <v>1.9125258887405225E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B104">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -8671,36 +8671,36 @@
         <v>0</v>
       </c>
       <c r="F104">
-        <v>0.21367986198260264</v>
+        <v>5.1070746880325146E-2</v>
       </c>
       <c r="G104">
-        <v>-5.5995179334707809E-2</v>
+        <v>-0.20563943801272749</v>
       </c>
       <c r="H104">
-        <v>-1.8566323867473109</v>
+        <v>-0.9084862820756171</v>
       </c>
       <c r="I104">
-        <v>1.3720205605942724E-3</v>
+        <v>-4.4806121859410578E-3</v>
       </c>
       <c r="J104">
-        <v>0.6358839619235559</v>
+        <v>0.67356942233129458</v>
       </c>
       <c r="K104">
-        <v>7.46922132412831E-3</v>
+        <v>1.8293177597732562E-2</v>
       </c>
       <c r="L104">
-        <v>1.8604870559400697</v>
+        <v>0.90884784585525014</v>
       </c>
       <c r="M104">
-        <v>0.17700513443223193</v>
+        <v>4.4171698979813906E-2</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>15</v>
+        <v>-10</v>
       </c>
       <c r="B105">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -8712,36 +8712,36 @@
         <v>0</v>
       </c>
       <c r="F105">
-        <v>0.36353755884268868</v>
+        <v>-5.0027938577338123E-2</v>
       </c>
       <c r="G105">
-        <v>-5.6972347940228305E-2</v>
+        <v>-0.16787578987678636</v>
       </c>
       <c r="H105">
-        <v>-2.2294407327960712</v>
+        <v>0.38554473622205221</v>
       </c>
       <c r="I105">
-        <v>2.4192421146164793E-3</v>
+        <v>2.575041145684303E-2</v>
       </c>
       <c r="J105">
-        <v>0.67650698563225609</v>
+        <v>0.58381833783153814</v>
       </c>
       <c r="K105">
-        <v>7.9294107456995833E-3</v>
+        <v>1.3972419247413822E-2</v>
       </c>
       <c r="L105">
-        <v>2.2475648258271175</v>
+        <v>-0.37100018499813575</v>
       </c>
       <c r="M105">
-        <v>0.22587140466270847</v>
+        <v>0.1162170426322178</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B106">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -8753,36 +8753,36 @@
         <v>0</v>
       </c>
       <c r="F106">
-        <v>0.55163035281987971</v>
+        <v>-4.2445598853748108E-2</v>
       </c>
       <c r="G106">
-        <v>-5.696113208327757E-2</v>
+        <v>-0.17410989314356345</v>
       </c>
       <c r="H106">
-        <v>-2.5984390803467106</v>
+        <v>-6.5695455195958236E-2</v>
       </c>
       <c r="I106">
-        <v>4.3182000198383787E-3</v>
+        <v>4.3400079189802607E-3</v>
       </c>
       <c r="J106">
-        <v>0.7172702506481976</v>
+        <v>0.60973770489389667</v>
       </c>
       <c r="K106">
-        <v>9.0375173385817253E-3</v>
+        <v>1.5545018857230822E-2</v>
       </c>
       <c r="L106">
-        <v>2.6417255731941163</v>
+        <v>6.7826852862145043E-2</v>
       </c>
       <c r="M106">
-        <v>0.27833019303960171</v>
+        <v>3.8949194167201794E-2</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B107">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -8794,36 +8794,36 @@
         <v>0</v>
       </c>
       <c r="F107">
-        <v>-1.244184118689425E-2</v>
+        <v>1.4562382430074136E-2</v>
       </c>
       <c r="G107">
-        <v>-4.7149660580241247E-2</v>
+        <v>-0.34117274201218539</v>
       </c>
       <c r="H107">
-        <v>-0.77286250802460776</v>
+        <v>-0.26292881549732261</v>
       </c>
       <c r="I107">
-        <v>7.0525740867477874E-5</v>
+        <v>1.2974792629972969E-2</v>
       </c>
       <c r="J107">
-        <v>0.53531573297310986</v>
+        <v>0.13071235106523052</v>
       </c>
       <c r="K107">
-        <v>5.8990528070585998E-3</v>
+        <v>3.6569708865806155E-2</v>
       </c>
       <c r="L107">
-        <v>0.77115217116192813</v>
+        <v>0.26292881549732261</v>
       </c>
       <c r="M107">
-        <v>5.2873288477746201E-2</v>
+        <v>-1.4562382430074136E-2</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B108">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -8835,36 +8835,36 @@
         <v>0</v>
       </c>
       <c r="F108">
-        <v>3.1097407134985693E-2</v>
+        <v>6.6744928603131207E-2</v>
       </c>
       <c r="G108">
-        <v>-5.1040282578760213E-2</v>
+        <v>-0.35855411499705614</v>
       </c>
       <c r="H108">
-        <v>-1.1291257642886272</v>
+        <v>-0.88189487677332457</v>
       </c>
       <c r="I108">
-        <v>1.1886544626932207E-3</v>
+        <v>1.1494985182503414E-3</v>
       </c>
       <c r="J108">
-        <v>0.57099008130640638</v>
+        <v>0.50424292019560746</v>
       </c>
       <c r="K108">
-        <v>6.4517436041181403E-3</v>
+        <v>1.5293832187298809E-2</v>
       </c>
       <c r="L108">
-        <v>1.1261908593889041</v>
+        <v>0.8765004087746503</v>
       </c>
       <c r="M108">
-        <v>8.7098728692080046E-2</v>
+        <v>0.11806986317915942</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>-10</v>
+        <v>15</v>
       </c>
       <c r="B109">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -8876,36 +8876,36 @@
         <v>0</v>
       </c>
       <c r="F109">
-        <v>-4.9948081335520665E-2</v>
+        <v>7.4681583023926496E-2</v>
       </c>
       <c r="G109">
-        <v>-5.0781022524719055E-2</v>
+        <v>-0.42493755420952761</v>
       </c>
       <c r="H109">
-        <v>0.36739139563870138</v>
+        <v>-0.89827728298763987</v>
       </c>
       <c r="I109">
-        <v>1.2529484356126138E-2</v>
+        <v>6.6431830838151089E-3</v>
       </c>
       <c r="J109">
-        <v>0.63690731732829309</v>
+        <v>0.35353635633790342</v>
       </c>
       <c r="K109">
-        <v>6.6491395005249922E-3</v>
+        <v>1.2082185600684459E-2</v>
       </c>
       <c r="L109">
-        <v>-0.35313650151309578</v>
+        <v>0.88699824281153261</v>
       </c>
       <c r="M109">
-        <v>0.11298610409047583</v>
+        <v>0.16035439882918592</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>-3</v>
+        <v>18</v>
       </c>
       <c r="B110">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -8917,68 +8917,560 @@
         <v>0</v>
       </c>
       <c r="F110">
-        <v>-6.6442545327944177E-2</v>
+        <v>0.12838033746056865</v>
       </c>
       <c r="G110">
-        <v>-4.4139661548338129E-2</v>
+        <v>-0.41139940038735839</v>
       </c>
       <c r="H110">
-        <v>-0.11865632733292179</v>
+        <v>-1.1484398118795685</v>
       </c>
       <c r="I110">
-        <v>1.1833717698856931E-3</v>
+        <v>1.1027315119311985E-2</v>
       </c>
       <c r="J110">
-        <v>0.50261730802701676</v>
+        <v>0.36333856542398846</v>
       </c>
       <c r="K110">
-        <v>4.2277992011485969E-3</v>
+        <v>1.1973187671428076E-2</v>
       </c>
       <c r="L110">
-        <v>0.12197104710511522</v>
+        <v>1.1319028726797504</v>
       </c>
       <c r="M110">
-        <v>6.0141495773510356E-2</v>
+        <v>0.23279046238150966</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B111">
+        <v>45</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>4.0050776551835844E-2</v>
+      </c>
+      <c r="G111">
+        <v>-0.34906734647434196</v>
+      </c>
+      <c r="H111">
+        <v>-0.42120721955691437</v>
+      </c>
+      <c r="I111">
+        <v>9.6645159441334314E-3</v>
+      </c>
+      <c r="J111">
+        <v>0.21134821837795698</v>
+      </c>
+      <c r="K111">
+        <v>3.5861930521240704E-2</v>
+      </c>
+      <c r="L111">
+        <v>0.42272606539050189</v>
+      </c>
+      <c r="M111">
+        <v>-1.7951605742576524E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>6</v>
+      </c>
+      <c r="B112">
+        <v>45</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>3.6049260753956452E-2</v>
+      </c>
+      <c r="G112">
+        <v>-0.33714576611907043</v>
+      </c>
+      <c r="H112">
+        <v>-0.58307267326184264</v>
+      </c>
+      <c r="I112">
+        <v>5.1722990716013108E-3</v>
+      </c>
+      <c r="J112">
+        <v>0.37265308151036075</v>
+      </c>
+      <c r="K112">
+        <v>2.5274150641253865E-2</v>
+      </c>
+      <c r="L112">
+        <v>0.58364671397835965</v>
+      </c>
+      <c r="M112">
+        <v>2.5095911377773148E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>-10</v>
+      </c>
+      <c r="B113">
+        <v>45</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>-5.2596574343978866E-2</v>
+      </c>
+      <c r="G113">
+        <v>-0.36697881086611123</v>
+      </c>
+      <c r="H113">
+        <v>0.16282144189795822</v>
+      </c>
+      <c r="I113">
+        <v>2.054244668063852E-2</v>
+      </c>
+      <c r="J113">
+        <v>1.8191006122906254E-2</v>
+      </c>
+      <c r="K113">
+        <v>3.2009131654802486E-2</v>
+      </c>
+      <c r="L113">
+        <v>-0.15121451905138086</v>
+      </c>
+      <c r="M113">
+        <v>8.0071160866515792E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>-3</v>
+      </c>
+      <c r="B114">
+        <v>45</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>-1.1467350049231788E-2</v>
+      </c>
+      <c r="G114">
+        <v>-0.33984985556685265</v>
+      </c>
+      <c r="H114">
+        <v>-0.12936593336962468</v>
+      </c>
+      <c r="I114">
+        <v>1.6670300320380294E-2</v>
+      </c>
+      <c r="J114">
+        <v>3.0627950040284596E-2</v>
+      </c>
+      <c r="K114">
+        <v>3.5839742035837806E-2</v>
+      </c>
+      <c r="L114">
+        <v>0.1297887965843986</v>
+      </c>
+      <c r="M114">
+        <v>4.681144616371917E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>5</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>-5.9277281356348716E-2</v>
+      </c>
+      <c r="G115">
+        <v>-4.5795131572825248E-2</v>
+      </c>
+      <c r="H115">
+        <v>-0.45321817305868006</v>
+      </c>
+      <c r="I115">
+        <v>4.790722037972777E-4</v>
+      </c>
+      <c r="J115">
+        <v>0.53588946501178747</v>
+      </c>
+      <c r="K115">
+        <v>4.556494574114188E-3</v>
+      </c>
+      <c r="L115">
+        <v>0.45321817305868006</v>
+      </c>
+      <c r="M115">
+        <v>5.9277281356348716E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>12</v>
+      </c>
+      <c r="B116">
+        <v>5</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>0.21367986198260264</v>
+      </c>
+      <c r="G116">
+        <v>-5.5995179334707809E-2</v>
+      </c>
+      <c r="H116">
+        <v>-1.8566323867473109</v>
+      </c>
+      <c r="I116">
+        <v>1.3720205605942724E-3</v>
+      </c>
+      <c r="J116">
+        <v>0.6358839619235559</v>
+      </c>
+      <c r="K116">
+        <v>7.46922132412831E-3</v>
+      </c>
+      <c r="L116">
+        <v>1.8604870559400697</v>
+      </c>
+      <c r="M116">
+        <v>0.17700513443223193</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>15</v>
+      </c>
+      <c r="B117">
+        <v>5</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>0.36353755884268868</v>
+      </c>
+      <c r="G117">
+        <v>-5.6972347940228305E-2</v>
+      </c>
+      <c r="H117">
+        <v>-2.2294407327960712</v>
+      </c>
+      <c r="I117">
+        <v>2.4192421146164793E-3</v>
+      </c>
+      <c r="J117">
+        <v>0.67650698563225609</v>
+      </c>
+      <c r="K117">
+        <v>7.9294107456995833E-3</v>
+      </c>
+      <c r="L117">
+        <v>2.2475648258271175</v>
+      </c>
+      <c r="M117">
+        <v>0.22587140466270847</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>18</v>
+      </c>
+      <c r="B118">
+        <v>5</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0.55163035281987971</v>
+      </c>
+      <c r="G118">
+        <v>-5.696113208327757E-2</v>
+      </c>
+      <c r="H118">
+        <v>-2.5984390803467106</v>
+      </c>
+      <c r="I118">
+        <v>4.3182000198383787E-3</v>
+      </c>
+      <c r="J118">
+        <v>0.7172702506481976</v>
+      </c>
+      <c r="K118">
+        <v>9.0375173385817253E-3</v>
+      </c>
+      <c r="L118">
+        <v>2.6417255731941163</v>
+      </c>
+      <c r="M118">
+        <v>0.27833019303960171</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>3</v>
+      </c>
+      <c r="B119">
+        <v>5</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>-1.244184118689425E-2</v>
+      </c>
+      <c r="G119">
+        <v>-4.7149660580241247E-2</v>
+      </c>
+      <c r="H119">
+        <v>-0.77286250802460776</v>
+      </c>
+      <c r="I119">
+        <v>7.0525740867477874E-5</v>
+      </c>
+      <c r="J119">
+        <v>0.53531573297310986</v>
+      </c>
+      <c r="K119">
+        <v>5.8990528070585998E-3</v>
+      </c>
+      <c r="L119">
+        <v>0.77115217116192813</v>
+      </c>
+      <c r="M119">
+        <v>5.2873288477746201E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>6</v>
+      </c>
+      <c r="B120">
+        <v>5</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>3.1097407134985693E-2</v>
+      </c>
+      <c r="G120">
+        <v>-5.1040282578760213E-2</v>
+      </c>
+      <c r="H120">
+        <v>-1.1291257642886272</v>
+      </c>
+      <c r="I120">
+        <v>1.1886544626932207E-3</v>
+      </c>
+      <c r="J120">
+        <v>0.57099008130640638</v>
+      </c>
+      <c r="K120">
+        <v>6.4517436041181403E-3</v>
+      </c>
+      <c r="L120">
+        <v>1.1261908593889041</v>
+      </c>
+      <c r="M120">
+        <v>8.7098728692080046E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>-10</v>
+      </c>
+      <c r="B121">
+        <v>5</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>-4.9948081335520665E-2</v>
+      </c>
+      <c r="G121">
+        <v>-5.0781022524719055E-2</v>
+      </c>
+      <c r="H121">
+        <v>0.36739139563870138</v>
+      </c>
+      <c r="I121">
+        <v>1.2529484356126138E-2</v>
+      </c>
+      <c r="J121">
+        <v>0.63690731732829309</v>
+      </c>
+      <c r="K121">
+        <v>6.6491395005249922E-3</v>
+      </c>
+      <c r="L121">
+        <v>-0.35313650151309578</v>
+      </c>
+      <c r="M121">
+        <v>0.11298610409047583</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>-3</v>
+      </c>
+      <c r="B122">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>-6.6442545327944177E-2</v>
+      </c>
+      <c r="G122">
+        <v>-4.4139661548338129E-2</v>
+      </c>
+      <c r="H122">
+        <v>-0.11865632733292179</v>
+      </c>
+      <c r="I122">
+        <v>1.1833717698856931E-3</v>
+      </c>
+      <c r="J122">
+        <v>0.50261730802701676</v>
+      </c>
+      <c r="K122">
+        <v>4.2277992011485969E-3</v>
+      </c>
+      <c r="L122">
+        <v>0.12197104710511522</v>
+      </c>
+      <c r="M122">
+        <v>6.0141495773510356E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>0</v>
+      </c>
+      <c r="B123">
         <v>90</v>
       </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-      <c r="D111">
-        <v>0</v>
-      </c>
-      <c r="E111">
-        <v>0</v>
-      </c>
-      <c r="F111">
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
         <v>1.7041213729324382E-2</v>
       </c>
-      <c r="G111">
+      <c r="G123">
         <v>-0.36392368744617631</v>
       </c>
-      <c r="H111">
+      <c r="H123">
         <v>-3.6261797567294335E-2</v>
       </c>
-      <c r="I111">
+      <c r="I123">
         <v>-4.0247807343861446E-4</v>
       </c>
-      <c r="J111">
+      <c r="J123">
         <v>1.072780736646251E-2</v>
       </c>
-      <c r="K111">
+      <c r="K123">
         <v>4.3191758762539965E-2</v>
       </c>
-      <c r="L111">
+      <c r="L123">
         <v>3.6261797567294335E-2</v>
       </c>
-      <c r="M111">
+      <c r="M123">
         <v>-1.7041213729324382E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Todos los datos y tablas CFD del modelado aerodinamico
</commit_message>
<xml_diff>
--- a/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
+++ b/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Posición de BAC desde morro</t>
   </si>
@@ -189,6 +189,33 @@
     <t>Y_r</t>
   </si>
   <si>
+    <t>C_l_p</t>
+  </si>
+  <si>
+    <t>C_l_r</t>
+  </si>
+  <si>
+    <t>C_Lift_q</t>
+  </si>
+  <si>
+    <t>C_D_q</t>
+  </si>
+  <si>
+    <t>C_Y_r</t>
+  </si>
+  <si>
+    <t>C_Y_p</t>
+  </si>
+  <si>
+    <t>C_m_q</t>
+  </si>
+  <si>
+    <t>C_n_p</t>
+  </si>
+  <si>
+    <t>C_n_r</t>
+  </si>
+  <si>
     <t>alfa_deg</t>
   </si>
   <si>
@@ -223,7 +250,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -272,6 +299,11 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -347,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -378,6 +410,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -706,10 +739,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -741,10 +774,10 @@
       <c r="B4" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
@@ -3782,7 +3815,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4045,12 +4078,12 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4147,7 +4180,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="29" t="s">
         <v>49</v>
       </c>
       <c r="I4" s="16"/>
@@ -4157,7 +4190,7 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B5" s="20">
         <v>-34.450000000000003</v>
@@ -4169,10 +4202,12 @@
       <c r="D5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="29"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
@@ -4180,7 +4215,7 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B6" s="20">
         <f>0.5*'Datos referencia'!B6*B2^2*F3*I3*H3*(ATAN(1*E3/B2))*D3</f>
@@ -4191,10 +4226,12 @@
         <v>3.4654185834361195E-2</v>
       </c>
       <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
-      <c r="H6" s="29"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
@@ -4202,7 +4239,7 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B7" s="21">
         <f>-0.5*'Datos referencia'!B6*B2^2*F3*I3*H3*(ATAN(1*E3/B2))*E3</f>
@@ -4213,10 +4250,12 @@
         <v>-0.18267811909579604</v>
       </c>
       <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="29"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
@@ -4224,7 +4263,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B8" s="20">
         <f>-0.5*'Datos referencia'!B6*B2^2*F3*I3*H3*(ATAN(1*D3/B2))*D3</f>
@@ -4235,7 +4274,9 @@
         <v>-6.5797446962677876E-3</v>
       </c>
       <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="E8" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
@@ -4246,7 +4287,7 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B9" s="20">
         <f>-0.5*'Datos referencia'!B6*B2^2*G3*I3*H3*(ATAN(1*E3/20))*E3</f>
@@ -4257,7 +4298,9 @@
         <v>-45.782830616102778</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="16"/>
+      <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
@@ -4268,7 +4311,7 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B10" s="21">
         <f>0.5*'Datos referencia'!B6*B2^2*G3*I3*H3*(ATAN(1*E3/20))</f>
@@ -4279,7 +4322,9 @@
         <v>10.900673956214945</v>
       </c>
       <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -4290,7 +4335,7 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B11" s="21">
         <f>0.5*'Datos referencia'!B6*B2^2*G3*J3*H3*(ATAN(1*E3/20))</f>
@@ -4301,7 +4346,9 @@
         <v>3.3631843422078783E-2</v>
       </c>
       <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="E11" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
@@ -4311,8 +4358,8 @@
       <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>53</v>
+      <c r="A12" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="B12" s="12">
         <f>-0.5*'Datos referencia'!B6*B2^2*F3*I3*H3*(ATAN(1*D3/20))</f>
@@ -4323,7 +4370,9 @@
         <v>-9.9099583606675326E-2</v>
       </c>
       <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+      <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
@@ -4334,7 +4383,7 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B13" s="12">
         <f>0.5*'Datos referencia'!B6*B2^2*F3*I3*H3*(ATAN(1*E3/B2))</f>
@@ -4345,7 +4394,9 @@
         <v>0.52193748313084587</v>
       </c>
       <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
@@ -4418,43 +4469,44 @@
     <hyperlink ref="D1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M123"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M123"/>
+      <selection activeCell="K1" sqref="K1:M129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -4797,7 +4849,7 @@
         <v>2.6159032424309991</v>
       </c>
       <c r="M9">
-        <v>0.47915250343567961</v>
+        <v>0.48910522850428789</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -4838,7 +4890,7 @@
         <v>2.2021087267983255</v>
       </c>
       <c r="M10">
-        <v>0.4476689776281999</v>
+        <v>0.50265478274679631</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -4879,7 +4931,7 @@
         <v>1.1797165676830084</v>
       </c>
       <c r="M11">
-        <v>0.28827286783673722</v>
+        <v>0.51932025936886261</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -4920,7 +4972,7 @@
         <v>2.7904571080549445</v>
       </c>
       <c r="M12">
-        <v>0.46571317345940377</v>
+        <v>0.4655552196062786</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -5002,7 +5054,7 @@
         <v>2.7856670546677567</v>
       </c>
       <c r="M14">
-        <v>0.59905399448358443</v>
+        <v>0.60422455801932451</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -5043,7 +5095,7 @@
         <v>2.3582835261975021</v>
       </c>
       <c r="M15">
-        <v>0.54796083267641138</v>
+        <v>0.59457233560527789</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -5084,7 +5136,7 @@
         <v>1.2908468906059773</v>
       </c>
       <c r="M16">
-        <v>0.34928342370854448</v>
+        <v>0.5714944072333854</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -5125,7 +5177,7 @@
         <v>2.8556608596391975</v>
       </c>
       <c r="M17">
-        <v>0.58513802914613056</v>
+        <v>0.58603026498810507</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -5207,7 +5259,7 @@
         <v>1.4552774960110393</v>
       </c>
       <c r="M19">
-        <v>1.0136972085446088</v>
+        <v>1.0204630191563318</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -5248,7 +5300,7 @@
         <v>1.4773585450330173</v>
       </c>
       <c r="M20">
-        <v>0.94397012748038178</v>
+        <v>0.96976636741979672</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -5289,7 +5341,7 @@
         <v>1.2816085670899657</v>
       </c>
       <c r="M21">
-        <v>0.60569334853151069</v>
+        <v>0.76113146441353707</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -5330,7 +5382,7 @@
         <v>1.4681689489973853</v>
       </c>
       <c r="M22">
-        <v>1.0307654858374153</v>
+        <v>1.0307253672546959</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -5909,7 +5961,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5924,33 +5976,33 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>-2.3304508550854926E-2</v>
+        <v>-1.5557685578775272E-2</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>-0.97656185923510674</v>
+        <v>-1.8203475590159175</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37">
-        <v>-0.24467922970624151</v>
+        <v>-0.35668664230964209</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>0.97400385140723522</v>
+        <v>1.4822179024322213</v>
       </c>
       <c r="M37">
-        <v>7.4381869265280662E-2</v>
+        <v>1.0568525757669345</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -5965,33 +6017,33 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>2.6952950831595199E-2</v>
+        <v>-2.3304508550854926E-2</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>-1.3307533742524675</v>
+        <v>-0.97656185923510674</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
       <c r="J38">
-        <v>-0.21095811311478116</v>
+        <v>-0.24467922970624151</v>
       </c>
       <c r="K38">
         <v>0</v>
       </c>
       <c r="L38">
-        <v>1.3262807185602445</v>
+        <v>0.97400385140723522</v>
       </c>
       <c r="M38">
-        <v>0.11229630545204901</v>
+        <v>7.4381869265280662E-2</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -6006,33 +6058,33 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>-7.718607828718764E-2</v>
+        <v>2.6952950831595199E-2</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0.18832547032290964</v>
+        <v>-1.3307533742524675</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39">
-        <v>-0.14746361651005876</v>
+        <v>-0.21095811311478116</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>-0.17206116142784475</v>
+        <v>1.3262807185602445</v>
       </c>
       <c r="M39">
-        <v>0.10871582305167048</v>
+        <v>0.11229630545204901</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -6047,33 +6099,33 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>-8.7916609710199989E-2</v>
+        <v>-7.718607828718764E-2</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>-0.32266759723232541</v>
+        <v>0.18832547032290964</v>
       </c>
       <c r="I40">
         <v>0</v>
       </c>
       <c r="J40">
-        <v>-0.30691885907496097</v>
+        <v>-0.14746361651005876</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>0.32682659234331435</v>
+        <v>-0.17206116142784475</v>
       </c>
       <c r="M40">
-        <v>7.0909005802329672E-2</v>
+        <v>0.10871582305167048</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -6082,39 +6134,39 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>-8.5429671993744891E-2</v>
+        <v>-8.7916609710199989E-2</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>-0.72370940298428799</v>
+        <v>-0.32266759723232541</v>
       </c>
       <c r="I41">
         <v>0</v>
       </c>
       <c r="J41">
-        <v>-0.54379963954552524</v>
+        <v>-0.30691885907496097</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>0.72370940298428799</v>
+        <v>0.32682659234331435</v>
       </c>
       <c r="M41">
-        <v>8.5429671993744891E-2</v>
+        <v>7.0909005802329672E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6129,33 +6181,33 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0.21332993320000762</v>
+        <v>-8.5429671993744891E-2</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>-2.0993820970085664</v>
+        <v>-0.72370940298428799</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>-0.25829277660138666</v>
+        <v>-0.54379963954552524</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>2.0978593483260881</v>
+        <v>0.72370940298428799</v>
       </c>
       <c r="M42">
-        <v>0.22781791913729374</v>
+        <v>8.5429671993744891E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6170,33 +6222,33 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0.36775805680102264</v>
+        <v>0.21332993320000762</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>-2.455894824377868</v>
+        <v>-2.0993820970085664</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
       <c r="J43">
-        <v>-0.14263048587484461</v>
+        <v>-0.25829277660138666</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>2.4673950266062379</v>
+        <v>2.0978593483260881</v>
       </c>
       <c r="M43">
-        <v>0.28040534842771281</v>
+        <v>0.22781791913729374</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6211,33 +6263,33 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0.55303757989544111</v>
+        <v>0.36775805680102264</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>-2.787104511410142</v>
+        <v>-2.455894824377868</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>5.6639586294437348E-2</v>
+        <v>-0.14263048587484461</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
-        <v>2.8215919178879201</v>
+        <v>2.4673950266062379</v>
       </c>
       <c r="M44">
-        <v>0.3352926650091575</v>
+        <v>0.28040534842771281</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6252,33 +6304,33 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0.68116461703126108</v>
+        <v>0.55303757989544111</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>-2.8980406823460374</v>
+        <v>-2.787104511410142</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>0.31872311046694207</v>
+        <v>5.6639586294437348E-2</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>2.9421852872904966</v>
+        <v>2.8215919178879201</v>
       </c>
       <c r="M45">
-        <v>0.45406031238082001</v>
+        <v>0.3352926650091575</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -6293,33 +6345,33 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>0.52641255960326594</v>
+        <v>0.68116461703126108</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>-2.670212924281651</v>
+        <v>-2.8980406823460374</v>
       </c>
       <c r="I46">
         <v>0</v>
       </c>
       <c r="J46">
-        <v>5.9318386681059529E-2</v>
+        <v>0.31872311046694207</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>2.6425063272203695</v>
+        <v>2.9421852872904966</v>
       </c>
       <c r="M46">
-        <v>0.65138894257512669</v>
+        <v>0.45406031238082001</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6334,33 +6386,33 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>-3.3598927806487079E-2</v>
+        <v>0.52641255960326594</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>-1.0353841375278308</v>
+        <v>-2.670212924281651</v>
       </c>
       <c r="I47">
         <v>0</v>
       </c>
       <c r="J47">
-        <v>-0.49392877418713621</v>
+        <v>5.9318386681059529E-2</v>
       </c>
       <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
-        <v>1.0322067475361931</v>
+        <v>2.6425063272203695</v>
       </c>
       <c r="M47">
-        <v>8.7740700559939391E-2</v>
+        <v>0.65138894257512669</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -6375,33 +6427,33 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>1.6491058929627832E-2</v>
+        <v>-1.6539195382390338E-2</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>-1.3852009656776634</v>
+        <v>-1.8891033887224336</v>
       </c>
       <c r="I48">
         <v>0</v>
       </c>
       <c r="J48">
-        <v>-0.41934117520233494</v>
+        <v>-0.36987756945978184</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
       <c r="L48">
-        <v>1.3793364748992825</v>
+        <v>1.5379764099976985</v>
       </c>
       <c r="M48">
-        <v>0.12839220907583238</v>
+        <v>1.0970933053104786</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>-10</v>
+        <v>3</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -6416,33 +6468,33 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>-9.8626430925695188E-2</v>
+        <v>-3.3598927806487079E-2</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>9.0518855786986888E-2</v>
+        <v>-1.0353841375278308</v>
       </c>
       <c r="I49">
         <v>0</v>
       </c>
       <c r="J49">
-        <v>-0.55841392539558155</v>
+        <v>-0.49392877418713621</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>-7.2017370972778313E-2</v>
+        <v>1.0322067475361931</v>
       </c>
       <c r="M49">
-        <v>0.11284650817945356</v>
+        <v>8.7740700559939391E-2</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -6457,33 +6509,33 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>-0.10181096777716636</v>
+        <v>1.6491058929627832E-2</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>-0.40003493281219354</v>
+        <v>-1.3852009656776634</v>
       </c>
       <c r="I50">
         <v>0</v>
       </c>
       <c r="J50">
-        <v>-0.62825495094738204</v>
+        <v>-0.41934117520233494</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
-        <v>0.40481507319445559</v>
+        <v>1.3793364748992825</v>
       </c>
       <c r="M50">
-        <v>8.0735228644916612E-2</v>
+        <v>0.12839220907583238</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -6492,39 +6544,39 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>-6.8496245088475988E-2</v>
+        <v>-9.8626430925695188E-2</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>-0.56496728530850515</v>
+        <v>9.0518855786986888E-2</v>
       </c>
       <c r="I51">
         <v>0</v>
       </c>
       <c r="J51">
-        <v>0.121901923520936</v>
+        <v>-0.55841392539558155</v>
       </c>
       <c r="K51">
         <v>0</v>
       </c>
       <c r="L51">
-        <v>0.56496728530850515</v>
+        <v>-7.2017370972778313E-2</v>
       </c>
       <c r="M51">
-        <v>6.8496245088475988E-2</v>
+        <v>0.11284650817945356</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>12</v>
+        <v>-3</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -6533,39 +6585,39 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>0.22271152705902242</v>
+        <v>-0.10181096777716636</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>-1.9788706129954865</v>
+        <v>-0.40003493281219354</v>
       </c>
       <c r="I52">
         <v>0</v>
       </c>
       <c r="J52">
-        <v>0.24523509821471629</v>
+        <v>-0.62825495094738204</v>
       </c>
       <c r="K52">
         <v>0</v>
       </c>
       <c r="L52">
-        <v>1.9819318724196169</v>
+        <v>0.40481507319445559</v>
       </c>
       <c r="M52">
-        <v>0.19358558920892258</v>
+        <v>8.0735228644916612E-2</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -6580,33 +6632,33 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0.37856085750210883</v>
+        <v>-6.8496245088475988E-2</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>-2.3520082753719005</v>
+        <v>-0.56496728530850515</v>
       </c>
       <c r="I53">
         <v>0</v>
       </c>
       <c r="J53">
-        <v>0.28937363651564396</v>
+        <v>0.121901923520936</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
-        <v>2.3698442964792168</v>
+        <v>0.56496728530850515</v>
       </c>
       <c r="M53">
-        <v>0.24308282682155927</v>
+        <v>6.8496245088475988E-2</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6621,33 +6673,33 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0.57310594071170506</v>
+        <v>0.22271152705902242</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>-2.7216349311976553</v>
+        <v>-1.9788706129954865</v>
       </c>
       <c r="I54">
         <v>0</v>
       </c>
       <c r="J54">
-        <v>0.32755054698950536</v>
+        <v>0.24523509821471629</v>
       </c>
       <c r="K54">
         <v>0</v>
       </c>
       <c r="L54">
-        <v>2.7655281115491999</v>
+        <v>1.9819318724196169</v>
       </c>
       <c r="M54">
-        <v>0.29597530678323508</v>
+        <v>0.19358558920892258</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -6662,33 +6714,33 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0.70886868953398696</v>
+        <v>0.37856085750210883</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>-2.8763578652502293</v>
+        <v>-2.3520082753719005</v>
       </c>
       <c r="I55">
         <v>0</v>
       </c>
       <c r="J55">
-        <v>0.33843077078853501</v>
+        <v>0.28937363651564396</v>
       </c>
       <c r="K55">
         <v>0</v>
       </c>
       <c r="L55">
-        <v>2.9324594575817322</v>
+        <v>2.3698442964792168</v>
       </c>
       <c r="M55">
-        <v>0.42025101740262394</v>
+        <v>0.24308282682155927</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -6703,33 +6755,33 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0.56918423918376349</v>
+        <v>0.57310594071170506</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>-2.6987792799381118</v>
+        <v>-2.7216349311976553</v>
       </c>
       <c r="I56">
         <v>0</v>
       </c>
       <c r="J56">
-        <v>0.22392012366737543</v>
+        <v>0.32755054698950536</v>
       </c>
       <c r="K56">
         <v>0</v>
       </c>
       <c r="L56">
-        <v>2.6864723306751181</v>
+        <v>2.7655281115491999</v>
       </c>
       <c r="M56">
-        <v>0.62469729987848532</v>
+        <v>0.29597530678323508</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -6744,33 +6796,33 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>-1.844713876167519E-2</v>
+        <v>0.70886868953398696</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>-0.88384405730146687</v>
+        <v>-2.8763578652502293</v>
       </c>
       <c r="I57">
         <v>0</v>
       </c>
       <c r="J57">
-        <v>0.14107790350215352</v>
+        <v>0.33843077078853501</v>
       </c>
       <c r="K57">
         <v>0</v>
       </c>
       <c r="L57">
-        <v>0.88166733109152029</v>
+        <v>2.9324594575817322</v>
       </c>
       <c r="M57">
-        <v>6.4678681507640265E-2</v>
+        <v>0.42025101740262394</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -6785,33 +6837,33 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>2.8352590222335456E-2</v>
+        <v>0.56918423918376349</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>-1.2563519895601134</v>
+        <v>-2.6987792799381118</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
       <c r="J58">
-        <v>0.18562367421745316</v>
+        <v>0.22392012366737543</v>
       </c>
       <c r="K58">
         <v>0</v>
       </c>
       <c r="L58">
-        <v>1.2524332145926234</v>
+        <v>2.6864723306751181</v>
       </c>
       <c r="M58">
-        <v>0.10312727102546061</v>
+        <v>0.62469729987848532</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>-10</v>
+        <v>35</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -6826,33 +6878,33 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>-6.0064392872935371E-2</v>
+        <v>-1.835141525929784E-2</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>0.28251967244743303</v>
+        <v>-1.7914918476078321</v>
       </c>
       <c r="I59">
         <v>0</v>
       </c>
       <c r="J59">
-        <v>0.25045575785478952</v>
+        <v>-0.34324515775510595</v>
       </c>
       <c r="K59">
         <v>0</v>
       </c>
       <c r="L59">
-        <v>-0.26779749143964576</v>
+        <v>1.4569782699285925</v>
       </c>
       <c r="M59">
-        <v>0.10821090605679277</v>
+        <v>1.0425901090281018</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -6867,33 +6919,33 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>-7.7799878933980257E-2</v>
+        <v>-1.844713876167519E-2</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>-0.22835660951135309</v>
+        <v>-0.88384405730146687</v>
       </c>
       <c r="I60">
         <v>0</v>
       </c>
       <c r="J60">
-        <v>8.3652201891138964E-2</v>
+        <v>0.14107790350215352</v>
       </c>
       <c r="K60">
         <v>0</v>
       </c>
       <c r="L60">
-        <v>0.23211538577404953</v>
+        <v>0.88166733109152029</v>
       </c>
       <c r="M60">
-        <v>6.5741995380629692E-2</v>
+        <v>6.4678681507640265E-2</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -6902,39 +6954,39 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>-7.7195931073887322E-2</v>
+        <v>2.8352590222335456E-2</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>-0.30548908261149982</v>
+        <v>-1.2563519895601134</v>
       </c>
       <c r="I61">
         <v>0</v>
       </c>
       <c r="J61">
-        <v>1.2170847420967017</v>
+        <v>0.18562367421745316</v>
       </c>
       <c r="K61">
         <v>0</v>
       </c>
       <c r="L61">
-        <v>0.30548908261149982</v>
+        <v>1.2524332145926234</v>
       </c>
       <c r="M61">
-        <v>7.7195931073887322E-2</v>
+        <v>0.10312727102546061</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>12</v>
+        <v>-10</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -6943,39 +6995,39 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>0.18073217616807821</v>
+        <v>-6.0064392872935371E-2</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>-1.7188149530669425</v>
+        <v>0.28251967244743303</v>
       </c>
       <c r="I62">
         <v>0</v>
       </c>
       <c r="J62">
-        <v>1.3494623786828075</v>
+        <v>0.25045575785478952</v>
       </c>
       <c r="K62">
         <v>0</v>
       </c>
       <c r="L62">
-        <v>1.7188310547800971</v>
+        <v>-0.26779749143964576</v>
       </c>
       <c r="M62">
-        <v>0.18057897860079045</v>
+        <v>0.10821090605679277</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>15</v>
+        <v>-3</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -6984,39 +7036,39 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0.3296738451692775</v>
+        <v>-7.7799878933980257E-2</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>-2.0922229843557751</v>
+        <v>-0.22835660951135309</v>
       </c>
       <c r="I63">
         <v>0</v>
       </c>
       <c r="J63">
-        <v>1.3871647891826986</v>
+        <v>8.3652201891138964E-2</v>
       </c>
       <c r="K63">
         <v>0</v>
       </c>
       <c r="L63">
-        <v>2.1062580847468211</v>
+        <v>0.23211538577404953</v>
       </c>
       <c r="M63">
-        <v>0.22306667365147909</v>
+        <v>6.5741995380629692E-2</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -7031,33 +7083,33 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0.51972032803105017</v>
+        <v>-7.7195931073887322E-2</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>-2.4682677185949227</v>
+        <v>-0.30548908261149982</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64">
-        <v>1.4034418238536202</v>
+        <v>1.2170847420967017</v>
       </c>
       <c r="K64">
         <v>0</v>
       </c>
       <c r="L64">
-        <v>2.5080645114143905</v>
+        <v>0.30548908261149982</v>
       </c>
       <c r="M64">
-        <v>0.26845326708792649</v>
+        <v>7.7195931073887322E-2</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -7072,33 +7124,33 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0.68599736513590925</v>
+        <v>0.18073217616807821</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>-2.7239339886543155</v>
+        <v>-1.7188149530669425</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65">
-        <v>1.1538807318073121</v>
+        <v>1.3494623786828075</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
-        <v>2.7825667512318466</v>
+        <v>1.7188310547800971</v>
       </c>
       <c r="M65">
-        <v>0.38435795095023834</v>
+        <v>0.18057897860079045</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -7113,33 +7165,33 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.54597524770037775</v>
+        <v>0.3296738451692775</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>-2.5273816121985733</v>
+        <v>-2.0922229843557751</v>
       </c>
       <c r="I66">
         <v>0</v>
       </c>
       <c r="J66">
-        <v>0.7076472884268511</v>
+        <v>1.3871647891826986</v>
       </c>
       <c r="K66">
         <v>0</v>
       </c>
       <c r="L66">
-        <v>2.5213247460853911</v>
+        <v>2.1062580847468211</v>
       </c>
       <c r="M66">
-        <v>0.57329600518265156</v>
+        <v>0.22306667365147909</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -7154,33 +7206,33 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>-3.5178793356106131E-2</v>
+        <v>0.51972032803105017</v>
       </c>
       <c r="G67">
         <v>0</v>
       </c>
       <c r="H67">
-        <v>-0.62958462063937748</v>
+        <v>-2.4682677185949227</v>
       </c>
       <c r="I67">
         <v>0</v>
       </c>
       <c r="J67">
-        <v>1.2167173554646495</v>
+        <v>1.4034418238536202</v>
       </c>
       <c r="K67">
         <v>0</v>
       </c>
       <c r="L67">
-        <v>0.62688068100797167</v>
+        <v>2.5080645114143905</v>
       </c>
       <c r="M67">
-        <v>6.8080495199448407E-2</v>
+        <v>0.26845326708792649</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -7195,33 +7247,33 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>4.3461943916355593E-3</v>
+        <v>0.68599736513590925</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>-0.98649921800662743</v>
+        <v>-2.7239339886543155</v>
       </c>
       <c r="I68">
         <v>0</v>
       </c>
       <c r="J68">
-        <v>1.2779142661211149</v>
+        <v>1.1538807318073121</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>0.98154937309209067</v>
+        <v>2.7825667512318466</v>
       </c>
       <c r="M68">
-        <v>9.8794861788966265E-2</v>
+        <v>0.38435795095023834</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>-10</v>
+        <v>25</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -7236,33 +7288,33 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>-4.7459353129715436E-2</v>
+        <v>0.54597524770037775</v>
       </c>
       <c r="G69">
         <v>0</v>
       </c>
       <c r="H69">
-        <v>0.53483256261998691</v>
+        <v>-2.5273816121985733</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69">
-        <v>1.3350547545921554</v>
+        <v>0.7076472884268511</v>
       </c>
       <c r="K69">
         <v>0</v>
       </c>
       <c r="L69">
-        <v>-0.518466024047324</v>
+        <v>2.5213247460853911</v>
       </c>
       <c r="M69">
-        <v>0.1396110387709831</v>
+        <v>0.57329600518265156</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>-3</v>
+        <v>35</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -7277,33 +7329,33 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>-7.9837764981612436E-2</v>
+        <v>-1.1039537451429347E-2</v>
       </c>
       <c r="G70">
         <v>0</v>
       </c>
       <c r="H70">
-        <v>3.3530079840469615E-2</v>
+        <v>-1.7913950011132203</v>
       </c>
       <c r="I70">
         <v>0</v>
       </c>
       <c r="J70">
-        <v>1.1838308031410509</v>
+        <v>2.7652072007542945E-2</v>
       </c>
       <c r="K70">
         <v>0</v>
       </c>
       <c r="L70">
-        <v>-2.9305742256759783E-2</v>
+        <v>1.4610928587406207</v>
       </c>
       <c r="M70">
-        <v>8.1483178890785865E-2</v>
+        <v>1.0365450205069424</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -7312,39 +7364,39 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71">
-        <v>-9.4084386734767128E-2</v>
+        <v>-3.5178793356106131E-2</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>-0.29196217368460958</v>
+        <v>-0.62958462063937748</v>
       </c>
       <c r="I71">
         <v>0</v>
       </c>
       <c r="J71">
-        <v>1.2767926677740682</v>
+        <v>1.2167173554646495</v>
       </c>
       <c r="K71">
         <v>0</v>
       </c>
       <c r="L71">
-        <v>0.29196217368460958</v>
+        <v>0.62688068100797167</v>
       </c>
       <c r="M71">
-        <v>9.4084386734767128E-2</v>
+        <v>6.8080495199448407E-2</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -7353,39 +7405,39 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0.16224482491377495</v>
+        <v>4.3461943916355593E-3</v>
       </c>
       <c r="G72">
         <v>0</v>
       </c>
       <c r="H72">
-        <v>-1.6758814822736328</v>
+        <v>-0.98649921800662743</v>
       </c>
       <c r="I72">
         <v>0</v>
       </c>
       <c r="J72">
-        <v>1.52793577983716</v>
+        <v>1.2779142661211149</v>
       </c>
       <c r="K72">
         <v>0</v>
       </c>
       <c r="L72">
-        <v>1.6729920468744219</v>
+        <v>0.98154937309209067</v>
       </c>
       <c r="M72">
-        <v>0.18973596636879836</v>
+        <v>9.8794861788966265E-2</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>15</v>
+        <v>-10</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -7394,39 +7446,39 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0.30967124915718819</v>
+        <v>-4.7459353129715436E-2</v>
       </c>
       <c r="G73">
         <v>0</v>
       </c>
       <c r="H73">
-        <v>-2.0444556517804156</v>
+        <v>0.53483256261998691</v>
       </c>
       <c r="I73">
         <v>0</v>
       </c>
       <c r="J73">
-        <v>1.5881823258710199</v>
+        <v>1.3350547545921554</v>
       </c>
       <c r="K73">
         <v>0</v>
       </c>
       <c r="L73">
-        <v>2.0549413317599217</v>
+        <v>-0.518466024047324</v>
       </c>
       <c r="M73">
-        <v>0.23002460232813388</v>
+        <v>0.1396110387709831</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -7435,39 +7487,39 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74">
-        <v>0.49826906045543068</v>
+        <v>-7.9837764981612436E-2</v>
       </c>
       <c r="G74">
         <v>0</v>
       </c>
       <c r="H74">
-        <v>-2.4167766263258925</v>
+        <v>3.3530079840469615E-2</v>
       </c>
       <c r="I74">
         <v>0</v>
       </c>
       <c r="J74">
-        <v>1.6217210464330269</v>
+        <v>1.1838308031410509</v>
       </c>
       <c r="K74">
         <v>0</v>
       </c>
       <c r="L74">
-        <v>2.4524647663490233</v>
+        <v>-2.9305742256759783E-2</v>
       </c>
       <c r="M74">
-        <v>0.27294301232845158</v>
+        <v>8.1483178890785865E-2</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -7482,33 +7534,33 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>0.66792475237610327</v>
+        <v>-9.4084386734767128E-2</v>
       </c>
       <c r="G75">
         <v>0</v>
       </c>
       <c r="H75">
-        <v>-2.6750815273685014</v>
+        <v>-0.29196217368460958</v>
       </c>
       <c r="I75">
         <v>0</v>
       </c>
       <c r="J75">
-        <v>1.3783582285479135</v>
+        <v>1.2767926677740682</v>
       </c>
       <c r="K75">
         <v>0</v>
       </c>
       <c r="L75">
-        <v>2.7305014179717149</v>
+        <v>0.29196217368460958</v>
       </c>
       <c r="M75">
-        <v>0.38281413160870664</v>
+        <v>9.4084386734767128E-2</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -7523,33 +7575,33 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <v>0.54569339438146058</v>
+        <v>0.16224482491377495</v>
       </c>
       <c r="G76">
         <v>0</v>
       </c>
       <c r="H76">
-        <v>-2.523399903135628</v>
+        <v>-1.6758814822736328</v>
       </c>
       <c r="I76">
         <v>0</v>
       </c>
       <c r="J76">
-        <v>0.89559177374302767</v>
+        <v>1.52793577983716</v>
       </c>
       <c r="K76">
         <v>0</v>
       </c>
       <c r="L76">
-        <v>2.5175969757962227</v>
+        <v>1.6729920468744219</v>
       </c>
       <c r="M76">
-        <v>0.57186870807744916</v>
+        <v>0.18973596636879836</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -7564,33 +7616,33 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <v>-5.128071050976004E-2</v>
+        <v>0.30967124915718819</v>
       </c>
       <c r="G77">
         <v>0</v>
       </c>
       <c r="H77">
-        <v>-0.60674342555727956</v>
+        <v>-2.0444556517804156</v>
       </c>
       <c r="I77">
         <v>0</v>
       </c>
       <c r="J77">
-        <v>1.3126931746017902</v>
+        <v>1.5881823258710199</v>
       </c>
       <c r="K77">
         <v>0</v>
       </c>
       <c r="L77">
-        <v>0.6032280797583166</v>
+        <v>2.0549413317599217</v>
       </c>
       <c r="M77">
-        <v>8.2964929448905295E-2</v>
+        <v>0.23002460232813388</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -7605,33 +7657,33 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>-1.1924779959131403E-2</v>
+        <v>0.49826906045543068</v>
       </c>
       <c r="G78">
         <v>0</v>
       </c>
       <c r="H78">
-        <v>-0.95197972830722333</v>
+        <v>-2.4167766263258925</v>
       </c>
       <c r="I78">
         <v>0</v>
       </c>
       <c r="J78">
-        <v>1.3932105676535247</v>
+        <v>1.6217210464330269</v>
       </c>
       <c r="K78">
         <v>0</v>
       </c>
       <c r="L78">
-        <v>0.9455182048243409</v>
+        <v>2.4524647663490233</v>
       </c>
       <c r="M78">
-        <v>0.11136843282871728</v>
+        <v>0.27294301232845158</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>-10</v>
+        <v>22</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -7646,33 +7698,33 @@
         <v>0</v>
       </c>
       <c r="F79">
-        <v>-7.273515734660975E-2</v>
+        <v>0.66792475237610327</v>
       </c>
       <c r="G79">
         <v>0</v>
       </c>
       <c r="H79">
-        <v>0.50501444943067242</v>
+        <v>-2.6750815273685014</v>
       </c>
       <c r="I79">
         <v>0</v>
       </c>
       <c r="J79">
-        <v>1.2261210668769142</v>
+        <v>1.3783582285479135</v>
       </c>
       <c r="K79">
         <v>0</v>
       </c>
       <c r="L79">
-        <v>-0.48471181765696153</v>
+        <v>2.7305014179717149</v>
       </c>
       <c r="M79">
-        <v>0.15932498571060855</v>
+        <v>0.38281413160870664</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>-3</v>
+        <v>25</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -7687,33 +7739,33 @@
         <v>0</v>
       </c>
       <c r="F80">
-        <v>-9.8108715481738343E-2</v>
+        <v>0.54569339438146058</v>
       </c>
       <c r="G80">
         <v>0</v>
       </c>
       <c r="H80">
-        <v>3.6631169446297338E-2</v>
+        <v>-2.523399903135628</v>
       </c>
       <c r="I80">
         <v>0</v>
       </c>
       <c r="J80">
-        <v>1.2019920439586451</v>
+        <v>0.89559177374302767</v>
       </c>
       <c r="K80">
         <v>0</v>
       </c>
       <c r="L80">
-        <v>-3.1446354261168187E-2</v>
+        <v>2.5175969757962227</v>
       </c>
       <c r="M80">
-        <v>9.9891388178166493E-2</v>
+        <v>0.57186870807744916</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -7722,39 +7774,39 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>-6.9506435658708704E-2</v>
+        <v>-2.2582412218437254E-2</v>
       </c>
       <c r="G81">
         <v>0</v>
       </c>
       <c r="H81">
-        <v>-0.38543276188102249</v>
+        <v>-1.707294422424021</v>
       </c>
       <c r="I81">
         <v>0</v>
       </c>
       <c r="J81">
-        <v>0.8757747552691485</v>
+        <v>5.8061316401631174E-2</v>
       </c>
       <c r="K81">
         <v>0</v>
       </c>
       <c r="L81">
-        <v>0.38543276188102249</v>
+        <v>1.3855809768073688</v>
       </c>
       <c r="M81">
-        <v>6.9506435658708704E-2</v>
+        <v>0.99776227974969711</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -7763,39 +7815,39 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82">
-        <v>0.19825346612774047</v>
+        <v>-5.128071050976004E-2</v>
       </c>
       <c r="G82">
         <v>0</v>
       </c>
       <c r="H82">
-        <v>-1.8003892255870124</v>
+        <v>-0.60674342555727956</v>
       </c>
       <c r="I82">
         <v>0</v>
       </c>
       <c r="J82">
-        <v>1.0042032638441956</v>
+        <v>1.3126931746017902</v>
       </c>
       <c r="K82">
         <v>0</v>
       </c>
       <c r="L82">
-        <v>1.8022656147480305</v>
+        <v>0.6032280797583166</v>
       </c>
       <c r="M82">
-        <v>0.18040081579186187</v>
+        <v>8.2964929448905295E-2</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -7804,39 +7856,39 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83">
-        <v>0.35013168866706651</v>
+        <v>-1.1924779959131403E-2</v>
       </c>
       <c r="G83">
         <v>0</v>
       </c>
       <c r="H83">
-        <v>-2.1757430242328892</v>
+        <v>-0.95197972830722333</v>
       </c>
       <c r="I83">
         <v>0</v>
       </c>
       <c r="J83">
-        <v>1.0383394874624312</v>
+        <v>1.3932105676535247</v>
       </c>
       <c r="K83">
         <v>0</v>
       </c>
       <c r="L83">
-        <v>2.1922271277957734</v>
+        <v>0.9455182048243409</v>
       </c>
       <c r="M83">
-        <v>0.22492249123470398</v>
+        <v>0.11136843282871728</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>18</v>
+        <v>-10</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -7845,39 +7897,39 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
-        <v>0.54186440388334123</v>
+        <v>-7.273515734660975E-2</v>
       </c>
       <c r="G84">
         <v>0</v>
       </c>
       <c r="H84">
-        <v>-2.550474490105854</v>
+        <v>0.50501444943067242</v>
       </c>
       <c r="I84">
         <v>0</v>
       </c>
       <c r="J84">
-        <v>1.0574676302980566</v>
+        <v>1.2261210668769142</v>
       </c>
       <c r="K84">
         <v>0</v>
       </c>
       <c r="L84">
-        <v>2.5930906929065345</v>
+        <v>-0.48471181765696153</v>
       </c>
       <c r="M84">
-        <v>0.27279628890084689</v>
+        <v>0.15932498571060855</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>22</v>
+        <v>-3</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -7886,39 +7938,39 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0.69502513502635788</v>
+        <v>-9.8108715481738343E-2</v>
       </c>
       <c r="G85">
         <v>0</v>
       </c>
       <c r="H85">
-        <v>-2.7704264894431851</v>
+        <v>3.6631169446297338E-2</v>
       </c>
       <c r="I85">
         <v>0</v>
       </c>
       <c r="J85">
-        <v>0.87795100675087234</v>
+        <v>1.2019920439586451</v>
       </c>
       <c r="K85">
         <v>0</v>
       </c>
       <c r="L85">
-        <v>2.8290557094465236</v>
+        <v>-3.1446354261168187E-2</v>
       </c>
       <c r="M85">
-        <v>0.39340394580497529</v>
+        <v>9.9891388178166493E-2</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -7933,33 +7985,33 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0.54353953160692858</v>
+        <v>-6.9506435658708704E-2</v>
       </c>
       <c r="G86">
         <v>0</v>
       </c>
       <c r="H86">
-        <v>-2.5745798477787449</v>
+        <v>-0.38543276188102249</v>
       </c>
       <c r="I86">
         <v>0</v>
       </c>
       <c r="J86">
-        <v>0.54974438996758113</v>
+        <v>0.8757747552691485</v>
       </c>
       <c r="K86">
         <v>0</v>
       </c>
       <c r="L86">
-        <v>2.5630714964245831</v>
+        <v>0.38543276188102249</v>
       </c>
       <c r="M86">
-        <v>0.59545034992327506</v>
+        <v>6.9506435658708704E-2</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -7974,33 +8026,33 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>-2.5652572187046505E-2</v>
+        <v>0.19825346612774047</v>
       </c>
       <c r="G87">
         <v>0</v>
       </c>
       <c r="H87">
-        <v>-0.70789263545777181</v>
+        <v>-1.8003892255870124</v>
       </c>
       <c r="I87">
         <v>0</v>
       </c>
       <c r="J87">
-        <v>0.88175100866170597</v>
+        <v>1.0042032638441956</v>
       </c>
       <c r="K87">
         <v>0</v>
       </c>
       <c r="L87">
-        <v>0.7055799413078836</v>
+        <v>1.8022656147480305</v>
       </c>
       <c r="M87">
-        <v>6.2665654222428507E-2</v>
+        <v>0.18040081579186187</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -8015,33 +8067,33 @@
         <v>0</v>
       </c>
       <c r="F88">
-        <v>1.6022318341714921E-2</v>
+        <v>0.35013168866706651</v>
       </c>
       <c r="G88">
         <v>0</v>
       </c>
       <c r="H88">
-        <v>-1.0616865599799663</v>
+        <v>-2.1757430242328892</v>
       </c>
       <c r="I88">
         <v>0</v>
       </c>
       <c r="J88">
-        <v>0.93396082483092047</v>
+        <v>1.0383394874624312</v>
       </c>
       <c r="K88">
         <v>0</v>
       </c>
       <c r="L88">
-        <v>1.0575453182325425</v>
+        <v>2.1922271277957734</v>
       </c>
       <c r="M88">
-        <v>9.5041918181231075E-2</v>
+        <v>0.22492249123470398</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>-10</v>
+        <v>18</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -8056,33 +8108,33 @@
         <v>0</v>
       </c>
       <c r="F89">
-        <v>-4.6563791707584221E-2</v>
+        <v>0.54186440388334123</v>
       </c>
       <c r="G89">
         <v>0</v>
       </c>
       <c r="H89">
-        <v>0.46332119055672866</v>
+        <v>-2.550474490105854</v>
       </c>
       <c r="I89">
         <v>0</v>
       </c>
       <c r="J89">
-        <v>1.0152388816190119</v>
+        <v>1.0574676302980566</v>
       </c>
       <c r="K89">
         <v>0</v>
       </c>
       <c r="L89">
-        <v>-0.44819658301982845</v>
+        <v>2.5930906929065345</v>
       </c>
       <c r="M89">
-        <v>0.12631126349792302</v>
+        <v>0.27279628890084689</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>-3</v>
+        <v>22</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -8097,279 +8149,279 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>-7.4515806858318878E-2</v>
+        <v>0.69502513502635788</v>
       </c>
       <c r="G90">
         <v>0</v>
       </c>
       <c r="H90">
-        <v>-4.5358521817180072E-2</v>
+        <v>-2.7704264894431851</v>
       </c>
       <c r="I90">
         <v>0</v>
       </c>
       <c r="J90">
-        <v>0.84653828497766881</v>
+        <v>0.87795100675087234</v>
       </c>
       <c r="K90">
         <v>0</v>
       </c>
       <c r="L90">
-        <v>4.9196215546590351E-2</v>
+        <v>2.8290557094465236</v>
       </c>
       <c r="M90">
-        <v>7.203980392171612E-2</v>
+        <v>0.39340394580497529</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B91">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>-4.7505716244460337E-2</v>
+        <v>0.54353953160692858</v>
       </c>
       <c r="G91">
-        <v>-9.1927912441848697E-2</v>
+        <v>0</v>
       </c>
       <c r="H91">
-        <v>-0.3972073187545293</v>
+        <v>-2.5745798477787449</v>
       </c>
       <c r="I91">
-        <v>-2.7772150835726466E-3</v>
+        <v>0</v>
       </c>
       <c r="J91">
-        <v>0.60339027191894345</v>
+        <v>0.54974438996758113</v>
       </c>
       <c r="K91">
-        <v>8.3511717676247581E-3</v>
+        <v>0</v>
       </c>
       <c r="L91">
-        <v>0.3972073187545293</v>
+        <v>2.5630714964245831</v>
       </c>
       <c r="M91">
-        <v>4.7505716244460337E-2</v>
+        <v>0.59545034992327506</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B92">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <v>0.21918338527098491</v>
+        <v>-1.2469282647748162E-2</v>
       </c>
       <c r="G92">
-        <v>-0.10936143335693478</v>
+        <v>0</v>
       </c>
       <c r="H92">
-        <v>-1.8066099806573888</v>
+        <v>-1.7775514666662569</v>
       </c>
       <c r="I92">
-        <v>3.4781461798756652E-3</v>
+        <v>0</v>
       </c>
       <c r="J92">
-        <v>0.65452518973355323</v>
+        <v>-0.142097312449145</v>
       </c>
       <c r="K92">
-        <v>1.4571289994414448E-2</v>
+        <v>0</v>
       </c>
       <c r="L92">
-        <v>1.8127020062726227</v>
+        <v>1.4489328310436105</v>
       </c>
       <c r="M92">
-        <v>0.16122163330318987</v>
+        <v>1.0297758740527272</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B93">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E93">
         <v>0</v>
       </c>
       <c r="F93">
-        <v>0.35502696510795262</v>
+        <v>-2.5652572187046505E-2</v>
       </c>
       <c r="G93">
-        <v>-5.632605405318529E-2</v>
+        <v>0</v>
       </c>
       <c r="H93">
-        <v>-2.1778292202838712</v>
+        <v>-0.70789263545777181</v>
       </c>
       <c r="I93">
-        <v>2.3263079710197521E-3</v>
+        <v>0</v>
       </c>
       <c r="J93">
-        <v>0.66060889480146268</v>
+        <v>0.88175100866170597</v>
       </c>
       <c r="K93">
-        <v>7.8148588022492471E-3</v>
+        <v>0</v>
       </c>
       <c r="L93">
-        <v>2.1955092292140619</v>
+        <v>0.7055799413078836</v>
       </c>
       <c r="M93">
-        <v>0.22073396456343947</v>
+        <v>6.2665654222428507E-2</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B94">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C94">
         <v>0</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94">
-        <v>0.55163035281987938</v>
+        <v>1.6022318341714921E-2</v>
       </c>
       <c r="G94">
-        <v>-5.696113208327748E-2</v>
+        <v>0</v>
       </c>
       <c r="H94">
-        <v>-2.5984390803467101</v>
+        <v>-1.0616865599799663</v>
       </c>
       <c r="I94">
-        <v>4.3182000198387091E-3</v>
+        <v>0</v>
       </c>
       <c r="J94">
-        <v>0.71727025064819516</v>
+        <v>0.93396082483092047</v>
       </c>
       <c r="K94">
-        <v>9.0375173385818137E-3</v>
+        <v>0</v>
       </c>
       <c r="L94">
-        <v>2.6417255731941154</v>
+        <v>1.0575453182325425</v>
       </c>
       <c r="M94">
-        <v>0.27833019303960183</v>
+        <v>9.5041918181231075E-2</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>3</v>
+        <v>-10</v>
       </c>
       <c r="B95">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95">
-        <v>-3.3400760249008552E-3</v>
+        <v>-4.6563791707584221E-2</v>
       </c>
       <c r="G95">
-        <v>-9.4667950871191994E-2</v>
+        <v>0</v>
       </c>
       <c r="H95">
-        <v>-0.72137281145379484</v>
+        <v>0.46332119055672866</v>
       </c>
       <c r="I95">
-        <v>-2.7330319478969314E-3</v>
+        <v>0</v>
       </c>
       <c r="J95">
-        <v>0.58733921900315789</v>
+        <v>1.0152388816190119</v>
       </c>
       <c r="K95">
-        <v>1.1036506388339591E-2</v>
+        <v>0</v>
       </c>
       <c r="L95">
-        <v>0.72020938901401477</v>
+        <v>-0.44819658301982845</v>
       </c>
       <c r="M95">
-        <v>4.1089234461886816E-2</v>
+        <v>0.12631126349792302</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96">
-        <v>4.1247313377936731E-2</v>
+        <v>-7.4515806858318878E-2</v>
       </c>
       <c r="G96">
-        <v>-0.1013204080783493</v>
+        <v>0</v>
       </c>
       <c r="H96">
-        <v>-1.0708453123226094</v>
+        <v>-4.5358521817180072E-2</v>
       </c>
       <c r="I96">
-        <v>-1.9956999129138462E-3</v>
+        <v>0</v>
       </c>
       <c r="J96">
-        <v>0.60730047628207351</v>
+        <v>0.84653828497766881</v>
       </c>
       <c r="K96">
-        <v>1.2228822106443904E-2</v>
+        <v>0</v>
       </c>
       <c r="L96">
-        <v>1.0692906279386272</v>
+        <v>4.9196215546590351E-2</v>
       </c>
       <c r="M96">
-        <v>7.0912458614977983E-2</v>
+        <v>7.203980392171612E-2</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="B97">
         <v>10</v>
@@ -8384,33 +8436,33 @@
         <v>0</v>
       </c>
       <c r="F97">
-        <v>-4.6016027279502686E-2</v>
+        <v>-4.7505716244460337E-2</v>
       </c>
       <c r="G97">
-        <v>-7.784002123974218E-2</v>
+        <v>-9.1927912441848697E-2</v>
       </c>
       <c r="H97">
-        <v>0.39817095225636107</v>
+        <v>-0.3972073187545293</v>
       </c>
       <c r="I97">
-        <v>1.6575631411882306E-2</v>
+        <v>-2.7772150835726466E-3</v>
       </c>
       <c r="J97">
-        <v>0.7114984781554804</v>
+        <v>0.60339027191894345</v>
       </c>
       <c r="K97">
-        <v>6.0144605612426332E-3</v>
+        <v>8.3511717676247581E-3</v>
       </c>
       <c r="L97">
-        <v>-0.38413124152576072</v>
+        <v>0.3972073187545293</v>
       </c>
       <c r="M97">
-        <v>0.11445860068689892</v>
+        <v>6.2747112142194694E-2</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>-3</v>
+        <v>12</v>
       </c>
       <c r="B98">
         <v>10</v>
@@ -8425,36 +8477,36 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <v>-5.680321631205857E-2</v>
+        <v>0.21918338527098491</v>
       </c>
       <c r="G98">
-        <v>-8.481552613842655E-2</v>
+        <v>-0.10936143335693478</v>
       </c>
       <c r="H98">
-        <v>-6.4259441263303296E-2</v>
+        <v>-1.8066099806573888</v>
       </c>
       <c r="I98">
-        <v>-3.0187146553080106E-3</v>
+        <v>3.4781461798756652E-3</v>
       </c>
       <c r="J98">
-        <v>0.60023980708646352</v>
+        <v>0.65452518973355323</v>
       </c>
       <c r="K98">
-        <v>6.5520842415802702E-3</v>
+        <v>1.4571289994414448E-2</v>
       </c>
       <c r="L98">
-        <v>6.71442265757278E-2</v>
+        <v>1.8127020062726227</v>
       </c>
       <c r="M98">
-        <v>5.3362290172122205E-2</v>
+        <v>0.1777627280397478</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B99">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -8466,36 +8518,36 @@
         <v>0</v>
       </c>
       <c r="F99">
-        <v>-2.3364533049572544E-2</v>
+        <v>0.35502696510795262</v>
       </c>
       <c r="G99">
-        <v>-0.19641942417667502</v>
+        <v>-5.632605405318529E-2</v>
       </c>
       <c r="H99">
-        <v>-0.30084637733205799</v>
+        <v>-2.1778292202838712</v>
       </c>
       <c r="I99">
-        <v>-2.4212806579202743E-3</v>
+        <v>2.3263079710197521E-3</v>
       </c>
       <c r="J99">
-        <v>0.60271620419005245</v>
+        <v>0.66060889480146268</v>
       </c>
       <c r="K99">
-        <v>1.5651856650643513E-2</v>
+        <v>7.8148588022492471E-3</v>
       </c>
       <c r="L99">
-        <v>0.30084637733205799</v>
+        <v>2.1955092292140619</v>
       </c>
       <c r="M99">
-        <v>2.3364533049572544E-2</v>
+        <v>0.2271614362967018</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B100">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -8507,36 +8559,36 @@
         <v>0</v>
       </c>
       <c r="F100">
-        <v>0.20131901999215693</v>
+        <v>0.55163035281987938</v>
       </c>
       <c r="G100">
-        <v>-0.2140853276862541</v>
+        <v>-5.696113208327748E-2</v>
       </c>
       <c r="H100">
-        <v>-1.5978304340908418</v>
+        <v>-2.5984390803467101</v>
       </c>
       <c r="I100">
-        <v>2.5996595099345016E-3</v>
+        <v>4.3182000198387091E-3</v>
       </c>
       <c r="J100">
-        <v>0.73759258791242588</v>
+        <v>0.71727025064819516</v>
       </c>
       <c r="K100">
-        <v>1.8409391591195663E-2</v>
+        <v>9.0375173385818137E-3</v>
       </c>
       <c r="L100">
-        <v>1.6047705833257557</v>
+        <v>2.6417255731941154</v>
       </c>
       <c r="M100">
-        <v>0.13528791080449187</v>
+        <v>0.28399292878689086</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B101">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -8548,36 +8600,36 @@
         <v>0</v>
       </c>
       <c r="F101">
-        <v>0.32793787472970998</v>
+        <v>-3.3400760249008552E-3</v>
       </c>
       <c r="G101">
-        <v>-0.21217478562063638</v>
+        <v>-9.4667950871191994E-2</v>
       </c>
       <c r="H101">
-        <v>-1.9352948053062868</v>
+        <v>-0.72137281145379484</v>
       </c>
       <c r="I101">
-        <v>5.3145576626830839E-3</v>
+        <v>-2.7330319478969314E-3</v>
       </c>
       <c r="J101">
-        <v>0.77104684638811694</v>
+        <v>0.58733921900315789</v>
       </c>
       <c r="K101">
-        <v>1.8521905389749266E-2</v>
+        <v>1.1036506388339591E-2</v>
       </c>
       <c r="L101">
-        <v>1.9542278015189098</v>
+        <v>0.72020938901401477</v>
       </c>
       <c r="M101">
-        <v>0.18412749088146577</v>
+        <v>5.6903913815647508E-2</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B102">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -8589,36 +8641,36 @@
         <v>0</v>
       </c>
       <c r="F102">
-        <v>0.28571565201086574</v>
+        <v>4.1247313377936731E-2</v>
       </c>
       <c r="G102">
-        <v>-0.23380216146242108</v>
+        <v>-0.1013204080783493</v>
       </c>
       <c r="H102">
-        <v>-1.9537223938165951</v>
+        <v>-1.0708453123226094</v>
       </c>
       <c r="I102">
-        <v>2.1534872412220261E-2</v>
+        <v>-1.9956999129138462E-3</v>
       </c>
       <c r="J102">
-        <v>0.52412751484017817</v>
+        <v>0.60730047628207351</v>
       </c>
       <c r="K102">
-        <v>1.7067399436774752E-2</v>
+        <v>1.2228822106443904E-2</v>
       </c>
       <c r="L102">
-        <v>1.946391405701315</v>
+        <v>1.0692906279386272</v>
       </c>
       <c r="M102">
-        <v>0.33200168932777918</v>
+        <v>8.7429243252462749E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>3</v>
+        <v>-10</v>
       </c>
       <c r="B103">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -8630,36 +8682,36 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <v>1.192535532286151E-2</v>
+        <v>-4.6016027279502686E-2</v>
       </c>
       <c r="G103">
-        <v>-0.1977505202515592</v>
+        <v>-7.784002123974218E-2</v>
       </c>
       <c r="H103">
-        <v>-0.59298182651323161</v>
+        <v>0.39817095225636107</v>
       </c>
       <c r="I103">
-        <v>-3.9364841775132121E-3</v>
+        <v>1.6575631411882306E-2</v>
       </c>
       <c r="J103">
-        <v>0.6254041524460493</v>
+        <v>0.7114984781554804</v>
       </c>
       <c r="K103">
-        <v>1.7362751369570727E-2</v>
+        <v>6.0144605612426332E-3</v>
       </c>
       <c r="L103">
-        <v>0.59279329040318485</v>
+        <v>-0.38413124152576072</v>
       </c>
       <c r="M103">
-        <v>1.9125258887405225E-2</v>
+        <v>0.12623649519322286</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="B104">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -8671,33 +8723,33 @@
         <v>0</v>
       </c>
       <c r="F104">
-        <v>5.1070746880325146E-2</v>
+        <v>-5.680321631205857E-2</v>
       </c>
       <c r="G104">
-        <v>-0.20563943801272749</v>
+        <v>-8.481552613842655E-2</v>
       </c>
       <c r="H104">
-        <v>-0.9084862820756171</v>
+        <v>-6.4259441263303296E-2</v>
       </c>
       <c r="I104">
-        <v>-4.4806121859410578E-3</v>
+        <v>-3.0187146553080106E-3</v>
       </c>
       <c r="J104">
-        <v>0.67356942233129458</v>
+        <v>0.60023980708646352</v>
       </c>
       <c r="K104">
-        <v>1.8293177597732562E-2</v>
+        <v>6.5520842415802702E-3</v>
       </c>
       <c r="L104">
-        <v>0.90884784585525014</v>
+        <v>6.71442265757278E-2</v>
       </c>
       <c r="M104">
-        <v>4.4171698979813906E-2</v>
+        <v>6.7279658631792763E-2</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="B105">
         <v>20</v>
@@ -8712,33 +8764,33 @@
         <v>0</v>
       </c>
       <c r="F105">
-        <v>-5.0027938577338123E-2</v>
+        <v>-2.3364533049572544E-2</v>
       </c>
       <c r="G105">
-        <v>-0.16787578987678636</v>
+        <v>-0.19641942417667502</v>
       </c>
       <c r="H105">
-        <v>0.38554473622205221</v>
+        <v>-0.30084637733205799</v>
       </c>
       <c r="I105">
-        <v>2.575041145684303E-2</v>
+        <v>-2.4212806579202743E-3</v>
       </c>
       <c r="J105">
-        <v>0.58381833783153814</v>
+        <v>0.60271620419005245</v>
       </c>
       <c r="K105">
-        <v>1.3972419247413822E-2</v>
+        <v>1.5651856650643513E-2</v>
       </c>
       <c r="L105">
-        <v>-0.37100018499813575</v>
+        <v>0.30084637733205799</v>
       </c>
       <c r="M105">
-        <v>0.1162170426322178</v>
+        <v>8.9134878903643494E-2</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>-3</v>
+        <v>12</v>
       </c>
       <c r="B106">
         <v>20</v>
@@ -8753,36 +8805,36 @@
         <v>0</v>
       </c>
       <c r="F106">
-        <v>-4.2445598853748108E-2</v>
+        <v>0.20131901999215693</v>
       </c>
       <c r="G106">
-        <v>-0.17410989314356345</v>
+        <v>-0.2140853276862541</v>
       </c>
       <c r="H106">
-        <v>-6.5695455195958236E-2</v>
+        <v>-1.5978304340908418</v>
       </c>
       <c r="I106">
-        <v>4.3400079189802607E-3</v>
+        <v>2.5996595099345016E-3</v>
       </c>
       <c r="J106">
-        <v>0.60973770489389667</v>
+        <v>0.73759258791242588</v>
       </c>
       <c r="K106">
-        <v>1.5545018857230822E-2</v>
+        <v>1.8409391591195663E-2</v>
       </c>
       <c r="L106">
-        <v>6.7826852862145043E-2</v>
+        <v>1.6047705833257557</v>
       </c>
       <c r="M106">
-        <v>3.8949194167201794E-2</v>
+        <v>0.20035054592369858</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B107">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -8794,36 +8846,36 @@
         <v>0</v>
       </c>
       <c r="F107">
-        <v>1.4562382430074136E-2</v>
+        <v>0.32793787472970998</v>
       </c>
       <c r="G107">
-        <v>-0.34117274201218539</v>
+        <v>-0.21217478562063638</v>
       </c>
       <c r="H107">
-        <v>-0.26292881549732261</v>
+        <v>-1.9352948053062868</v>
       </c>
       <c r="I107">
-        <v>1.2974792629972969E-2</v>
+        <v>5.3145576626830839E-3</v>
       </c>
       <c r="J107">
-        <v>0.13071235106523052</v>
+        <v>0.77104684638811694</v>
       </c>
       <c r="K107">
-        <v>3.6569708865806155E-2</v>
+        <v>1.8521905389749266E-2</v>
       </c>
       <c r="L107">
-        <v>0.26292881549732261</v>
+        <v>1.9542278015189098</v>
       </c>
       <c r="M107">
-        <v>-1.4562382430074136E-2</v>
+        <v>0.24559129505320115</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B108">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -8835,36 +8887,36 @@
         <v>0</v>
       </c>
       <c r="F108">
-        <v>6.6744928603131207E-2</v>
+        <v>0.28571565201086574</v>
       </c>
       <c r="G108">
-        <v>-0.35855411499705614</v>
+        <v>-0.23380216146242108</v>
       </c>
       <c r="H108">
-        <v>-0.88189487677332457</v>
+        <v>-1.9537223938165951</v>
       </c>
       <c r="I108">
-        <v>1.1494985182503414E-3</v>
+        <v>2.1534872412220261E-2</v>
       </c>
       <c r="J108">
-        <v>0.50424292019560746</v>
+        <v>0.52412751484017817</v>
       </c>
       <c r="K108">
-        <v>1.5293832187298809E-2</v>
+        <v>1.7067399436774752E-2</v>
       </c>
       <c r="L108">
-        <v>0.8765004087746503</v>
+        <v>1.946391405701315</v>
       </c>
       <c r="M108">
-        <v>0.11806986317915942</v>
+        <v>0.39194458632299817</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B109">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -8876,36 +8928,36 @@
         <v>0</v>
       </c>
       <c r="F109">
-        <v>7.4681583023926496E-2</v>
+        <v>1.192535532286151E-2</v>
       </c>
       <c r="G109">
-        <v>-0.42493755420952761</v>
+        <v>-0.1977505202515592</v>
       </c>
       <c r="H109">
-        <v>-0.89827728298763987</v>
+        <v>-0.59298182651323161</v>
       </c>
       <c r="I109">
-        <v>6.6431830838151089E-3</v>
+        <v>-3.9364841775132121E-3</v>
       </c>
       <c r="J109">
-        <v>0.35353635633790342</v>
+        <v>0.6254041524460493</v>
       </c>
       <c r="K109">
-        <v>1.2082185600684459E-2</v>
+        <v>1.7362751369570727E-2</v>
       </c>
       <c r="L109">
-        <v>0.88699824281153261</v>
+        <v>0.59279329040318485</v>
       </c>
       <c r="M109">
-        <v>0.16035439882918592</v>
+        <v>8.560652592627864E-2</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B110">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -8917,36 +8969,36 @@
         <v>0</v>
       </c>
       <c r="F110">
-        <v>0.12838033746056865</v>
+        <v>5.1070746880325146E-2</v>
       </c>
       <c r="G110">
-        <v>-0.41139940038735839</v>
+        <v>-0.20563943801272749</v>
       </c>
       <c r="H110">
-        <v>-1.1484398118795685</v>
+        <v>-0.9084862820756171</v>
       </c>
       <c r="I110">
-        <v>1.1027315119311985E-2</v>
+        <v>-4.4806121859410578E-3</v>
       </c>
       <c r="J110">
-        <v>0.36333856542398846</v>
+        <v>0.67356942233129458</v>
       </c>
       <c r="K110">
-        <v>1.1973187671428076E-2</v>
+        <v>1.8293177597732562E-2</v>
       </c>
       <c r="L110">
-        <v>1.1319028726797504</v>
+        <v>0.90884784585525014</v>
       </c>
       <c r="M110">
-        <v>0.23279046238150966</v>
+        <v>0.1118406496414306</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>3</v>
+        <v>-10</v>
       </c>
       <c r="B111">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -8958,36 +9010,36 @@
         <v>0</v>
       </c>
       <c r="F111">
-        <v>4.0050776551835844E-2</v>
+        <v>-5.0027938577338123E-2</v>
       </c>
       <c r="G111">
-        <v>-0.34906734647434196</v>
+        <v>-0.16787578987678636</v>
       </c>
       <c r="H111">
-        <v>-0.42120721955691437</v>
+        <v>0.38554473622205221</v>
       </c>
       <c r="I111">
-        <v>9.6645159441334314E-3</v>
+        <v>2.575041145684303E-2</v>
       </c>
       <c r="J111">
-        <v>0.21134821837795698</v>
+        <v>0.58381833783153814</v>
       </c>
       <c r="K111">
-        <v>3.5861930521240704E-2</v>
+        <v>1.3972419247413822E-2</v>
       </c>
       <c r="L111">
-        <v>0.42272606539050189</v>
+        <v>-0.37100018499813575</v>
       </c>
       <c r="M111">
-        <v>-1.7951605742576524E-2</v>
+        <v>0.1666251990856247</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="B112">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -8999,33 +9051,33 @@
         <v>0</v>
       </c>
       <c r="F112">
-        <v>3.6049260753956452E-2</v>
+        <v>-4.2445598853748108E-2</v>
       </c>
       <c r="G112">
-        <v>-0.33714576611907043</v>
+        <v>-0.17410989314356345</v>
       </c>
       <c r="H112">
-        <v>-0.58307267326184264</v>
+        <v>-6.5695455195958236E-2</v>
       </c>
       <c r="I112">
-        <v>5.1722990716013108E-3</v>
+        <v>4.3400079189802607E-3</v>
       </c>
       <c r="J112">
-        <v>0.37265308151036075</v>
+        <v>0.60973770489389667</v>
       </c>
       <c r="K112">
-        <v>2.5274150641253865E-2</v>
+        <v>1.5545018857230822E-2</v>
       </c>
       <c r="L112">
-        <v>0.58364671397835965</v>
+        <v>6.7826852862145043E-2</v>
       </c>
       <c r="M112">
-        <v>2.5095911377773148E-2</v>
+        <v>9.61493609518555E-2</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="B113">
         <v>45</v>
@@ -9040,33 +9092,33 @@
         <v>0</v>
       </c>
       <c r="F113">
-        <v>-5.2596574343978866E-2</v>
+        <v>1.4562382430074136E-2</v>
       </c>
       <c r="G113">
-        <v>-0.36697881086611123</v>
+        <v>-0.34117274201218539</v>
       </c>
       <c r="H113">
-        <v>0.16282144189795822</v>
+        <v>-0.26292881549732261</v>
       </c>
       <c r="I113">
-        <v>2.054244668063852E-2</v>
+        <v>1.2974792629972969E-2</v>
       </c>
       <c r="J113">
-        <v>1.8191006122906254E-2</v>
+        <v>0.13071235106523052</v>
       </c>
       <c r="K113">
-        <v>3.2009131654802486E-2</v>
+        <v>3.6569708865806155E-2</v>
       </c>
       <c r="L113">
-        <v>-0.15121451905138086</v>
+        <v>0.26292881549732261</v>
       </c>
       <c r="M113">
-        <v>8.0071160866515792E-2</v>
+        <v>0.23094840006628753</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>-3</v>
+        <v>12</v>
       </c>
       <c r="B114">
         <v>45</v>
@@ -9081,36 +9133,36 @@
         <v>0</v>
       </c>
       <c r="F114">
-        <v>-1.1467350049231788E-2</v>
+        <v>6.6744928603131207E-2</v>
       </c>
       <c r="G114">
-        <v>-0.33984985556685265</v>
+        <v>-0.35855411499705614</v>
       </c>
       <c r="H114">
-        <v>-0.12936593336962468</v>
+        <v>-0.88189487677332457</v>
       </c>
       <c r="I114">
-        <v>1.6670300320380294E-2</v>
+        <v>1.1494985182503414E-3</v>
       </c>
       <c r="J114">
-        <v>3.0627950040284596E-2</v>
+        <v>0.50424292019560746</v>
       </c>
       <c r="K114">
-        <v>3.5839742035837806E-2</v>
+        <v>1.5293832187298809E-2</v>
       </c>
       <c r="L114">
-        <v>0.1297887965843986</v>
+        <v>0.8765004087746503</v>
       </c>
       <c r="M114">
-        <v>4.681144616371917E-3</v>
+        <v>0.33702404704451111</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B115">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -9122,36 +9174,36 @@
         <v>0</v>
       </c>
       <c r="F115">
-        <v>-5.9277281356348716E-2</v>
+        <v>7.4681583023926496E-2</v>
       </c>
       <c r="G115">
-        <v>-4.5795131572825248E-2</v>
+        <v>-0.42493755420952761</v>
       </c>
       <c r="H115">
-        <v>-0.45321817305868006</v>
+        <v>-0.89827728298763987</v>
       </c>
       <c r="I115">
-        <v>4.790722037972777E-4</v>
+        <v>6.6431830838151089E-3</v>
       </c>
       <c r="J115">
-        <v>0.53588946501178747</v>
+        <v>0.35353635633790342</v>
       </c>
       <c r="K115">
-        <v>4.556494574114188E-3</v>
+        <v>1.2082185600684459E-2</v>
       </c>
       <c r="L115">
-        <v>0.45321817305868006</v>
+        <v>0.88699824281153261</v>
       </c>
       <c r="M115">
-        <v>5.9277281356348716E-2</v>
+        <v>0.41386390896759262</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B116">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -9163,36 +9215,36 @@
         <v>0</v>
       </c>
       <c r="F116">
-        <v>0.21367986198260264</v>
+        <v>0.12838033746056865</v>
       </c>
       <c r="G116">
-        <v>-5.5995179334707809E-2</v>
+        <v>-0.41139940038735839</v>
       </c>
       <c r="H116">
-        <v>-1.8566323867473109</v>
+        <v>-1.1484398118795685</v>
       </c>
       <c r="I116">
-        <v>1.3720205605942724E-3</v>
+        <v>1.1027315119311985E-2</v>
       </c>
       <c r="J116">
-        <v>0.6358839619235559</v>
+        <v>0.36333856542398846</v>
       </c>
       <c r="K116">
-        <v>7.46922132412831E-3</v>
+        <v>1.1973187671428076E-2</v>
       </c>
       <c r="L116">
-        <v>1.8604870559400697</v>
+        <v>1.1319028726797504</v>
       </c>
       <c r="M116">
-        <v>0.17700513443223193</v>
+        <v>0.45551102033549801</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B117">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -9204,36 +9256,36 @@
         <v>0</v>
       </c>
       <c r="F117">
-        <v>0.36353755884268868</v>
+        <v>4.0050776551835844E-2</v>
       </c>
       <c r="G117">
-        <v>-5.6972347940228305E-2</v>
+        <v>-0.34906734647434196</v>
       </c>
       <c r="H117">
-        <v>-2.2294407327960712</v>
+        <v>-0.42120721955691437</v>
       </c>
       <c r="I117">
-        <v>2.4192421146164793E-3</v>
+        <v>9.6645159441334314E-3</v>
       </c>
       <c r="J117">
-        <v>0.67650698563225609</v>
+        <v>0.21134821837795698</v>
       </c>
       <c r="K117">
-        <v>7.9294107456995833E-3</v>
+        <v>3.5861930521240704E-2</v>
       </c>
       <c r="L117">
-        <v>2.2475648258271175</v>
+        <v>0.42272606539050189</v>
       </c>
       <c r="M117">
-        <v>0.22587140466270847</v>
+        <v>0.23413418562903801</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B118">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -9245,36 +9297,36 @@
         <v>0</v>
       </c>
       <c r="F118">
-        <v>0.55163035281987971</v>
+        <v>3.6049260753956452E-2</v>
       </c>
       <c r="G118">
-        <v>-5.696113208327757E-2</v>
+        <v>-0.33714576611907043</v>
       </c>
       <c r="H118">
-        <v>-2.5984390803467106</v>
+        <v>-0.58307267326184264</v>
       </c>
       <c r="I118">
-        <v>4.3182000198383787E-3</v>
+        <v>5.1722990716013108E-3</v>
       </c>
       <c r="J118">
-        <v>0.7172702506481976</v>
+        <v>0.37265308151036075</v>
       </c>
       <c r="K118">
-        <v>9.0375173385817253E-3</v>
+        <v>2.5274150641253865E-2</v>
       </c>
       <c r="L118">
-        <v>2.6417255731941163</v>
+        <v>0.58364671397835965</v>
       </c>
       <c r="M118">
-        <v>0.27833019303960171</v>
+        <v>0.25614354658640848</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>3</v>
+        <v>-10</v>
       </c>
       <c r="B119">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -9286,36 +9338,36 @@
         <v>0</v>
       </c>
       <c r="F119">
-        <v>-1.244184118689425E-2</v>
+        <v>-5.2596574343978866E-2</v>
       </c>
       <c r="G119">
-        <v>-4.7149660580241247E-2</v>
+        <v>-0.36697881086611123</v>
       </c>
       <c r="H119">
-        <v>-0.77286250802460776</v>
+        <v>0.16282144189795822</v>
       </c>
       <c r="I119">
-        <v>7.0525740867477874E-5</v>
+        <v>2.054244668063852E-2</v>
       </c>
       <c r="J119">
-        <v>0.53531573297310986</v>
+        <v>1.8191006122906254E-2</v>
       </c>
       <c r="K119">
-        <v>5.8990528070585998E-3</v>
+        <v>3.2009131654802486E-2</v>
       </c>
       <c r="L119">
-        <v>0.77115217116192813</v>
+        <v>-0.15121451905138086</v>
       </c>
       <c r="M119">
-        <v>5.2873288477746201E-2</v>
+        <v>0.3161120665413949</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="B120">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -9327,33 +9379,33 @@
         <v>0</v>
       </c>
       <c r="F120">
-        <v>3.1097407134985693E-2</v>
+        <v>-1.1467350049231788E-2</v>
       </c>
       <c r="G120">
-        <v>-5.1040282578760213E-2</v>
+        <v>-0.33984985556685265</v>
       </c>
       <c r="H120">
-        <v>-1.1291257642886272</v>
+        <v>-0.12936593336962468</v>
       </c>
       <c r="I120">
-        <v>1.1886544626932207E-3</v>
+        <v>1.6670300320380294E-2</v>
       </c>
       <c r="J120">
-        <v>0.57099008130640638</v>
+        <v>3.0627950040284596E-2</v>
       </c>
       <c r="K120">
-        <v>6.4517436041181403E-3</v>
+        <v>3.5839742035837806E-2</v>
       </c>
       <c r="L120">
-        <v>1.1261908593889041</v>
+        <v>0.1297887965843986</v>
       </c>
       <c r="M120">
-        <v>8.7098728692080046E-2</v>
+        <v>0.24362020655854169</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="B121">
         <v>5</v>
@@ -9368,33 +9420,33 @@
         <v>0</v>
       </c>
       <c r="F121">
-        <v>-4.9948081335520665E-2</v>
+        <v>-5.9277281356348716E-2</v>
       </c>
       <c r="G121">
-        <v>-5.0781022524719055E-2</v>
+        <v>-4.5795131572825248E-2</v>
       </c>
       <c r="H121">
-        <v>0.36739139563870138</v>
+        <v>-0.45321817305868006</v>
       </c>
       <c r="I121">
-        <v>1.2529484356126138E-2</v>
+        <v>4.790722037972777E-4</v>
       </c>
       <c r="J121">
-        <v>0.63690731732829309</v>
+        <v>0.53588946501178747</v>
       </c>
       <c r="K121">
-        <v>6.6491395005249922E-3</v>
+        <v>4.556494574114188E-3</v>
       </c>
       <c r="L121">
-        <v>-0.35313650151309578</v>
+        <v>0.45321817305868006</v>
       </c>
       <c r="M121">
-        <v>0.11298610409047583</v>
+        <v>6.3043022110943578E-2</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>-3</v>
+        <v>12</v>
       </c>
       <c r="B122">
         <v>5</v>
@@ -9409,69 +9461,315 @@
         <v>0</v>
       </c>
       <c r="F122">
-        <v>-6.6442545327944177E-2</v>
+        <v>0.21367986198260264</v>
       </c>
       <c r="G122">
-        <v>-4.4139661548338129E-2</v>
+        <v>-5.5995179334707809E-2</v>
       </c>
       <c r="H122">
-        <v>-0.11865632733292179</v>
+        <v>-1.8566323867473109</v>
       </c>
       <c r="I122">
-        <v>1.1833717698856931E-3</v>
+        <v>1.3720205605942724E-3</v>
       </c>
       <c r="J122">
-        <v>0.50261730802701676</v>
+        <v>0.6358839619235559</v>
       </c>
       <c r="K122">
-        <v>4.2277992011485969E-3</v>
+        <v>7.46922132412831E-3</v>
       </c>
       <c r="L122">
-        <v>0.12197104710511522</v>
+        <v>1.8604870559400697</v>
       </c>
       <c r="M122">
-        <v>6.0141495773510356E-2</v>
+        <v>0.18121187790161089</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B123">
+        <v>5</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>0.36353755884268868</v>
+      </c>
+      <c r="G123">
+        <v>-5.6972347940228305E-2</v>
+      </c>
+      <c r="H123">
+        <v>-2.2294407327960712</v>
+      </c>
+      <c r="I123">
+        <v>2.4192421146164793E-3</v>
+      </c>
+      <c r="J123">
+        <v>0.67650698563225609</v>
+      </c>
+      <c r="K123">
+        <v>7.9294107456995833E-3</v>
+      </c>
+      <c r="L123">
+        <v>2.2475648258271175</v>
+      </c>
+      <c r="M123">
+        <v>0.22997736307633398</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>18</v>
+      </c>
+      <c r="B124">
+        <v>5</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>0.55163035281987971</v>
+      </c>
+      <c r="G124">
+        <v>-5.696113208327757E-2</v>
+      </c>
+      <c r="H124">
+        <v>-2.5984390803467106</v>
+      </c>
+      <c r="I124">
+        <v>4.3182000198383787E-3</v>
+      </c>
+      <c r="J124">
+        <v>0.7172702506481976</v>
+      </c>
+      <c r="K124">
+        <v>9.0375173385817253E-3</v>
+      </c>
+      <c r="L124">
+        <v>2.6417255731941163</v>
+      </c>
+      <c r="M124">
+        <v>0.28223555239936887</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>3</v>
+      </c>
+      <c r="B125">
+        <v>5</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>-1.244184118689425E-2</v>
+      </c>
+      <c r="G125">
+        <v>-4.7149660580241247E-2</v>
+      </c>
+      <c r="H125">
+        <v>-0.77286250802460776</v>
+      </c>
+      <c r="I125">
+        <v>7.0525740867477874E-5</v>
+      </c>
+      <c r="J125">
+        <v>0.53531573297310986</v>
+      </c>
+      <c r="K125">
+        <v>5.8990528070585998E-3</v>
+      </c>
+      <c r="L125">
+        <v>0.77115217116192813</v>
+      </c>
+      <c r="M125">
+        <v>5.6781453340377042E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>6</v>
+      </c>
+      <c r="B126">
+        <v>5</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>3.1097407134985693E-2</v>
+      </c>
+      <c r="G126">
+        <v>-5.1040282578760213E-2</v>
+      </c>
+      <c r="H126">
+        <v>-1.1291257642886272</v>
+      </c>
+      <c r="I126">
+        <v>1.1886544626932207E-3</v>
+      </c>
+      <c r="J126">
+        <v>0.57099008130640638</v>
+      </c>
+      <c r="K126">
+        <v>6.4517436041181403E-3</v>
+      </c>
+      <c r="L126">
+        <v>1.1261908593889041</v>
+      </c>
+      <c r="M126">
+        <v>9.1215745471783752E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>-10</v>
+      </c>
+      <c r="B127">
+        <v>5</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <v>-4.9948081335520665E-2</v>
+      </c>
+      <c r="G127">
+        <v>-5.0781022524719055E-2</v>
+      </c>
+      <c r="H127">
+        <v>0.36739139563870138</v>
+      </c>
+      <c r="I127">
+        <v>1.2529484356126138E-2</v>
+      </c>
+      <c r="J127">
+        <v>0.63690731732829309</v>
+      </c>
+      <c r="K127">
+        <v>6.6491395005249922E-3</v>
+      </c>
+      <c r="L127">
+        <v>-0.35313650151309578</v>
+      </c>
+      <c r="M127">
+        <v>0.11698201558860154</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>-3</v>
+      </c>
+      <c r="B128">
+        <v>5</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>-6.6442545327944177E-2</v>
+      </c>
+      <c r="G128">
+        <v>-4.4139661548338129E-2</v>
+      </c>
+      <c r="H128">
+        <v>-0.11865632733292179</v>
+      </c>
+      <c r="I128">
+        <v>1.1833717698856931E-3</v>
+      </c>
+      <c r="J128">
+        <v>0.50261730802701676</v>
+      </c>
+      <c r="K128">
+        <v>4.2277992011485969E-3</v>
+      </c>
+      <c r="L128">
+        <v>0.12197104710511522</v>
+      </c>
+      <c r="M128">
+        <v>6.3759664211753816E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>0</v>
+      </c>
+      <c r="B129">
         <v>90</v>
       </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
-      <c r="D123">
-        <v>0</v>
-      </c>
-      <c r="E123">
-        <v>0</v>
-      </c>
-      <c r="F123">
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
         <v>1.7041213729324382E-2</v>
       </c>
-      <c r="G123">
+      <c r="G129">
         <v>-0.36392368744617631</v>
       </c>
-      <c r="H123">
+      <c r="H129">
         <v>-3.6261797567294335E-2</v>
       </c>
-      <c r="I123">
+      <c r="I129">
         <v>-4.0247807343861446E-4</v>
       </c>
-      <c r="J123">
+      <c r="J129">
         <v>1.072780736646251E-2</v>
       </c>
-      <c r="K123">
+      <c r="K129">
         <v>4.3191758762539965E-2</v>
       </c>
-      <c r="L123">
+      <c r="L129">
         <v>3.6261797567294335E-2</v>
       </c>
-      <c r="M123">
-        <v>-1.7041213729324382E-2</v>
+      <c r="M129">
+        <v>0.36392368744617631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modelo dinamico implementado y compilando en Simulink. El modelo dinamico est acompleto!
NO corre en tiempo real, requeire de la optimizacion de Luis
</commit_message>
<xml_diff>
--- a/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
+++ b/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
@@ -4475,10 +4475,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M129"/>
+  <dimension ref="A1:M131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M129"/>
+      <selection activeCell="K1" sqref="K1:M131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5387,7 +5387,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -5402,33 +5402,33 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>-6.6967697591863898E-2</v>
+        <v>0.40509845602615019</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>-8.3563578592191351E-3</v>
       </c>
       <c r="H23">
-        <v>-0.47286118395287446</v>
+        <v>-1.7614898218215362</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>-2.4137552639073067E-3</v>
       </c>
       <c r="J23">
-        <v>0.51028211598236661</v>
+        <v>-1.2480834362936954</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>1.1477498080717985E-3</v>
       </c>
       <c r="L23">
-        <v>0.47286118395287446</v>
+        <v>0.4050984560261503</v>
       </c>
       <c r="M23">
-        <v>6.6967697591863898E-2</v>
+        <v>1.7614898218215362</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5443,33 +5443,33 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0.21137997655391308</v>
+        <v>-6.6967697591863898E-2</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>-1.8867447069043743</v>
+        <v>-0.47286118395287446</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.63536313621467222</v>
+        <v>0.51028211598236661</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>1.8894631765860634</v>
+        <v>0.47286118395287446</v>
       </c>
       <c r="M24">
-        <v>0.185515465244568</v>
+        <v>6.6967697591863898E-2</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -5484,33 +5484,33 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0.36536814081062885</v>
+        <v>0.21137997655391308</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>-2.2610833989652912</v>
+        <v>-1.8867447069043743</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0.67269751360448837</v>
+        <v>0.63536313621467222</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>2.2786030837695344</v>
+        <v>1.8894631765860634</v>
       </c>
       <c r="M25">
-        <v>0.23229292290515124</v>
+        <v>0.185515465244568</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -5525,33 +5525,33 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0.55847162213707935</v>
+        <v>0.36536814081062885</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>-2.6339987948482624</v>
+        <v>-2.2610833989652912</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0.69835427003245021</v>
+        <v>0.67269751360448837</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>2.6776589398705228</v>
+        <v>2.2786030837695344</v>
       </c>
       <c r="M26">
-        <v>0.2828123153718497</v>
+        <v>0.23229292290515124</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -5566,33 +5566,33 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>-2.1753720153178752E-2</v>
+        <v>0.55847162213707935</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>-0.79265197140277466</v>
+        <v>-2.6339987948482624</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
       <c r="J27">
-        <v>0.5262434022890089</v>
+        <v>0.69835427003245021</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>0.79042716767819055</v>
+        <v>2.6776589398705228</v>
       </c>
       <c r="M27">
-        <v>6.3208106326968869E-2</v>
+        <v>0.2828123153718497</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -5607,33 +5607,33 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>2.3062574236263095E-2</v>
+        <v>-2.1753720153178752E-2</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>-1.1557532330474607</v>
+        <v>-0.79265197140277466</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
       <c r="J28">
-        <v>0.57426304489880331</v>
+        <v>0.5262434022890089</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1.1518325913522831</v>
+        <v>0.79042716767819055</v>
       </c>
       <c r="M28">
-        <v>9.7872874325553361E-2</v>
+        <v>6.3208106326968869E-2</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5648,33 +5648,33 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>-4.985516053549531E-2</v>
+        <v>2.3062574236263095E-2</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0.37620460456128124</v>
+        <v>-1.1557532330474607</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>0.65093204377041869</v>
+        <v>0.57426304489880331</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>-0.36183195351656067</v>
+        <v>1.1518325913522831</v>
       </c>
       <c r="M29">
-        <v>0.11442499263499868</v>
+        <v>9.7872874325553361E-2</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -5689,33 +5689,33 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>-7.4538276617457086E-2</v>
+        <v>-4.985516053549531E-2</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>-0.13398232744714891</v>
+        <v>0.37620460456128124</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0.47918821351918878</v>
+        <v>0.65093204377041869</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
       <c r="L30">
-        <v>0.13769974130735699</v>
+        <v>-0.36183195351656067</v>
       </c>
       <c r="M30">
-        <v>6.7424031273297144E-2</v>
+        <v>0.11442499263499868</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -5724,39 +5724,39 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>-7.4681987612586848E-2</v>
+        <v>-7.4538276617457086E-2</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>-0.65750743101589437</v>
+        <v>-0.13398232744714891</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>-0.26343901632569489</v>
+        <v>0.47918821351918878</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
       <c r="L31">
-        <v>0.65750743101589437</v>
+        <v>0.13769974130735699</v>
       </c>
       <c r="M31">
-        <v>7.4681987612586848E-2</v>
+        <v>6.7424031273297144E-2</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -5771,33 +5771,33 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0.22653618396510811</v>
+        <v>-7.4681987612586848E-2</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>-2.0705025777114399</v>
+        <v>-0.65750743101589437</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>-0.13700551117229398</v>
+        <v>-0.26343901632569489</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>2.0723566497411938</v>
+        <v>0.65750743101589437</v>
       </c>
       <c r="M32">
-        <v>0.20889586694965206</v>
+        <v>7.4681987612586848E-2</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -5812,33 +5812,33 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0.38433949272260276</v>
+        <v>0.22653618396510811</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>-2.4406084677959718</v>
+        <v>-2.0705025777114399</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33">
-        <v>-7.9499234033366797E-2</v>
+        <v>-0.13700551117229398</v>
       </c>
       <c r="K33">
         <v>0</v>
       </c>
       <c r="L33">
-        <v>2.4569211314055726</v>
+        <v>2.0723566497411938</v>
       </c>
       <c r="M33">
-        <v>0.26043251102047832</v>
+        <v>0.20889586694965206</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -5853,33 +5853,33 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0.58043086328364413</v>
+        <v>0.38433949272260276</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>-2.8066200370508598</v>
+        <v>-2.4406084677959718</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>-2.7714158216158725E-2</v>
+        <v>-7.9499234033366797E-2</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>2.8486172758161334</v>
+        <v>2.4569211314055726</v>
       </c>
       <c r="M34">
-        <v>0.31527073341722911</v>
+        <v>0.26043251102047832</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5894,33 +5894,33 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0.72257858245084117</v>
+        <v>0.58043086328364413</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>-2.9578097861150385</v>
+        <v>-2.8066200370508598</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>0.12330119266677141</v>
+        <v>-2.7714158216158725E-2</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
-        <v>3.0131161798127146</v>
+        <v>2.8486172758161334</v>
       </c>
       <c r="M35">
-        <v>0.43805185264462587</v>
+        <v>0.31527073341722911</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5935,33 +5935,33 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.58565621338973528</v>
+        <v>0.72257858245084117</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>-2.7818879292521048</v>
+        <v>-2.9578097861150385</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>4.7748252489993689E-2</v>
+        <v>0.12330119266677141</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>2.768755703824854</v>
+        <v>3.0131161798127146</v>
       </c>
       <c r="M36">
-        <v>0.64489185429644336</v>
+        <v>0.43805185264462587</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5976,33 +5976,33 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>-1.5557685578775272E-2</v>
+        <v>0.58565621338973528</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>-1.8203475590159175</v>
+        <v>-2.7818879292521048</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37">
-        <v>-0.35668664230964209</v>
+        <v>4.7748252489993689E-2</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>1.4822179024322213</v>
+        <v>2.768755703824854</v>
       </c>
       <c r="M37">
-        <v>1.0568525757669345</v>
+        <v>0.64489185429644336</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -6017,33 +6017,33 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>-2.3304508550854926E-2</v>
+        <v>-1.5557685578775272E-2</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>-0.97656185923510674</v>
+        <v>-1.8203475590159175</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
       <c r="J38">
-        <v>-0.24467922970624151</v>
+        <v>-0.35668664230964209</v>
       </c>
       <c r="K38">
         <v>0</v>
       </c>
       <c r="L38">
-        <v>0.97400385140723522</v>
+        <v>1.4822179024322213</v>
       </c>
       <c r="M38">
-        <v>7.4381869265280662E-2</v>
+        <v>1.0568525757669345</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -6058,33 +6058,33 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>2.6952950831595199E-2</v>
+        <v>-2.3304508550854926E-2</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>-1.3307533742524675</v>
+        <v>-0.97656185923510674</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39">
-        <v>-0.21095811311478116</v>
+        <v>-0.24467922970624151</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>1.3262807185602445</v>
+        <v>0.97400385140723522</v>
       </c>
       <c r="M39">
-        <v>0.11229630545204901</v>
+        <v>7.4381869265280662E-2</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -6099,33 +6099,33 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>-7.718607828718764E-2</v>
+        <v>2.6952950831595199E-2</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>0.18832547032290964</v>
+        <v>-1.3307533742524675</v>
       </c>
       <c r="I40">
         <v>0</v>
       </c>
       <c r="J40">
-        <v>-0.14746361651005876</v>
+        <v>-0.21095811311478116</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>-0.17206116142784475</v>
+        <v>1.3262807185602445</v>
       </c>
       <c r="M40">
-        <v>0.10871582305167048</v>
+        <v>0.11229630545204901</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -6140,33 +6140,33 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>-8.7916609710199989E-2</v>
+        <v>-7.718607828718764E-2</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>-0.32266759723232541</v>
+        <v>0.18832547032290964</v>
       </c>
       <c r="I41">
         <v>0</v>
       </c>
       <c r="J41">
-        <v>-0.30691885907496097</v>
+        <v>-0.14746361651005876</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>0.32682659234331435</v>
+        <v>-0.17206116142784475</v>
       </c>
       <c r="M41">
-        <v>7.0909005802329672E-2</v>
+        <v>0.10871582305167048</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6175,39 +6175,39 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>-8.5429671993744891E-2</v>
+        <v>-8.7916609710199989E-2</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>-0.72370940298428799</v>
+        <v>-0.32266759723232541</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>-0.54379963954552524</v>
+        <v>-0.30691885907496097</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>0.72370940298428799</v>
+        <v>0.32682659234331435</v>
       </c>
       <c r="M42">
-        <v>8.5429671993744891E-2</v>
+        <v>7.0909005802329672E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6222,33 +6222,33 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0.21332993320000762</v>
+        <v>-8.5429671993744891E-2</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>-2.0993820970085664</v>
+        <v>-0.72370940298428799</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
       <c r="J43">
-        <v>-0.25829277660138666</v>
+        <v>-0.54379963954552524</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>2.0978593483260881</v>
+        <v>0.72370940298428799</v>
       </c>
       <c r="M43">
-        <v>0.22781791913729374</v>
+        <v>8.5429671993744891E-2</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6263,33 +6263,33 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0.36775805680102264</v>
+        <v>0.21332993320000762</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>-2.455894824377868</v>
+        <v>-2.0993820970085664</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>-0.14263048587484461</v>
+        <v>-0.25829277660138666</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
-        <v>2.4673950266062379</v>
+        <v>2.0978593483260881</v>
       </c>
       <c r="M44">
-        <v>0.28040534842771281</v>
+        <v>0.22781791913729374</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6304,33 +6304,33 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0.55303757989544111</v>
+        <v>0.36775805680102264</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>-2.787104511410142</v>
+        <v>-2.455894824377868</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>5.6639586294437348E-2</v>
+        <v>-0.14263048587484461</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>2.8215919178879201</v>
+        <v>2.4673950266062379</v>
       </c>
       <c r="M45">
-        <v>0.3352926650091575</v>
+        <v>0.28040534842771281</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -6345,33 +6345,33 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>0.68116461703126108</v>
+        <v>0.55303757989544111</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>-2.8980406823460374</v>
+        <v>-2.787104511410142</v>
       </c>
       <c r="I46">
         <v>0</v>
       </c>
       <c r="J46">
-        <v>0.31872311046694207</v>
+        <v>5.6639586294437348E-2</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>2.9421852872904966</v>
+        <v>2.8215919178879201</v>
       </c>
       <c r="M46">
-        <v>0.45406031238082001</v>
+        <v>0.3352926650091575</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6386,33 +6386,33 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0.52641255960326594</v>
+        <v>0.68116461703126108</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>-2.670212924281651</v>
+        <v>-2.8980406823460374</v>
       </c>
       <c r="I47">
         <v>0</v>
       </c>
       <c r="J47">
-        <v>5.9318386681059529E-2</v>
+        <v>0.31872311046694207</v>
       </c>
       <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
-        <v>2.6425063272203695</v>
+        <v>2.9421852872904966</v>
       </c>
       <c r="M47">
-        <v>0.65138894257512669</v>
+        <v>0.45406031238082001</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -6427,33 +6427,33 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>-1.6539195382390338E-2</v>
+        <v>0.52641255960326594</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>-1.8891033887224336</v>
+        <v>-2.670212924281651</v>
       </c>
       <c r="I48">
         <v>0</v>
       </c>
       <c r="J48">
-        <v>-0.36987756945978184</v>
+        <v>5.9318386681059529E-2</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
       <c r="L48">
-        <v>1.5379764099976985</v>
+        <v>2.6425063272203695</v>
       </c>
       <c r="M48">
-        <v>1.0970933053104786</v>
+        <v>0.65138894257512669</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -6468,33 +6468,33 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>-3.3598927806487079E-2</v>
+        <v>-1.6539195382390338E-2</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>-1.0353841375278308</v>
+        <v>-1.8891033887224336</v>
       </c>
       <c r="I49">
         <v>0</v>
       </c>
       <c r="J49">
-        <v>-0.49392877418713621</v>
+        <v>-0.36987756945978184</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>1.0322067475361931</v>
+        <v>1.5379764099976985</v>
       </c>
       <c r="M49">
-        <v>8.7740700559939391E-2</v>
+        <v>1.0970933053104786</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -6509,33 +6509,33 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>1.6491058929627832E-2</v>
+        <v>-3.3598927806487079E-2</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>-1.3852009656776634</v>
+        <v>-1.0353841375278308</v>
       </c>
       <c r="I50">
         <v>0</v>
       </c>
       <c r="J50">
-        <v>-0.41934117520233494</v>
+        <v>-0.49392877418713621</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
-        <v>1.3793364748992825</v>
+        <v>1.0322067475361931</v>
       </c>
       <c r="M50">
-        <v>0.12839220907583238</v>
+        <v>8.7740700559939391E-2</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -6550,33 +6550,33 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>-9.8626430925695188E-2</v>
+        <v>1.6491058929627832E-2</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>9.0518855786986888E-2</v>
+        <v>-1.3852009656776634</v>
       </c>
       <c r="I51">
         <v>0</v>
       </c>
       <c r="J51">
-        <v>-0.55841392539558155</v>
+        <v>-0.41934117520233494</v>
       </c>
       <c r="K51">
         <v>0</v>
       </c>
       <c r="L51">
-        <v>-7.2017370972778313E-2</v>
+        <v>1.3793364748992825</v>
       </c>
       <c r="M51">
-        <v>0.11284650817945356</v>
+        <v>0.12839220907583238</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -6591,33 +6591,33 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <v>-0.10181096777716636</v>
+        <v>-9.8626430925695188E-2</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>-0.40003493281219354</v>
+        <v>9.0518855786986888E-2</v>
       </c>
       <c r="I52">
         <v>0</v>
       </c>
       <c r="J52">
-        <v>-0.62825495094738204</v>
+        <v>-0.55841392539558155</v>
       </c>
       <c r="K52">
         <v>0</v>
       </c>
       <c r="L52">
-        <v>0.40481507319445559</v>
+        <v>-7.2017370972778313E-2</v>
       </c>
       <c r="M52">
-        <v>8.0735228644916612E-2</v>
+        <v>0.11284650817945356</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -6626,39 +6626,39 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>-6.8496245088475988E-2</v>
+        <v>-0.10181096777716636</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>-0.56496728530850515</v>
+        <v>-0.40003493281219354</v>
       </c>
       <c r="I53">
         <v>0</v>
       </c>
       <c r="J53">
-        <v>0.121901923520936</v>
+        <v>-0.62825495094738204</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
-        <v>0.56496728530850515</v>
+        <v>0.40481507319445559</v>
       </c>
       <c r="M53">
-        <v>6.8496245088475988E-2</v>
+        <v>8.0735228644916612E-2</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6673,33 +6673,33 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0.22271152705902242</v>
+        <v>-6.8496245088475988E-2</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>-1.9788706129954865</v>
+        <v>-0.56496728530850515</v>
       </c>
       <c r="I54">
         <v>0</v>
       </c>
       <c r="J54">
-        <v>0.24523509821471629</v>
+        <v>0.121901923520936</v>
       </c>
       <c r="K54">
         <v>0</v>
       </c>
       <c r="L54">
-        <v>1.9819318724196169</v>
+        <v>0.56496728530850515</v>
       </c>
       <c r="M54">
-        <v>0.19358558920892258</v>
+        <v>6.8496245088475988E-2</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -6714,33 +6714,33 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0.37856085750210883</v>
+        <v>0.22271152705902242</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>-2.3520082753719005</v>
+        <v>-1.9788706129954865</v>
       </c>
       <c r="I55">
         <v>0</v>
       </c>
       <c r="J55">
-        <v>0.28937363651564396</v>
+        <v>0.24523509821471629</v>
       </c>
       <c r="K55">
         <v>0</v>
       </c>
       <c r="L55">
-        <v>2.3698442964792168</v>
+        <v>1.9819318724196169</v>
       </c>
       <c r="M55">
-        <v>0.24308282682155927</v>
+        <v>0.19358558920892258</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -6755,33 +6755,33 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0.57310594071170506</v>
+        <v>0.37856085750210883</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>-2.7216349311976553</v>
+        <v>-2.3520082753719005</v>
       </c>
       <c r="I56">
         <v>0</v>
       </c>
       <c r="J56">
-        <v>0.32755054698950536</v>
+        <v>0.28937363651564396</v>
       </c>
       <c r="K56">
         <v>0</v>
       </c>
       <c r="L56">
-        <v>2.7655281115491999</v>
+        <v>2.3698442964792168</v>
       </c>
       <c r="M56">
-        <v>0.29597530678323508</v>
+        <v>0.24308282682155927</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -6796,33 +6796,33 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0.70886868953398696</v>
+        <v>0.57310594071170506</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>-2.8763578652502293</v>
+        <v>-2.7216349311976553</v>
       </c>
       <c r="I57">
         <v>0</v>
       </c>
       <c r="J57">
-        <v>0.33843077078853501</v>
+        <v>0.32755054698950536</v>
       </c>
       <c r="K57">
         <v>0</v>
       </c>
       <c r="L57">
-        <v>2.9324594575817322</v>
+        <v>2.7655281115491999</v>
       </c>
       <c r="M57">
-        <v>0.42025101740262394</v>
+        <v>0.29597530678323508</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -6837,33 +6837,33 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>0.56918423918376349</v>
+        <v>0.70886868953398696</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>-2.6987792799381118</v>
+        <v>-2.8763578652502293</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
       <c r="J58">
-        <v>0.22392012366737543</v>
+        <v>0.33843077078853501</v>
       </c>
       <c r="K58">
         <v>0</v>
       </c>
       <c r="L58">
-        <v>2.6864723306751181</v>
+        <v>2.9324594575817322</v>
       </c>
       <c r="M58">
-        <v>0.62469729987848532</v>
+        <v>0.42025101740262394</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -6878,33 +6878,33 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>-1.835141525929784E-2</v>
+        <v>0.56918423918376349</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>-1.7914918476078321</v>
+        <v>-2.6987792799381118</v>
       </c>
       <c r="I59">
         <v>0</v>
       </c>
       <c r="J59">
-        <v>-0.34324515775510595</v>
+        <v>0.22392012366737543</v>
       </c>
       <c r="K59">
         <v>0</v>
       </c>
       <c r="L59">
-        <v>1.4569782699285925</v>
+        <v>2.6864723306751181</v>
       </c>
       <c r="M59">
-        <v>1.0425901090281018</v>
+        <v>0.62469729987848532</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -6919,33 +6919,33 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>-1.844713876167519E-2</v>
+        <v>-1.835141525929784E-2</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>-0.88384405730146687</v>
+        <v>-1.7914918476078321</v>
       </c>
       <c r="I60">
         <v>0</v>
       </c>
       <c r="J60">
-        <v>0.14107790350215352</v>
+        <v>-0.34324515775510595</v>
       </c>
       <c r="K60">
         <v>0</v>
       </c>
       <c r="L60">
-        <v>0.88166733109152029</v>
+        <v>1.4569782699285925</v>
       </c>
       <c r="M60">
-        <v>6.4678681507640265E-2</v>
+        <v>1.0425901090281018</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -6960,33 +6960,33 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>2.8352590222335456E-2</v>
+        <v>-1.844713876167519E-2</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>-1.2563519895601134</v>
+        <v>-0.88384405730146687</v>
       </c>
       <c r="I61">
         <v>0</v>
       </c>
       <c r="J61">
-        <v>0.18562367421745316</v>
+        <v>0.14107790350215352</v>
       </c>
       <c r="K61">
         <v>0</v>
       </c>
       <c r="L61">
-        <v>1.2524332145926234</v>
+        <v>0.88166733109152029</v>
       </c>
       <c r="M61">
-        <v>0.10312727102546061</v>
+        <v>6.4678681507640265E-2</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -7001,33 +7001,33 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>-6.0064392872935371E-2</v>
+        <v>2.8352590222335456E-2</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>0.28251967244743303</v>
+        <v>-1.2563519895601134</v>
       </c>
       <c r="I62">
         <v>0</v>
       </c>
       <c r="J62">
-        <v>0.25045575785478952</v>
+        <v>0.18562367421745316</v>
       </c>
       <c r="K62">
         <v>0</v>
       </c>
       <c r="L62">
-        <v>-0.26779749143964576</v>
+        <v>1.2524332145926234</v>
       </c>
       <c r="M62">
-        <v>0.10821090605679277</v>
+        <v>0.10312727102546061</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -7042,33 +7042,33 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>-7.7799878933980257E-2</v>
+        <v>-6.0064392872935371E-2</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>-0.22835660951135309</v>
+        <v>0.28251967244743303</v>
       </c>
       <c r="I63">
         <v>0</v>
       </c>
       <c r="J63">
-        <v>8.3652201891138964E-2</v>
+        <v>0.25045575785478952</v>
       </c>
       <c r="K63">
         <v>0</v>
       </c>
       <c r="L63">
-        <v>0.23211538577404953</v>
+        <v>-0.26779749143964576</v>
       </c>
       <c r="M63">
-        <v>6.5741995380629692E-2</v>
+        <v>0.10821090605679277</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -7077,39 +7077,39 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <v>-7.7195931073887322E-2</v>
+        <v>-7.7799878933980257E-2</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>-0.30548908261149982</v>
+        <v>-0.22835660951135309</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64">
-        <v>1.2170847420967017</v>
+        <v>8.3652201891138964E-2</v>
       </c>
       <c r="K64">
         <v>0</v>
       </c>
       <c r="L64">
-        <v>0.30548908261149982</v>
+        <v>0.23211538577404953</v>
       </c>
       <c r="M64">
-        <v>7.7195931073887322E-2</v>
+        <v>6.5741995380629692E-2</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -7124,33 +7124,33 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0.18073217616807821</v>
+        <v>-7.7195931073887322E-2</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>-1.7188149530669425</v>
+        <v>-0.30548908261149982</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65">
-        <v>1.3494623786828075</v>
+        <v>1.2170847420967017</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
-        <v>1.7188310547800971</v>
+        <v>0.30548908261149982</v>
       </c>
       <c r="M65">
-        <v>0.18057897860079045</v>
+        <v>7.7195931073887322E-2</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -7165,33 +7165,33 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.3296738451692775</v>
+        <v>0.18073217616807821</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>-2.0922229843557751</v>
+        <v>-1.7188149530669425</v>
       </c>
       <c r="I66">
         <v>0</v>
       </c>
       <c r="J66">
-        <v>1.3871647891826986</v>
+        <v>1.3494623786828075</v>
       </c>
       <c r="K66">
         <v>0</v>
       </c>
       <c r="L66">
-        <v>2.1062580847468211</v>
+        <v>1.7188310547800971</v>
       </c>
       <c r="M66">
-        <v>0.22306667365147909</v>
+        <v>0.18057897860079045</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -7206,33 +7206,33 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0.51972032803105017</v>
+        <v>0.3296738451692775</v>
       </c>
       <c r="G67">
         <v>0</v>
       </c>
       <c r="H67">
-        <v>-2.4682677185949227</v>
+        <v>-2.0922229843557751</v>
       </c>
       <c r="I67">
         <v>0</v>
       </c>
       <c r="J67">
-        <v>1.4034418238536202</v>
+        <v>1.3871647891826986</v>
       </c>
       <c r="K67">
         <v>0</v>
       </c>
       <c r="L67">
-        <v>2.5080645114143905</v>
+        <v>2.1062580847468211</v>
       </c>
       <c r="M67">
-        <v>0.26845326708792649</v>
+        <v>0.22306667365147909</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -7247,33 +7247,33 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>0.68599736513590925</v>
+        <v>0.51972032803105017</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>-2.7239339886543155</v>
+        <v>-2.4682677185949227</v>
       </c>
       <c r="I68">
         <v>0</v>
       </c>
       <c r="J68">
-        <v>1.1538807318073121</v>
+        <v>1.4034418238536202</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>2.7825667512318466</v>
+        <v>2.5080645114143905</v>
       </c>
       <c r="M68">
-        <v>0.38435795095023834</v>
+        <v>0.26845326708792649</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -7288,33 +7288,33 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>0.54597524770037775</v>
+        <v>0.68599736513590925</v>
       </c>
       <c r="G69">
         <v>0</v>
       </c>
       <c r="H69">
-        <v>-2.5273816121985733</v>
+        <v>-2.7239339886543155</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69">
-        <v>0.7076472884268511</v>
+        <v>1.1538807318073121</v>
       </c>
       <c r="K69">
         <v>0</v>
       </c>
       <c r="L69">
-        <v>2.5213247460853911</v>
+        <v>2.7825667512318466</v>
       </c>
       <c r="M69">
-        <v>0.57329600518265156</v>
+        <v>0.38435795095023834</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -7329,33 +7329,33 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>-1.1039537451429347E-2</v>
+        <v>0.54597524770037775</v>
       </c>
       <c r="G70">
         <v>0</v>
       </c>
       <c r="H70">
-        <v>-1.7913950011132203</v>
+        <v>-2.5273816121985733</v>
       </c>
       <c r="I70">
         <v>0</v>
       </c>
       <c r="J70">
-        <v>2.7652072007542945E-2</v>
+        <v>0.7076472884268511</v>
       </c>
       <c r="K70">
         <v>0</v>
       </c>
       <c r="L70">
-        <v>1.4610928587406207</v>
+        <v>2.5213247460853911</v>
       </c>
       <c r="M70">
-        <v>1.0365450205069424</v>
+        <v>0.57329600518265156</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -7370,33 +7370,33 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>-3.5178793356106131E-2</v>
+        <v>-1.1039537451429347E-2</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>-0.62958462063937748</v>
+        <v>-1.7913950011132203</v>
       </c>
       <c r="I71">
         <v>0</v>
       </c>
       <c r="J71">
-        <v>1.2167173554646495</v>
+        <v>2.7652072007542945E-2</v>
       </c>
       <c r="K71">
         <v>0</v>
       </c>
       <c r="L71">
-        <v>0.62688068100797167</v>
+        <v>1.4610928587406207</v>
       </c>
       <c r="M71">
-        <v>6.8080495199448407E-2</v>
+        <v>1.0365450205069424</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -7411,33 +7411,33 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <v>4.3461943916355593E-3</v>
+        <v>-3.5178793356106131E-2</v>
       </c>
       <c r="G72">
         <v>0</v>
       </c>
       <c r="H72">
-        <v>-0.98649921800662743</v>
+        <v>-0.62958462063937748</v>
       </c>
       <c r="I72">
         <v>0</v>
       </c>
       <c r="J72">
-        <v>1.2779142661211149</v>
+        <v>1.2167173554646495</v>
       </c>
       <c r="K72">
         <v>0</v>
       </c>
       <c r="L72">
-        <v>0.98154937309209067</v>
+        <v>0.62688068100797167</v>
       </c>
       <c r="M72">
-        <v>9.8794861788966265E-2</v>
+        <v>6.8080495199448407E-2</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -7452,33 +7452,33 @@
         <v>0</v>
       </c>
       <c r="F73">
-        <v>-4.7459353129715436E-2</v>
+        <v>4.3461943916355593E-3</v>
       </c>
       <c r="G73">
         <v>0</v>
       </c>
       <c r="H73">
-        <v>0.53483256261998691</v>
+        <v>-0.98649921800662743</v>
       </c>
       <c r="I73">
         <v>0</v>
       </c>
       <c r="J73">
-        <v>1.3350547545921554</v>
+        <v>1.2779142661211149</v>
       </c>
       <c r="K73">
         <v>0</v>
       </c>
       <c r="L73">
-        <v>-0.518466024047324</v>
+        <v>0.98154937309209067</v>
       </c>
       <c r="M73">
-        <v>0.1396110387709831</v>
+        <v>9.8794861788966265E-2</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -7493,33 +7493,33 @@
         <v>0</v>
       </c>
       <c r="F74">
-        <v>-7.9837764981612436E-2</v>
+        <v>-4.7459353129715436E-2</v>
       </c>
       <c r="G74">
         <v>0</v>
       </c>
       <c r="H74">
-        <v>3.3530079840469615E-2</v>
+        <v>0.53483256261998691</v>
       </c>
       <c r="I74">
         <v>0</v>
       </c>
       <c r="J74">
-        <v>1.1838308031410509</v>
+        <v>1.3350547545921554</v>
       </c>
       <c r="K74">
         <v>0</v>
       </c>
       <c r="L74">
-        <v>-2.9305742256759783E-2</v>
+        <v>-0.518466024047324</v>
       </c>
       <c r="M74">
-        <v>8.1483178890785865E-2</v>
+        <v>0.1396110387709831</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -7528,39 +7528,39 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75">
-        <v>-9.4084386734767128E-2</v>
+        <v>-7.9837764981612436E-2</v>
       </c>
       <c r="G75">
         <v>0</v>
       </c>
       <c r="H75">
-        <v>-0.29196217368460958</v>
+        <v>3.3530079840469615E-2</v>
       </c>
       <c r="I75">
         <v>0</v>
       </c>
       <c r="J75">
-        <v>1.2767926677740682</v>
+        <v>1.1838308031410509</v>
       </c>
       <c r="K75">
         <v>0</v>
       </c>
       <c r="L75">
-        <v>0.29196217368460958</v>
+        <v>-2.9305742256759783E-2</v>
       </c>
       <c r="M75">
-        <v>9.4084386734767128E-2</v>
+        <v>8.1483178890785865E-2</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -7575,33 +7575,33 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <v>0.16224482491377495</v>
+        <v>-9.4084386734767128E-2</v>
       </c>
       <c r="G76">
         <v>0</v>
       </c>
       <c r="H76">
-        <v>-1.6758814822736328</v>
+        <v>-0.29196217368460958</v>
       </c>
       <c r="I76">
         <v>0</v>
       </c>
       <c r="J76">
-        <v>1.52793577983716</v>
+        <v>1.2767926677740682</v>
       </c>
       <c r="K76">
         <v>0</v>
       </c>
       <c r="L76">
-        <v>1.6729920468744219</v>
+        <v>0.29196217368460958</v>
       </c>
       <c r="M76">
-        <v>0.18973596636879836</v>
+        <v>9.4084386734767128E-2</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -7616,33 +7616,33 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <v>0.30967124915718819</v>
+        <v>0.16224482491377495</v>
       </c>
       <c r="G77">
         <v>0</v>
       </c>
       <c r="H77">
-        <v>-2.0444556517804156</v>
+        <v>-1.6758814822736328</v>
       </c>
       <c r="I77">
         <v>0</v>
       </c>
       <c r="J77">
-        <v>1.5881823258710199</v>
+        <v>1.52793577983716</v>
       </c>
       <c r="K77">
         <v>0</v>
       </c>
       <c r="L77">
-        <v>2.0549413317599217</v>
+        <v>1.6729920468744219</v>
       </c>
       <c r="M77">
-        <v>0.23002460232813388</v>
+        <v>0.18973596636879836</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -7657,33 +7657,33 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>0.49826906045543068</v>
+        <v>0.30967124915718819</v>
       </c>
       <c r="G78">
         <v>0</v>
       </c>
       <c r="H78">
-        <v>-2.4167766263258925</v>
+        <v>-2.0444556517804156</v>
       </c>
       <c r="I78">
         <v>0</v>
       </c>
       <c r="J78">
-        <v>1.6217210464330269</v>
+        <v>1.5881823258710199</v>
       </c>
       <c r="K78">
         <v>0</v>
       </c>
       <c r="L78">
-        <v>2.4524647663490233</v>
+        <v>2.0549413317599217</v>
       </c>
       <c r="M78">
-        <v>0.27294301232845158</v>
+        <v>0.23002460232813388</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -7698,33 +7698,33 @@
         <v>0</v>
       </c>
       <c r="F79">
-        <v>0.66792475237610327</v>
+        <v>0.49826906045543068</v>
       </c>
       <c r="G79">
         <v>0</v>
       </c>
       <c r="H79">
-        <v>-2.6750815273685014</v>
+        <v>-2.4167766263258925</v>
       </c>
       <c r="I79">
         <v>0</v>
       </c>
       <c r="J79">
-        <v>1.3783582285479135</v>
+        <v>1.6217210464330269</v>
       </c>
       <c r="K79">
         <v>0</v>
       </c>
       <c r="L79">
-        <v>2.7305014179717149</v>
+        <v>2.4524647663490233</v>
       </c>
       <c r="M79">
-        <v>0.38281413160870664</v>
+        <v>0.27294301232845158</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -7739,33 +7739,33 @@
         <v>0</v>
       </c>
       <c r="F80">
-        <v>0.54569339438146058</v>
+        <v>0.66792475237610327</v>
       </c>
       <c r="G80">
         <v>0</v>
       </c>
       <c r="H80">
-        <v>-2.523399903135628</v>
+        <v>-2.6750815273685014</v>
       </c>
       <c r="I80">
         <v>0</v>
       </c>
       <c r="J80">
-        <v>0.89559177374302767</v>
+        <v>1.3783582285479135</v>
       </c>
       <c r="K80">
         <v>0</v>
       </c>
       <c r="L80">
-        <v>2.5175969757962227</v>
+        <v>2.7305014179717149</v>
       </c>
       <c r="M80">
-        <v>0.57186870807744916</v>
+        <v>0.38281413160870664</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -7780,33 +7780,33 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <v>-2.2582412218437254E-2</v>
+        <v>0.54569339438146058</v>
       </c>
       <c r="G81">
         <v>0</v>
       </c>
       <c r="H81">
-        <v>-1.707294422424021</v>
+        <v>-2.523399903135628</v>
       </c>
       <c r="I81">
         <v>0</v>
       </c>
       <c r="J81">
-        <v>5.8061316401631174E-2</v>
+        <v>0.89559177374302767</v>
       </c>
       <c r="K81">
         <v>0</v>
       </c>
       <c r="L81">
-        <v>1.3855809768073688</v>
+        <v>2.5175969757962227</v>
       </c>
       <c r="M81">
-        <v>0.99776227974969711</v>
+        <v>0.57186870807744916</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -7821,33 +7821,33 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <v>-5.128071050976004E-2</v>
+        <v>-2.2582412218437254E-2</v>
       </c>
       <c r="G82">
         <v>0</v>
       </c>
       <c r="H82">
-        <v>-0.60674342555727956</v>
+        <v>-1.707294422424021</v>
       </c>
       <c r="I82">
         <v>0</v>
       </c>
       <c r="J82">
-        <v>1.3126931746017902</v>
+        <v>5.8061316401631174E-2</v>
       </c>
       <c r="K82">
         <v>0</v>
       </c>
       <c r="L82">
-        <v>0.6032280797583166</v>
+        <v>1.3855809768073688</v>
       </c>
       <c r="M82">
-        <v>8.2964929448905295E-2</v>
+        <v>0.99776227974969711</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -7862,33 +7862,33 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>-1.1924779959131403E-2</v>
+        <v>-5.128071050976004E-2</v>
       </c>
       <c r="G83">
         <v>0</v>
       </c>
       <c r="H83">
-        <v>-0.95197972830722333</v>
+        <v>-0.60674342555727956</v>
       </c>
       <c r="I83">
         <v>0</v>
       </c>
       <c r="J83">
-        <v>1.3932105676535247</v>
+        <v>1.3126931746017902</v>
       </c>
       <c r="K83">
         <v>0</v>
       </c>
       <c r="L83">
-        <v>0.9455182048243409</v>
+        <v>0.6032280797583166</v>
       </c>
       <c r="M83">
-        <v>0.11136843282871728</v>
+        <v>8.2964929448905295E-2</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -7903,33 +7903,33 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>-7.273515734660975E-2</v>
+        <v>-1.1924779959131403E-2</v>
       </c>
       <c r="G84">
         <v>0</v>
       </c>
       <c r="H84">
-        <v>0.50501444943067242</v>
+        <v>-0.95197972830722333</v>
       </c>
       <c r="I84">
         <v>0</v>
       </c>
       <c r="J84">
-        <v>1.2261210668769142</v>
+        <v>1.3932105676535247</v>
       </c>
       <c r="K84">
         <v>0</v>
       </c>
       <c r="L84">
-        <v>-0.48471181765696153</v>
+        <v>0.9455182048243409</v>
       </c>
       <c r="M84">
-        <v>0.15932498571060855</v>
+        <v>0.11136843282871728</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -7944,33 +7944,33 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <v>-9.8108715481738343E-2</v>
+        <v>-7.273515734660975E-2</v>
       </c>
       <c r="G85">
         <v>0</v>
       </c>
       <c r="H85">
-        <v>3.6631169446297338E-2</v>
+        <v>0.50501444943067242</v>
       </c>
       <c r="I85">
         <v>0</v>
       </c>
       <c r="J85">
-        <v>1.2019920439586451</v>
+        <v>1.2261210668769142</v>
       </c>
       <c r="K85">
         <v>0</v>
       </c>
       <c r="L85">
-        <v>-3.1446354261168187E-2</v>
+        <v>-0.48471181765696153</v>
       </c>
       <c r="M85">
-        <v>9.9891388178166493E-2</v>
+        <v>0.15932498571060855</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -7979,39 +7979,39 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86">
-        <v>-6.9506435658708704E-2</v>
+        <v>-9.8108715481738343E-2</v>
       </c>
       <c r="G86">
         <v>0</v>
       </c>
       <c r="H86">
-        <v>-0.38543276188102249</v>
+        <v>3.6631169446297338E-2</v>
       </c>
       <c r="I86">
         <v>0</v>
       </c>
       <c r="J86">
-        <v>0.8757747552691485</v>
+        <v>1.2019920439586451</v>
       </c>
       <c r="K86">
         <v>0</v>
       </c>
       <c r="L86">
-        <v>0.38543276188102249</v>
+        <v>-3.1446354261168187E-2</v>
       </c>
       <c r="M86">
-        <v>6.9506435658708704E-2</v>
+        <v>9.9891388178166493E-2</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -8026,33 +8026,33 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>0.19825346612774047</v>
+        <v>-6.9506435658708704E-2</v>
       </c>
       <c r="G87">
         <v>0</v>
       </c>
       <c r="H87">
-        <v>-1.8003892255870124</v>
+        <v>-0.38543276188102249</v>
       </c>
       <c r="I87">
         <v>0</v>
       </c>
       <c r="J87">
-        <v>1.0042032638441956</v>
+        <v>0.8757747552691485</v>
       </c>
       <c r="K87">
         <v>0</v>
       </c>
       <c r="L87">
-        <v>1.8022656147480305</v>
+        <v>0.38543276188102249</v>
       </c>
       <c r="M87">
-        <v>0.18040081579186187</v>
+        <v>6.9506435658708704E-2</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -8067,33 +8067,33 @@
         <v>0</v>
       </c>
       <c r="F88">
-        <v>0.35013168866706651</v>
+        <v>0.19825346612774047</v>
       </c>
       <c r="G88">
         <v>0</v>
       </c>
       <c r="H88">
-        <v>-2.1757430242328892</v>
+        <v>-1.8003892255870124</v>
       </c>
       <c r="I88">
         <v>0</v>
       </c>
       <c r="J88">
-        <v>1.0383394874624312</v>
+        <v>1.0042032638441956</v>
       </c>
       <c r="K88">
         <v>0</v>
       </c>
       <c r="L88">
-        <v>2.1922271277957734</v>
+        <v>1.8022656147480305</v>
       </c>
       <c r="M88">
-        <v>0.22492249123470398</v>
+        <v>0.18040081579186187</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -8108,33 +8108,33 @@
         <v>0</v>
       </c>
       <c r="F89">
-        <v>0.54186440388334123</v>
+        <v>0.35013168866706651</v>
       </c>
       <c r="G89">
         <v>0</v>
       </c>
       <c r="H89">
-        <v>-2.550474490105854</v>
+        <v>-2.1757430242328892</v>
       </c>
       <c r="I89">
         <v>0</v>
       </c>
       <c r="J89">
-        <v>1.0574676302980566</v>
+        <v>1.0383394874624312</v>
       </c>
       <c r="K89">
         <v>0</v>
       </c>
       <c r="L89">
-        <v>2.5930906929065345</v>
+        <v>2.1922271277957734</v>
       </c>
       <c r="M89">
-        <v>0.27279628890084689</v>
+        <v>0.22492249123470398</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -8149,33 +8149,33 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0.69502513502635788</v>
+        <v>0.54186440388334123</v>
       </c>
       <c r="G90">
         <v>0</v>
       </c>
       <c r="H90">
-        <v>-2.7704264894431851</v>
+        <v>-2.550474490105854</v>
       </c>
       <c r="I90">
         <v>0</v>
       </c>
       <c r="J90">
-        <v>0.87795100675087234</v>
+        <v>1.0574676302980566</v>
       </c>
       <c r="K90">
         <v>0</v>
       </c>
       <c r="L90">
-        <v>2.8290557094465236</v>
+        <v>2.5930906929065345</v>
       </c>
       <c r="M90">
-        <v>0.39340394580497529</v>
+        <v>0.27279628890084689</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -8190,33 +8190,33 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <v>0.54353953160692858</v>
+        <v>0.69502513502635788</v>
       </c>
       <c r="G91">
         <v>0</v>
       </c>
       <c r="H91">
-        <v>-2.5745798477787449</v>
+        <v>-2.7704264894431851</v>
       </c>
       <c r="I91">
         <v>0</v>
       </c>
       <c r="J91">
-        <v>0.54974438996758113</v>
+        <v>0.87795100675087234</v>
       </c>
       <c r="K91">
         <v>0</v>
       </c>
       <c r="L91">
-        <v>2.5630714964245831</v>
+        <v>2.8290557094465236</v>
       </c>
       <c r="M91">
-        <v>0.59545034992327506</v>
+        <v>0.39340394580497529</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -8231,33 +8231,33 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <v>-1.2469282647748162E-2</v>
+        <v>0.54353953160692858</v>
       </c>
       <c r="G92">
         <v>0</v>
       </c>
       <c r="H92">
-        <v>-1.7775514666662569</v>
+        <v>-2.5745798477787449</v>
       </c>
       <c r="I92">
         <v>0</v>
       </c>
       <c r="J92">
-        <v>-0.142097312449145</v>
+        <v>0.54974438996758113</v>
       </c>
       <c r="K92">
         <v>0</v>
       </c>
       <c r="L92">
-        <v>1.4489328310436105</v>
+        <v>2.5630714964245831</v>
       </c>
       <c r="M92">
-        <v>1.0297758740527272</v>
+        <v>0.59545034992327506</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -8272,33 +8272,33 @@
         <v>0</v>
       </c>
       <c r="F93">
-        <v>-2.5652572187046505E-2</v>
+        <v>-1.2469282647748162E-2</v>
       </c>
       <c r="G93">
         <v>0</v>
       </c>
       <c r="H93">
-        <v>-0.70789263545777181</v>
+        <v>-1.7775514666662569</v>
       </c>
       <c r="I93">
         <v>0</v>
       </c>
       <c r="J93">
-        <v>0.88175100866170597</v>
+        <v>-0.142097312449145</v>
       </c>
       <c r="K93">
         <v>0</v>
       </c>
       <c r="L93">
-        <v>0.7055799413078836</v>
+        <v>1.4489328310436105</v>
       </c>
       <c r="M93">
-        <v>6.2665654222428507E-2</v>
+        <v>1.0297758740527272</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -8313,33 +8313,33 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <v>1.6022318341714921E-2</v>
+        <v>-2.5652572187046505E-2</v>
       </c>
       <c r="G94">
         <v>0</v>
       </c>
       <c r="H94">
-        <v>-1.0616865599799663</v>
+        <v>-0.70789263545777181</v>
       </c>
       <c r="I94">
         <v>0</v>
       </c>
       <c r="J94">
-        <v>0.93396082483092047</v>
+        <v>0.88175100866170597</v>
       </c>
       <c r="K94">
         <v>0</v>
       </c>
       <c r="L94">
-        <v>1.0575453182325425</v>
+        <v>0.7055799413078836</v>
       </c>
       <c r="M94">
-        <v>9.5041918181231075E-2</v>
+        <v>6.2665654222428507E-2</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -8354,33 +8354,33 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <v>-4.6563791707584221E-2</v>
+        <v>1.6022318341714921E-2</v>
       </c>
       <c r="G95">
         <v>0</v>
       </c>
       <c r="H95">
-        <v>0.46332119055672866</v>
+        <v>-1.0616865599799663</v>
       </c>
       <c r="I95">
         <v>0</v>
       </c>
       <c r="J95">
-        <v>1.0152388816190119</v>
+        <v>0.93396082483092047</v>
       </c>
       <c r="K95">
         <v>0</v>
       </c>
       <c r="L95">
-        <v>-0.44819658301982845</v>
+        <v>1.0575453182325425</v>
       </c>
       <c r="M95">
-        <v>0.12631126349792302</v>
+        <v>9.5041918181231075E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -8395,74 +8395,74 @@
         <v>0</v>
       </c>
       <c r="F96">
-        <v>-7.4515806858318878E-2</v>
+        <v>-4.6563791707584221E-2</v>
       </c>
       <c r="G96">
         <v>0</v>
       </c>
       <c r="H96">
-        <v>-4.5358521817180072E-2</v>
+        <v>0.46332119055672866</v>
       </c>
       <c r="I96">
         <v>0</v>
       </c>
       <c r="J96">
-        <v>0.84653828497766881</v>
+        <v>1.0152388816190119</v>
       </c>
       <c r="K96">
         <v>0</v>
       </c>
       <c r="L96">
-        <v>4.9196215546590351E-2</v>
+        <v>-0.44819658301982845</v>
       </c>
       <c r="M96">
-        <v>7.203980392171612E-2</v>
+        <v>0.12631126349792302</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <v>-4.7505716244460337E-2</v>
+        <v>-7.4515806858318878E-2</v>
       </c>
       <c r="G97">
-        <v>-9.1927912441848697E-2</v>
+        <v>0</v>
       </c>
       <c r="H97">
-        <v>-0.3972073187545293</v>
+        <v>-4.5358521817180072E-2</v>
       </c>
       <c r="I97">
-        <v>-2.7772150835726466E-3</v>
+        <v>0</v>
       </c>
       <c r="J97">
-        <v>0.60339027191894345</v>
+        <v>0.84653828497766881</v>
       </c>
       <c r="K97">
-        <v>8.3511717676247581E-3</v>
+        <v>0</v>
       </c>
       <c r="L97">
-        <v>0.3972073187545293</v>
+        <v>4.9196215546590351E-2</v>
       </c>
       <c r="M97">
-        <v>6.2747112142194694E-2</v>
+        <v>7.203980392171612E-2</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B98">
         <v>10</v>
@@ -8477,33 +8477,33 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <v>0.21918338527098491</v>
+        <v>-4.7505716244460337E-2</v>
       </c>
       <c r="G98">
-        <v>-0.10936143335693478</v>
+        <v>-9.1927912441848697E-2</v>
       </c>
       <c r="H98">
-        <v>-1.8066099806573888</v>
+        <v>-0.3972073187545293</v>
       </c>
       <c r="I98">
-        <v>3.4781461798756652E-3</v>
+        <v>-2.7772150835726466E-3</v>
       </c>
       <c r="J98">
-        <v>0.65452518973355323</v>
+        <v>0.60339027191894345</v>
       </c>
       <c r="K98">
-        <v>1.4571289994414448E-2</v>
+        <v>8.3511717676247581E-3</v>
       </c>
       <c r="L98">
-        <v>1.8127020062726227</v>
+        <v>0.3972073187545293</v>
       </c>
       <c r="M98">
-        <v>0.1777627280397478</v>
+        <v>6.2747112142194694E-2</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B99">
         <v>10</v>
@@ -8518,33 +8518,33 @@
         <v>0</v>
       </c>
       <c r="F99">
-        <v>0.35502696510795262</v>
+        <v>0.21918338527098491</v>
       </c>
       <c r="G99">
-        <v>-5.632605405318529E-2</v>
+        <v>-0.10936143335693478</v>
       </c>
       <c r="H99">
-        <v>-2.1778292202838712</v>
+        <v>-1.8066099806573888</v>
       </c>
       <c r="I99">
-        <v>2.3263079710197521E-3</v>
+        <v>3.4781461798756652E-3</v>
       </c>
       <c r="J99">
-        <v>0.66060889480146268</v>
+        <v>0.65452518973355323</v>
       </c>
       <c r="K99">
-        <v>7.8148588022492471E-3</v>
+        <v>1.4571289994414448E-2</v>
       </c>
       <c r="L99">
-        <v>2.1955092292140619</v>
+        <v>1.8127020062726227</v>
       </c>
       <c r="M99">
-        <v>0.2271614362967018</v>
+        <v>0.1777627280397478</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B100">
         <v>10</v>
@@ -8559,33 +8559,33 @@
         <v>0</v>
       </c>
       <c r="F100">
-        <v>0.55163035281987938</v>
+        <v>0.35502696510795262</v>
       </c>
       <c r="G100">
-        <v>-5.696113208327748E-2</v>
+        <v>-5.632605405318529E-2</v>
       </c>
       <c r="H100">
-        <v>-2.5984390803467101</v>
+        <v>-2.1778292202838712</v>
       </c>
       <c r="I100">
-        <v>4.3182000198387091E-3</v>
+        <v>2.3263079710197521E-3</v>
       </c>
       <c r="J100">
-        <v>0.71727025064819516</v>
+        <v>0.66060889480146268</v>
       </c>
       <c r="K100">
-        <v>9.0375173385818137E-3</v>
+        <v>7.8148588022492471E-3</v>
       </c>
       <c r="L100">
-        <v>2.6417255731941154</v>
+        <v>2.1955092292140619</v>
       </c>
       <c r="M100">
-        <v>0.28399292878689086</v>
+        <v>0.2271614362967018</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B101">
         <v>10</v>
@@ -8600,33 +8600,33 @@
         <v>0</v>
       </c>
       <c r="F101">
-        <v>-3.3400760249008552E-3</v>
+        <v>0.55163035281987938</v>
       </c>
       <c r="G101">
-        <v>-9.4667950871191994E-2</v>
+        <v>-5.696113208327748E-2</v>
       </c>
       <c r="H101">
-        <v>-0.72137281145379484</v>
+        <v>-2.5984390803467101</v>
       </c>
       <c r="I101">
-        <v>-2.7330319478969314E-3</v>
+        <v>4.3182000198387091E-3</v>
       </c>
       <c r="J101">
-        <v>0.58733921900315789</v>
+        <v>0.71727025064819516</v>
       </c>
       <c r="K101">
-        <v>1.1036506388339591E-2</v>
+        <v>9.0375173385818137E-3</v>
       </c>
       <c r="L101">
-        <v>0.72020938901401477</v>
+        <v>2.6417255731941154</v>
       </c>
       <c r="M101">
-        <v>5.6903913815647508E-2</v>
+        <v>0.28399292878689086</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B102">
         <v>10</v>
@@ -8641,33 +8641,33 @@
         <v>0</v>
       </c>
       <c r="F102">
-        <v>4.1247313377936731E-2</v>
+        <v>-3.3400760249008552E-3</v>
       </c>
       <c r="G102">
-        <v>-0.1013204080783493</v>
+        <v>-9.4667950871191994E-2</v>
       </c>
       <c r="H102">
-        <v>-1.0708453123226094</v>
+        <v>-0.72137281145379484</v>
       </c>
       <c r="I102">
-        <v>-1.9956999129138462E-3</v>
+        <v>-2.7330319478969314E-3</v>
       </c>
       <c r="J102">
-        <v>0.60730047628207351</v>
+        <v>0.58733921900315789</v>
       </c>
       <c r="K102">
-        <v>1.2228822106443904E-2</v>
+        <v>1.1036506388339591E-2</v>
       </c>
       <c r="L102">
-        <v>1.0692906279386272</v>
+        <v>0.72020938901401477</v>
       </c>
       <c r="M102">
-        <v>8.7429243252462749E-2</v>
+        <v>5.6903913815647508E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B103">
         <v>10</v>
@@ -8682,33 +8682,33 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <v>-4.6016027279502686E-2</v>
+        <v>4.1247313377936731E-2</v>
       </c>
       <c r="G103">
-        <v>-7.784002123974218E-2</v>
+        <v>-0.1013204080783493</v>
       </c>
       <c r="H103">
-        <v>0.39817095225636107</v>
+        <v>-1.0708453123226094</v>
       </c>
       <c r="I103">
-        <v>1.6575631411882306E-2</v>
+        <v>-1.9956999129138462E-3</v>
       </c>
       <c r="J103">
-        <v>0.7114984781554804</v>
+        <v>0.60730047628207351</v>
       </c>
       <c r="K103">
-        <v>6.0144605612426332E-3</v>
+        <v>1.2228822106443904E-2</v>
       </c>
       <c r="L103">
-        <v>-0.38413124152576072</v>
+        <v>1.0692906279386272</v>
       </c>
       <c r="M103">
-        <v>0.12623649519322286</v>
+        <v>8.7429243252462749E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B104">
         <v>10</v>
@@ -8723,36 +8723,36 @@
         <v>0</v>
       </c>
       <c r="F104">
-        <v>-5.680321631205857E-2</v>
+        <v>-4.6016027279502686E-2</v>
       </c>
       <c r="G104">
-        <v>-8.481552613842655E-2</v>
+        <v>-7.784002123974218E-2</v>
       </c>
       <c r="H104">
-        <v>-6.4259441263303296E-2</v>
+        <v>0.39817095225636107</v>
       </c>
       <c r="I104">
-        <v>-3.0187146553080106E-3</v>
+        <v>1.6575631411882306E-2</v>
       </c>
       <c r="J104">
-        <v>0.60023980708646352</v>
+        <v>0.7114984781554804</v>
       </c>
       <c r="K104">
-        <v>6.5520842415802702E-3</v>
+        <v>6.0144605612426332E-3</v>
       </c>
       <c r="L104">
-        <v>6.71442265757278E-2</v>
+        <v>-0.38413124152576072</v>
       </c>
       <c r="M104">
-        <v>6.7279658631792763E-2</v>
+        <v>0.12623649519322286</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -8764,33 +8764,33 @@
         <v>0</v>
       </c>
       <c r="F105">
-        <v>-2.3364533049572544E-2</v>
+        <v>-5.680321631205857E-2</v>
       </c>
       <c r="G105">
-        <v>-0.19641942417667502</v>
+        <v>-8.481552613842655E-2</v>
       </c>
       <c r="H105">
-        <v>-0.30084637733205799</v>
+        <v>-6.4259441263303296E-2</v>
       </c>
       <c r="I105">
-        <v>-2.4212806579202743E-3</v>
+        <v>-3.0187146553080106E-3</v>
       </c>
       <c r="J105">
-        <v>0.60271620419005245</v>
+        <v>0.60023980708646352</v>
       </c>
       <c r="K105">
-        <v>1.5651856650643513E-2</v>
+        <v>6.5520842415802702E-3</v>
       </c>
       <c r="L105">
-        <v>0.30084637733205799</v>
+        <v>6.71442265757278E-2</v>
       </c>
       <c r="M105">
-        <v>8.9134878903643494E-2</v>
+        <v>6.7279658631792763E-2</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B106">
         <v>20</v>
@@ -8805,33 +8805,33 @@
         <v>0</v>
       </c>
       <c r="F106">
-        <v>0.20131901999215693</v>
+        <v>-2.3364533049572544E-2</v>
       </c>
       <c r="G106">
-        <v>-0.2140853276862541</v>
+        <v>-0.19641942417667502</v>
       </c>
       <c r="H106">
-        <v>-1.5978304340908418</v>
+        <v>-0.30084637733205799</v>
       </c>
       <c r="I106">
-        <v>2.5996595099345016E-3</v>
+        <v>-2.4212806579202743E-3</v>
       </c>
       <c r="J106">
-        <v>0.73759258791242588</v>
+        <v>0.60271620419005245</v>
       </c>
       <c r="K106">
-        <v>1.8409391591195663E-2</v>
+        <v>1.5651856650643513E-2</v>
       </c>
       <c r="L106">
-        <v>1.6047705833257557</v>
+        <v>0.30084637733205799</v>
       </c>
       <c r="M106">
-        <v>0.20035054592369858</v>
+        <v>8.9134878903643494E-2</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B107">
         <v>20</v>
@@ -8846,33 +8846,33 @@
         <v>0</v>
       </c>
       <c r="F107">
-        <v>0.32793787472970998</v>
+        <v>0.20131901999215693</v>
       </c>
       <c r="G107">
-        <v>-0.21217478562063638</v>
+        <v>-0.2140853276862541</v>
       </c>
       <c r="H107">
-        <v>-1.9352948053062868</v>
+        <v>-1.5978304340908418</v>
       </c>
       <c r="I107">
-        <v>5.3145576626830839E-3</v>
+        <v>2.5996595099345016E-3</v>
       </c>
       <c r="J107">
-        <v>0.77104684638811694</v>
+        <v>0.73759258791242588</v>
       </c>
       <c r="K107">
-        <v>1.8521905389749266E-2</v>
+        <v>1.8409391591195663E-2</v>
       </c>
       <c r="L107">
-        <v>1.9542278015189098</v>
+        <v>1.6047705833257557</v>
       </c>
       <c r="M107">
-        <v>0.24559129505320115</v>
+        <v>0.20035054592369858</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B108">
         <v>20</v>
@@ -8887,33 +8887,33 @@
         <v>0</v>
       </c>
       <c r="F108">
-        <v>0.28571565201086574</v>
+        <v>0.32793787472970998</v>
       </c>
       <c r="G108">
-        <v>-0.23380216146242108</v>
+        <v>-0.21217478562063638</v>
       </c>
       <c r="H108">
-        <v>-1.9537223938165951</v>
+        <v>-1.9352948053062868</v>
       </c>
       <c r="I108">
-        <v>2.1534872412220261E-2</v>
+        <v>5.3145576626830839E-3</v>
       </c>
       <c r="J108">
-        <v>0.52412751484017817</v>
+        <v>0.77104684638811694</v>
       </c>
       <c r="K108">
-        <v>1.7067399436774752E-2</v>
+        <v>1.8521905389749266E-2</v>
       </c>
       <c r="L108">
-        <v>1.946391405701315</v>
+        <v>1.9542278015189098</v>
       </c>
       <c r="M108">
-        <v>0.39194458632299817</v>
+        <v>0.24559129505320115</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B109">
         <v>20</v>
@@ -8928,33 +8928,33 @@
         <v>0</v>
       </c>
       <c r="F109">
-        <v>1.192535532286151E-2</v>
+        <v>0.28571565201086574</v>
       </c>
       <c r="G109">
-        <v>-0.1977505202515592</v>
+        <v>-0.23380216146242108</v>
       </c>
       <c r="H109">
-        <v>-0.59298182651323161</v>
+        <v>-1.9537223938165951</v>
       </c>
       <c r="I109">
-        <v>-3.9364841775132121E-3</v>
+        <v>2.1534872412220261E-2</v>
       </c>
       <c r="J109">
-        <v>0.6254041524460493</v>
+        <v>0.52412751484017817</v>
       </c>
       <c r="K109">
-        <v>1.7362751369570727E-2</v>
+        <v>1.7067399436774752E-2</v>
       </c>
       <c r="L109">
-        <v>0.59279329040318485</v>
+        <v>1.946391405701315</v>
       </c>
       <c r="M109">
-        <v>8.560652592627864E-2</v>
+        <v>0.39194458632299817</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B110">
         <v>20</v>
@@ -8969,33 +8969,33 @@
         <v>0</v>
       </c>
       <c r="F110">
-        <v>5.1070746880325146E-2</v>
+        <v>1.192535532286151E-2</v>
       </c>
       <c r="G110">
-        <v>-0.20563943801272749</v>
+        <v>-0.1977505202515592</v>
       </c>
       <c r="H110">
-        <v>-0.9084862820756171</v>
+        <v>-0.59298182651323161</v>
       </c>
       <c r="I110">
-        <v>-4.4806121859410578E-3</v>
+        <v>-3.9364841775132121E-3</v>
       </c>
       <c r="J110">
-        <v>0.67356942233129458</v>
+        <v>0.6254041524460493</v>
       </c>
       <c r="K110">
-        <v>1.8293177597732562E-2</v>
+        <v>1.7362751369570727E-2</v>
       </c>
       <c r="L110">
-        <v>0.90884784585525014</v>
+        <v>0.59279329040318485</v>
       </c>
       <c r="M110">
-        <v>0.1118406496414306</v>
+        <v>8.560652592627864E-2</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B111">
         <v>20</v>
@@ -9010,33 +9010,33 @@
         <v>0</v>
       </c>
       <c r="F111">
-        <v>-5.0027938577338123E-2</v>
+        <v>5.1070746880325146E-2</v>
       </c>
       <c r="G111">
-        <v>-0.16787578987678636</v>
+        <v>-0.20563943801272749</v>
       </c>
       <c r="H111">
-        <v>0.38554473622205221</v>
+        <v>-0.9084862820756171</v>
       </c>
       <c r="I111">
-        <v>2.575041145684303E-2</v>
+        <v>-4.4806121859410578E-3</v>
       </c>
       <c r="J111">
-        <v>0.58381833783153814</v>
+        <v>0.67356942233129458</v>
       </c>
       <c r="K111">
-        <v>1.3972419247413822E-2</v>
+        <v>1.8293177597732562E-2</v>
       </c>
       <c r="L111">
-        <v>-0.37100018499813575</v>
+        <v>0.90884784585525014</v>
       </c>
       <c r="M111">
-        <v>0.1666251990856247</v>
+        <v>0.1118406496414306</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B112">
         <v>20</v>
@@ -9051,36 +9051,36 @@
         <v>0</v>
       </c>
       <c r="F112">
-        <v>-4.2445598853748108E-2</v>
+        <v>-5.0027938577338123E-2</v>
       </c>
       <c r="G112">
-        <v>-0.17410989314356345</v>
+        <v>-0.16787578987678636</v>
       </c>
       <c r="H112">
-        <v>-6.5695455195958236E-2</v>
+        <v>0.38554473622205221</v>
       </c>
       <c r="I112">
-        <v>4.3400079189802607E-3</v>
+        <v>2.575041145684303E-2</v>
       </c>
       <c r="J112">
-        <v>0.60973770489389667</v>
+        <v>0.58381833783153814</v>
       </c>
       <c r="K112">
-        <v>1.5545018857230822E-2</v>
+        <v>1.3972419247413822E-2</v>
       </c>
       <c r="L112">
-        <v>6.7826852862145043E-2</v>
+        <v>-0.37100018499813575</v>
       </c>
       <c r="M112">
-        <v>9.61493609518555E-2</v>
+        <v>0.1666251990856247</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B113">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -9092,33 +9092,33 @@
         <v>0</v>
       </c>
       <c r="F113">
-        <v>1.4562382430074136E-2</v>
+        <v>-4.2445598853748108E-2</v>
       </c>
       <c r="G113">
-        <v>-0.34117274201218539</v>
+        <v>-0.17410989314356345</v>
       </c>
       <c r="H113">
-        <v>-0.26292881549732261</v>
+        <v>-6.5695455195958236E-2</v>
       </c>
       <c r="I113">
-        <v>1.2974792629972969E-2</v>
+        <v>4.3400079189802607E-3</v>
       </c>
       <c r="J113">
-        <v>0.13071235106523052</v>
+        <v>0.60973770489389667</v>
       </c>
       <c r="K113">
-        <v>3.6569708865806155E-2</v>
+        <v>1.5545018857230822E-2</v>
       </c>
       <c r="L113">
-        <v>0.26292881549732261</v>
+        <v>6.7826852862145043E-2</v>
       </c>
       <c r="M113">
-        <v>0.23094840006628753</v>
+        <v>9.61493609518555E-2</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B114">
         <v>45</v>
@@ -9133,33 +9133,33 @@
         <v>0</v>
       </c>
       <c r="F114">
-        <v>6.6744928603131207E-2</v>
+        <v>1.4562382430074136E-2</v>
       </c>
       <c r="G114">
-        <v>-0.35855411499705614</v>
+        <v>-0.34117274201218539</v>
       </c>
       <c r="H114">
-        <v>-0.88189487677332457</v>
+        <v>-0.26292881549732261</v>
       </c>
       <c r="I114">
-        <v>1.1494985182503414E-3</v>
+        <v>1.2974792629972969E-2</v>
       </c>
       <c r="J114">
-        <v>0.50424292019560746</v>
+        <v>0.13071235106523052</v>
       </c>
       <c r="K114">
-        <v>1.5293832187298809E-2</v>
+        <v>3.6569708865806155E-2</v>
       </c>
       <c r="L114">
-        <v>0.8765004087746503</v>
+        <v>0.26292881549732261</v>
       </c>
       <c r="M114">
-        <v>0.33702404704451111</v>
+        <v>0.23094840006628753</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B115">
         <v>45</v>
@@ -9174,33 +9174,33 @@
         <v>0</v>
       </c>
       <c r="F115">
-        <v>7.4681583023926496E-2</v>
+        <v>6.6744928603131207E-2</v>
       </c>
       <c r="G115">
-        <v>-0.42493755420952761</v>
+        <v>-0.35855411499705614</v>
       </c>
       <c r="H115">
-        <v>-0.89827728298763987</v>
+        <v>-0.88189487677332457</v>
       </c>
       <c r="I115">
-        <v>6.6431830838151089E-3</v>
+        <v>1.1494985182503414E-3</v>
       </c>
       <c r="J115">
-        <v>0.35353635633790342</v>
+        <v>0.50424292019560746</v>
       </c>
       <c r="K115">
-        <v>1.2082185600684459E-2</v>
+        <v>1.5293832187298809E-2</v>
       </c>
       <c r="L115">
-        <v>0.88699824281153261</v>
+        <v>0.8765004087746503</v>
       </c>
       <c r="M115">
-        <v>0.41386390896759262</v>
+        <v>0.33702404704451111</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B116">
         <v>45</v>
@@ -9215,33 +9215,33 @@
         <v>0</v>
       </c>
       <c r="F116">
-        <v>0.12838033746056865</v>
+        <v>7.4681583023926496E-2</v>
       </c>
       <c r="G116">
-        <v>-0.41139940038735839</v>
+        <v>-0.42493755420952761</v>
       </c>
       <c r="H116">
-        <v>-1.1484398118795685</v>
+        <v>-0.89827728298763987</v>
       </c>
       <c r="I116">
-        <v>1.1027315119311985E-2</v>
+        <v>6.6431830838151089E-3</v>
       </c>
       <c r="J116">
-        <v>0.36333856542398846</v>
+        <v>0.35353635633790342</v>
       </c>
       <c r="K116">
-        <v>1.1973187671428076E-2</v>
+        <v>1.2082185600684459E-2</v>
       </c>
       <c r="L116">
-        <v>1.1319028726797504</v>
+        <v>0.88699824281153261</v>
       </c>
       <c r="M116">
-        <v>0.45551102033549801</v>
+        <v>0.41386390896759262</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B117">
         <v>45</v>
@@ -9256,33 +9256,33 @@
         <v>0</v>
       </c>
       <c r="F117">
-        <v>4.0050776551835844E-2</v>
+        <v>0.12838033746056865</v>
       </c>
       <c r="G117">
-        <v>-0.34906734647434196</v>
+        <v>-0.41139940038735839</v>
       </c>
       <c r="H117">
-        <v>-0.42120721955691437</v>
+        <v>-1.1484398118795685</v>
       </c>
       <c r="I117">
-        <v>9.6645159441334314E-3</v>
+        <v>1.1027315119311985E-2</v>
       </c>
       <c r="J117">
-        <v>0.21134821837795698</v>
+        <v>0.36333856542398846</v>
       </c>
       <c r="K117">
-        <v>3.5861930521240704E-2</v>
+        <v>1.1973187671428076E-2</v>
       </c>
       <c r="L117">
-        <v>0.42272606539050189</v>
+        <v>1.1319028726797504</v>
       </c>
       <c r="M117">
-        <v>0.23413418562903801</v>
+        <v>0.45551102033549801</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B118">
         <v>45</v>
@@ -9297,33 +9297,33 @@
         <v>0</v>
       </c>
       <c r="F118">
-        <v>3.6049260753956452E-2</v>
+        <v>4.0050776551835844E-2</v>
       </c>
       <c r="G118">
-        <v>-0.33714576611907043</v>
+        <v>-0.34906734647434196</v>
       </c>
       <c r="H118">
-        <v>-0.58307267326184264</v>
+        <v>-0.42120721955691437</v>
       </c>
       <c r="I118">
-        <v>5.1722990716013108E-3</v>
+        <v>9.6645159441334314E-3</v>
       </c>
       <c r="J118">
-        <v>0.37265308151036075</v>
+        <v>0.21134821837795698</v>
       </c>
       <c r="K118">
-        <v>2.5274150641253865E-2</v>
+        <v>3.5861930521240704E-2</v>
       </c>
       <c r="L118">
-        <v>0.58364671397835965</v>
+        <v>0.42272606539050189</v>
       </c>
       <c r="M118">
-        <v>0.25614354658640848</v>
+        <v>0.23413418562903801</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B119">
         <v>45</v>
@@ -9338,33 +9338,33 @@
         <v>0</v>
       </c>
       <c r="F119">
-        <v>-5.2596574343978866E-2</v>
+        <v>3.6049260753956452E-2</v>
       </c>
       <c r="G119">
-        <v>-0.36697881086611123</v>
+        <v>-0.33714576611907043</v>
       </c>
       <c r="H119">
-        <v>0.16282144189795822</v>
+        <v>-0.58307267326184264</v>
       </c>
       <c r="I119">
-        <v>2.054244668063852E-2</v>
+        <v>5.1722990716013108E-3</v>
       </c>
       <c r="J119">
-        <v>1.8191006122906254E-2</v>
+        <v>0.37265308151036075</v>
       </c>
       <c r="K119">
-        <v>3.2009131654802486E-2</v>
+        <v>2.5274150641253865E-2</v>
       </c>
       <c r="L119">
-        <v>-0.15121451905138086</v>
+        <v>0.58364671397835965</v>
       </c>
       <c r="M119">
-        <v>0.3161120665413949</v>
+        <v>0.25614354658640848</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B120">
         <v>45</v>
@@ -9379,36 +9379,36 @@
         <v>0</v>
       </c>
       <c r="F120">
-        <v>-1.1467350049231788E-2</v>
+        <v>-5.2596574343978866E-2</v>
       </c>
       <c r="G120">
-        <v>-0.33984985556685265</v>
+        <v>-0.36697881086611123</v>
       </c>
       <c r="H120">
-        <v>-0.12936593336962468</v>
+        <v>0.16282144189795822</v>
       </c>
       <c r="I120">
-        <v>1.6670300320380294E-2</v>
+        <v>2.054244668063852E-2</v>
       </c>
       <c r="J120">
-        <v>3.0627950040284596E-2</v>
+        <v>1.8191006122906254E-2</v>
       </c>
       <c r="K120">
-        <v>3.5839742035837806E-2</v>
+        <v>3.2009131654802486E-2</v>
       </c>
       <c r="L120">
-        <v>0.1297887965843986</v>
+        <v>-0.15121451905138086</v>
       </c>
       <c r="M120">
-        <v>0.24362020655854169</v>
+        <v>0.3161120665413949</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B121">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -9420,33 +9420,33 @@
         <v>0</v>
       </c>
       <c r="F121">
-        <v>-5.9277281356348716E-2</v>
+        <v>-1.1467350049231788E-2</v>
       </c>
       <c r="G121">
-        <v>-4.5795131572825248E-2</v>
+        <v>-0.33984985556685265</v>
       </c>
       <c r="H121">
-        <v>-0.45321817305868006</v>
+        <v>-0.12936593336962468</v>
       </c>
       <c r="I121">
-        <v>4.790722037972777E-4</v>
+        <v>1.6670300320380294E-2</v>
       </c>
       <c r="J121">
-        <v>0.53588946501178747</v>
+        <v>3.0627950040284596E-2</v>
       </c>
       <c r="K121">
-        <v>4.556494574114188E-3</v>
+        <v>3.5839742035837806E-2</v>
       </c>
       <c r="L121">
-        <v>0.45321817305868006</v>
+        <v>0.1297887965843986</v>
       </c>
       <c r="M121">
-        <v>6.3043022110943578E-2</v>
+        <v>0.24362020655854169</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B122">
         <v>5</v>
@@ -9461,33 +9461,33 @@
         <v>0</v>
       </c>
       <c r="F122">
-        <v>0.21367986198260264</v>
+        <v>-5.9277281356348716E-2</v>
       </c>
       <c r="G122">
-        <v>-5.5995179334707809E-2</v>
+        <v>-4.5795131572825248E-2</v>
       </c>
       <c r="H122">
-        <v>-1.8566323867473109</v>
+        <v>-0.45321817305868006</v>
       </c>
       <c r="I122">
-        <v>1.3720205605942724E-3</v>
+        <v>4.790722037972777E-4</v>
       </c>
       <c r="J122">
-        <v>0.6358839619235559</v>
+        <v>0.53588946501178747</v>
       </c>
       <c r="K122">
-        <v>7.46922132412831E-3</v>
+        <v>4.556494574114188E-3</v>
       </c>
       <c r="L122">
-        <v>1.8604870559400697</v>
+        <v>0.45321817305868006</v>
       </c>
       <c r="M122">
-        <v>0.18121187790161089</v>
+        <v>6.3043022110943578E-2</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B123">
         <v>5</v>
@@ -9502,33 +9502,33 @@
         <v>0</v>
       </c>
       <c r="F123">
-        <v>0.36353755884268868</v>
+        <v>0.21367986198260264</v>
       </c>
       <c r="G123">
-        <v>-5.6972347940228305E-2</v>
+        <v>-5.5995179334707809E-2</v>
       </c>
       <c r="H123">
-        <v>-2.2294407327960712</v>
+        <v>-1.8566323867473109</v>
       </c>
       <c r="I123">
-        <v>2.4192421146164793E-3</v>
+        <v>1.3720205605942724E-3</v>
       </c>
       <c r="J123">
-        <v>0.67650698563225609</v>
+        <v>0.6358839619235559</v>
       </c>
       <c r="K123">
-        <v>7.9294107456995833E-3</v>
+        <v>7.46922132412831E-3</v>
       </c>
       <c r="L123">
-        <v>2.2475648258271175</v>
+        <v>1.8604870559400697</v>
       </c>
       <c r="M123">
-        <v>0.22997736307633398</v>
+        <v>0.18121187790161089</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B124">
         <v>5</v>
@@ -9543,33 +9543,33 @@
         <v>0</v>
       </c>
       <c r="F124">
-        <v>0.55163035281987971</v>
+        <v>0.36353755884268868</v>
       </c>
       <c r="G124">
-        <v>-5.696113208327757E-2</v>
+        <v>-5.6972347940228305E-2</v>
       </c>
       <c r="H124">
-        <v>-2.5984390803467106</v>
+        <v>-2.2294407327960712</v>
       </c>
       <c r="I124">
-        <v>4.3182000198383787E-3</v>
+        <v>2.4192421146164793E-3</v>
       </c>
       <c r="J124">
-        <v>0.7172702506481976</v>
+        <v>0.67650698563225609</v>
       </c>
       <c r="K124">
-        <v>9.0375173385817253E-3</v>
+        <v>7.9294107456995833E-3</v>
       </c>
       <c r="L124">
-        <v>2.6417255731941163</v>
+        <v>2.2475648258271175</v>
       </c>
       <c r="M124">
-        <v>0.28223555239936887</v>
+        <v>0.22997736307633398</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B125">
         <v>5</v>
@@ -9584,33 +9584,33 @@
         <v>0</v>
       </c>
       <c r="F125">
-        <v>-1.244184118689425E-2</v>
+        <v>0.55163035281987971</v>
       </c>
       <c r="G125">
-        <v>-4.7149660580241247E-2</v>
+        <v>-5.696113208327757E-2</v>
       </c>
       <c r="H125">
-        <v>-0.77286250802460776</v>
+        <v>-2.5984390803467106</v>
       </c>
       <c r="I125">
-        <v>7.0525740867477874E-5</v>
+        <v>4.3182000198383787E-3</v>
       </c>
       <c r="J125">
-        <v>0.53531573297310986</v>
+        <v>0.7172702506481976</v>
       </c>
       <c r="K125">
-        <v>5.8990528070585998E-3</v>
+        <v>9.0375173385817253E-3</v>
       </c>
       <c r="L125">
-        <v>0.77115217116192813</v>
+        <v>2.6417255731941163</v>
       </c>
       <c r="M125">
-        <v>5.6781453340377042E-2</v>
+        <v>0.28223555239936887</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B126">
         <v>5</v>
@@ -9625,33 +9625,33 @@
         <v>0</v>
       </c>
       <c r="F126">
-        <v>3.1097407134985693E-2</v>
+        <v>-1.244184118689425E-2</v>
       </c>
       <c r="G126">
-        <v>-5.1040282578760213E-2</v>
+        <v>-4.7149660580241247E-2</v>
       </c>
       <c r="H126">
-        <v>-1.1291257642886272</v>
+        <v>-0.77286250802460776</v>
       </c>
       <c r="I126">
-        <v>1.1886544626932207E-3</v>
+        <v>7.0525740867477874E-5</v>
       </c>
       <c r="J126">
-        <v>0.57099008130640638</v>
+        <v>0.53531573297310986</v>
       </c>
       <c r="K126">
-        <v>6.4517436041181403E-3</v>
+        <v>5.8990528070585998E-3</v>
       </c>
       <c r="L126">
-        <v>1.1261908593889041</v>
+        <v>0.77115217116192813</v>
       </c>
       <c r="M126">
-        <v>9.1215745471783752E-2</v>
+        <v>5.6781453340377042E-2</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>-10</v>
+        <v>6</v>
       </c>
       <c r="B127">
         <v>5</v>
@@ -9666,33 +9666,33 @@
         <v>0</v>
       </c>
       <c r="F127">
-        <v>-4.9948081335520665E-2</v>
+        <v>3.1097407134985693E-2</v>
       </c>
       <c r="G127">
-        <v>-5.0781022524719055E-2</v>
+        <v>-5.1040282578760213E-2</v>
       </c>
       <c r="H127">
-        <v>0.36739139563870138</v>
+        <v>-1.1291257642886272</v>
       </c>
       <c r="I127">
-        <v>1.2529484356126138E-2</v>
+        <v>1.1886544626932207E-3</v>
       </c>
       <c r="J127">
-        <v>0.63690731732829309</v>
+        <v>0.57099008130640638</v>
       </c>
       <c r="K127">
-        <v>6.6491395005249922E-3</v>
+        <v>6.4517436041181403E-3</v>
       </c>
       <c r="L127">
-        <v>-0.35313650151309578</v>
+        <v>1.1261908593889041</v>
       </c>
       <c r="M127">
-        <v>0.11698201558860154</v>
+        <v>9.1215745471783752E-2</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="B128">
         <v>5</v>
@@ -9707,69 +9707,151 @@
         <v>0</v>
       </c>
       <c r="F128">
-        <v>-6.6442545327944177E-2</v>
+        <v>-4.9948081335520665E-2</v>
       </c>
       <c r="G128">
-        <v>-4.4139661548338129E-2</v>
+        <v>-5.0781022524719055E-2</v>
       </c>
       <c r="H128">
-        <v>-0.11865632733292179</v>
+        <v>0.36739139563870138</v>
       </c>
       <c r="I128">
-        <v>1.1833717698856931E-3</v>
+        <v>1.2529484356126138E-2</v>
       </c>
       <c r="J128">
-        <v>0.50261730802701676</v>
+        <v>0.63690731732829309</v>
       </c>
       <c r="K128">
-        <v>4.2277992011485969E-3</v>
+        <v>6.6491395005249922E-3</v>
       </c>
       <c r="L128">
-        <v>0.12197104710511522</v>
+        <v>-0.35313650151309578</v>
       </c>
       <c r="M128">
-        <v>6.3759664211753816E-2</v>
+        <v>0.11698201558860154</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B129">
+        <v>5</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>-6.6442545327944177E-2</v>
+      </c>
+      <c r="G129">
+        <v>-4.4139661548338129E-2</v>
+      </c>
+      <c r="H129">
+        <v>-0.11865632733292179</v>
+      </c>
+      <c r="I129">
+        <v>1.1833717698856931E-3</v>
+      </c>
+      <c r="J129">
+        <v>0.50261730802701676</v>
+      </c>
+      <c r="K129">
+        <v>4.2277992011485969E-3</v>
+      </c>
+      <c r="L129">
+        <v>0.12197104710511522</v>
+      </c>
+      <c r="M129">
+        <v>6.3759664211753816E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>0</v>
+      </c>
+      <c r="B130">
         <v>90</v>
       </c>
-      <c r="C129">
-        <v>0</v>
-      </c>
-      <c r="D129">
-        <v>0</v>
-      </c>
-      <c r="E129">
-        <v>0</v>
-      </c>
-      <c r="F129">
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
         <v>1.7041213729324382E-2</v>
       </c>
-      <c r="G129">
+      <c r="G130">
         <v>-0.36392368744617631</v>
       </c>
-      <c r="H129">
+      <c r="H130">
         <v>-3.6261797567294335E-2</v>
       </c>
-      <c r="I129">
+      <c r="I130">
         <v>-4.0247807343861446E-4</v>
       </c>
-      <c r="J129">
+      <c r="J130">
         <v>1.072780736646251E-2</v>
       </c>
-      <c r="K129">
+      <c r="K130">
         <v>4.3191758762539965E-2</v>
       </c>
-      <c r="L129">
+      <c r="L130">
         <v>3.6261797567294335E-2</v>
       </c>
-      <c r="M129">
+      <c r="M130">
         <v>0.36392368744617631</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>-90</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>0.15316996570630381</v>
+      </c>
+      <c r="G131">
+        <v>1.1236940653992767E-2</v>
+      </c>
+      <c r="H131">
+        <v>1.8409158950242044</v>
+      </c>
+      <c r="I131">
+        <v>9.0540662991842619E-3</v>
+      </c>
+      <c r="J131">
+        <v>1.0436648502996442</v>
+      </c>
+      <c r="K131">
+        <v>-6.4741679085321576E-4</v>
+      </c>
+      <c r="L131">
+        <v>-0.15316996570630392</v>
+      </c>
+      <c r="M131">
+        <v>1.8409158950242044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadir modelo Aero parametrico
</commit_message>
<xml_diff>
--- a/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
+++ b/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Estudios y formación academica\Proyectos\xxcopter\trunk\Modelling and Control\DroneBoX\Modelo CFD DroneBoX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTorres\Desktop\New folder (2)\Modelo CFD DroneBoX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Datos referencia" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -733,7 +733,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
@@ -3818,7 +3818,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
   </cols>
@@ -4081,7 +4081,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
@@ -4481,7 +4481,7 @@
       <selection activeCell="K1" sqref="K1:M131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5505,7 +5505,7 @@
         <v>1.8894631765860634</v>
       </c>
       <c r="M25">
-        <v>0.185515465244568</v>
+        <v>0.18551546524456805</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -5833,7 +5833,7 @@
         <v>2.0723566497411938</v>
       </c>
       <c r="M33">
-        <v>0.20889586694965206</v>
+        <v>0.20889586694965218</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -6120,7 +6120,7 @@
         <v>1.3262807185602445</v>
       </c>
       <c r="M40">
-        <v>0.11229630545204901</v>
+        <v>0.11229630545204904</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -6284,7 +6284,7 @@
         <v>2.0978593483260881</v>
       </c>
       <c r="M44">
-        <v>0.22781791913729374</v>
+        <v>0.2278179191372938</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -6571,7 +6571,7 @@
         <v>1.3793364748992825</v>
       </c>
       <c r="M51">
-        <v>0.12839220907583238</v>
+        <v>0.1283922090758324</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -6735,7 +6735,7 @@
         <v>1.9819318724196169</v>
       </c>
       <c r="M55">
-        <v>0.19358558920892258</v>
+        <v>0.19358558920892263</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -7022,7 +7022,7 @@
         <v>1.2524332145926234</v>
       </c>
       <c r="M62">
-        <v>0.10312727102546061</v>
+        <v>0.10312727102546064</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -7186,7 +7186,7 @@
         <v>1.7188310547800971</v>
       </c>
       <c r="M66">
-        <v>0.18057897860079045</v>
+        <v>0.1805789786007905</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -7637,7 +7637,7 @@
         <v>1.6729920468744219</v>
       </c>
       <c r="M77">
-        <v>0.18973596636879836</v>
+        <v>0.18973596636879841</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -7924,7 +7924,7 @@
         <v>0.9455182048243409</v>
       </c>
       <c r="M84">
-        <v>0.11136843282871728</v>
+        <v>0.11136843282871729</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -8088,7 +8088,7 @@
         <v>1.8022656147480305</v>
       </c>
       <c r="M88">
-        <v>0.18040081579186187</v>
+        <v>0.18040081579186193</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -8375,7 +8375,7 @@
         <v>1.0575453182325425</v>
       </c>
       <c r="M95">
-        <v>9.5041918181231075E-2</v>
+        <v>9.5041918181231089E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -8539,7 +8539,7 @@
         <v>1.8127020062726227</v>
       </c>
       <c r="M99">
-        <v>0.1777627280397478</v>
+        <v>0.17776272803974785</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -8662,7 +8662,7 @@
         <v>0.72020938901401477</v>
       </c>
       <c r="M102">
-        <v>5.6903913815647508E-2</v>
+        <v>5.6903913815647522E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -8703,7 +8703,7 @@
         <v>1.0692906279386272</v>
       </c>
       <c r="M103">
-        <v>8.7429243252462749E-2</v>
+        <v>8.7429243252462763E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -8782,7 +8782,7 @@
         <v>6.5520842415802702E-3</v>
       </c>
       <c r="L105">
-        <v>6.71442265757278E-2</v>
+        <v>6.7144226575727814E-2</v>
       </c>
       <c r="M105">
         <v>6.7279658631792763E-2</v>
@@ -8867,7 +8867,7 @@
         <v>1.6047705833257557</v>
       </c>
       <c r="M107">
-        <v>0.20035054592369858</v>
+        <v>0.20035054592369864</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -9031,7 +9031,7 @@
         <v>0.90884784585525014</v>
       </c>
       <c r="M111">
-        <v>0.1118406496414306</v>
+        <v>0.11184064964143062</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -9523,7 +9523,7 @@
         <v>1.8604870559400697</v>
       </c>
       <c r="M123">
-        <v>0.18121187790161089</v>
+        <v>0.18121187790161095</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
@@ -9646,7 +9646,7 @@
         <v>0.77115217116192813</v>
       </c>
       <c r="M126">
-        <v>5.6781453340377042E-2</v>
+        <v>5.6781453340377055E-2</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
@@ -9687,7 +9687,7 @@
         <v>1.1261908593889041</v>
       </c>
       <c r="M127">
-        <v>9.1215745471783752E-2</v>
+        <v>9.121574547178378E-2</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
@@ -9769,7 +9769,7 @@
         <v>0.12197104710511522</v>
       </c>
       <c r="M129">
-        <v>6.3759664211753816E-2</v>
+        <v>6.3759664211753803E-2</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Implementacion modelo aero parametrico en simulink! Corre superrapido!!!!
</commit_message>
<xml_diff>
--- a/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
+++ b/Modelo CFD DroneBoX/Datos Aero DBX v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTorres\Desktop\New folder (2)\Modelo CFD DroneBoX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Estudios y formación academica\Proyectos\xxcopter\trunk\Modelling and Control\DroneBoX\Modelo CFD DroneBoX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -733,7 +733,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
@@ -3818,7 +3818,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
   </cols>
@@ -4081,7 +4081,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
@@ -4481,7 +4481,7 @@
       <selection activeCell="K1" sqref="K1:M131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5505,7 +5505,7 @@
         <v>1.8894631765860634</v>
       </c>
       <c r="M25">
-        <v>0.18551546524456805</v>
+        <v>0.185515465244568</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -5833,7 +5833,7 @@
         <v>2.0723566497411938</v>
       </c>
       <c r="M33">
-        <v>0.20889586694965218</v>
+        <v>0.20889586694965206</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -6120,7 +6120,7 @@
         <v>1.3262807185602445</v>
       </c>
       <c r="M40">
-        <v>0.11229630545204904</v>
+        <v>0.11229630545204901</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -6284,7 +6284,7 @@
         <v>2.0978593483260881</v>
       </c>
       <c r="M44">
-        <v>0.2278179191372938</v>
+        <v>0.22781791913729374</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -6571,7 +6571,7 @@
         <v>1.3793364748992825</v>
       </c>
       <c r="M51">
-        <v>0.1283922090758324</v>
+        <v>0.12839220907583238</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -6735,7 +6735,7 @@
         <v>1.9819318724196169</v>
       </c>
       <c r="M55">
-        <v>0.19358558920892263</v>
+        <v>0.19358558920892258</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -7022,7 +7022,7 @@
         <v>1.2524332145926234</v>
       </c>
       <c r="M62">
-        <v>0.10312727102546064</v>
+        <v>0.10312727102546061</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -7186,7 +7186,7 @@
         <v>1.7188310547800971</v>
       </c>
       <c r="M66">
-        <v>0.1805789786007905</v>
+        <v>0.18057897860079045</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -7637,7 +7637,7 @@
         <v>1.6729920468744219</v>
       </c>
       <c r="M77">
-        <v>0.18973596636879841</v>
+        <v>0.18973596636879836</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -7924,7 +7924,7 @@
         <v>0.9455182048243409</v>
       </c>
       <c r="M84">
-        <v>0.11136843282871729</v>
+        <v>0.11136843282871728</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -8088,7 +8088,7 @@
         <v>1.8022656147480305</v>
       </c>
       <c r="M88">
-        <v>0.18040081579186193</v>
+        <v>0.18040081579186187</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -8375,7 +8375,7 @@
         <v>1.0575453182325425</v>
       </c>
       <c r="M95">
-        <v>9.5041918181231089E-2</v>
+        <v>9.5041918181231075E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -8539,7 +8539,7 @@
         <v>1.8127020062726227</v>
       </c>
       <c r="M99">
-        <v>0.17776272803974785</v>
+        <v>0.1777627280397478</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -8662,7 +8662,7 @@
         <v>0.72020938901401477</v>
       </c>
       <c r="M102">
-        <v>5.6903913815647522E-2</v>
+        <v>5.6903913815647508E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -8703,7 +8703,7 @@
         <v>1.0692906279386272</v>
       </c>
       <c r="M103">
-        <v>8.7429243252462763E-2</v>
+        <v>8.7429243252462749E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -8782,7 +8782,7 @@
         <v>6.5520842415802702E-3</v>
       </c>
       <c r="L105">
-        <v>6.7144226575727814E-2</v>
+        <v>6.71442265757278E-2</v>
       </c>
       <c r="M105">
         <v>6.7279658631792763E-2</v>
@@ -8867,7 +8867,7 @@
         <v>1.6047705833257557</v>
       </c>
       <c r="M107">
-        <v>0.20035054592369864</v>
+        <v>0.20035054592369858</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -9031,7 +9031,7 @@
         <v>0.90884784585525014</v>
       </c>
       <c r="M111">
-        <v>0.11184064964143062</v>
+        <v>0.1118406496414306</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -9523,7 +9523,7 @@
         <v>1.8604870559400697</v>
       </c>
       <c r="M123">
-        <v>0.18121187790161095</v>
+        <v>0.18121187790161089</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
@@ -9646,7 +9646,7 @@
         <v>0.77115217116192813</v>
       </c>
       <c r="M126">
-        <v>5.6781453340377055E-2</v>
+        <v>5.6781453340377042E-2</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
@@ -9687,7 +9687,7 @@
         <v>1.1261908593889041</v>
       </c>
       <c r="M127">
-        <v>9.121574547178378E-2</v>
+        <v>9.1215745471783752E-2</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
@@ -9769,7 +9769,7 @@
         <v>0.12197104710511522</v>
       </c>
       <c r="M129">
-        <v>6.3759664211753803E-2</v>
+        <v>6.3759664211753816E-2</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>